<commit_message>
Added more experiments results
</commit_message>
<xml_diff>
--- a/model_building/summary_speaker_counting.xlsx
+++ b/model_building/summary_speaker_counting.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{23E0B00C-8705-4B02-BFE9-4DD65B8C1827}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C81F0102-49D2-43B4-A79E-5E20FD35E015}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="500ms" sheetId="1" r:id="rId1"/>
-    <sheet name="100ms" sheetId="3" r:id="rId2"/>
-    <sheet name="confusion matrices" sheetId="2" r:id="rId3"/>
+    <sheet name="300ms" sheetId="4" r:id="rId2"/>
+    <sheet name="100ms" sheetId="3" r:id="rId3"/>
+    <sheet name="confusion matrices" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
   <si>
     <t>Metric</t>
   </si>
@@ -214,13 +215,31 @@
   </si>
   <si>
     <t>4 x 1D convolutional blocks with [3, 3, 3, 3] layers per block with [32, 64, 128, 256] filters of [5, 5, 5, 5]. Max pooling 1D [1, 2, 2, 1]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.5]. After convolutional blocks dropout is 0.75. Batch normalization after convolutional blocks._x0000_</t>
+  </si>
+  <si>
+    <t>500ms_fft_env_hist/model1</t>
+  </si>
+  <si>
+    <t>fft clipped at 4000 Hz and between (-3 and -40 dB), signal envelope (Hilbert) at 2000 Hz, 50 bins of histogram between 0 and 0.5</t>
+  </si>
+  <si>
+    <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [5, 5, 5]. Max pooling 1D of [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.75]. After convolutional blocks, dropout is 0.75. Batch normalization after convolutional blocks.</t>
+  </si>
+  <si>
+    <t>500ms_mfcc_env_hist/model1</t>
+  </si>
+  <si>
+    <t>12mfcc per frame "E0" melcepst, signal envelope (Hilbert) at 2000 Hz, 100 bins of histogram between 0 and 1</t>
+  </si>
+  <si>
+    <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [16, 8, 4]. Max pooling 1D of [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.5]. After convolutional blocks, dropout is 0.75. Batch normalization after convolutional blocks.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +282,13 @@
     <font>
       <b/>
       <sz val="8"/>
+      <name val="MS Reference Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="MS Reference Sans Serif"/>
       <family val="2"/>
     </font>
@@ -321,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -426,6 +452,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -714,18 +752,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
-    <col min="2" max="6" width="25.77734375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="8" width="25.77734375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -744,8 +782,14 @@
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
@@ -764,8 +808,14 @@
       <c r="F2" s="14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -784,8 +834,14 @@
       <c r="F3" s="2">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="2">
+        <v>500</v>
+      </c>
+      <c r="H3" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -804,8 +860,14 @@
       <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -824,8 +886,14 @@
       <c r="F5" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="2">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -844,8 +912,14 @@
       <c r="F6" s="2">
         <v>600000</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="2">
+        <v>600000</v>
+      </c>
+      <c r="H6" s="2">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -869,8 +943,14 @@
         <f>0.04*F6</f>
         <v>24000</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="2">
+        <v>24000</v>
+      </c>
+      <c r="H7" s="2">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -889,18 +969,24 @@
       <c r="F8" s="2">
         <v>6016</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="2">
+        <v>2351</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -919,8 +1005,14 @@
       <c r="F11" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -939,8 +1031,13 @@
       <c r="F12" s="2">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="37">
+        <f>G13*F12/F13</f>
+        <v>21.102726063829788</v>
+      </c>
+      <c r="H12" s="37"/>
+    </row>
+    <row r="13" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -949,7 +1046,7 @@
         <v>8.96453857421875</v>
       </c>
       <c r="C13" s="13">
-        <f t="shared" ref="C13:F13" si="1">C6*C8*4/1024/1024/1024</f>
+        <f t="shared" ref="C13:G13" si="1">C6*C8*4/1024/1024/1024</f>
         <v>8.96453857421875</v>
       </c>
       <c r="D13" s="13">
@@ -964,8 +1061,16 @@
         <f t="shared" si="1"/>
         <v>13.446807861328125</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="G13" s="13">
+        <f t="shared" si="1"/>
+        <v>5.254894495010376</v>
+      </c>
+      <c r="H13" s="13">
+        <f>H8*H6*4/1024/1024/1024</f>
+        <v>4.3697655200958252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -984,8 +1089,14 @@
       <c r="F14" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1004,8 +1115,14 @@
       <c r="F15" s="2">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="2">
+        <v>64</v>
+      </c>
+      <c r="H15" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1024,8 +1141,14 @@
       <c r="F16" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1044,8 +1167,14 @@
       <c r="F17" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H17" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -1064,8 +1193,14 @@
       <c r="F18" s="10">
         <v>0.74939999999999996</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="38">
+        <v>0.8397</v>
+      </c>
+      <c r="H18" s="38">
+        <v>0.88619999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1084,8 +1219,14 @@
       <c r="F19" s="11">
         <v>0.71289999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="38">
+        <v>0.67979999999999996</v>
+      </c>
+      <c r="H19" s="39">
+        <v>0.74980000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1099,23 +1240,25 @@
         <v>39</v>
       </c>
       <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -1130,6 +1273,12 @@
       </c>
       <c r="F24" s="2">
         <v>3650</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1500</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1365</v>
       </c>
     </row>
   </sheetData>
@@ -1139,6 +1288,152 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE69C90-D583-4A21-B578-829C81F8277B}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="13"/>
+    </row>
+    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE1B5DB-A7CE-4976-BA44-166DD16E4014}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -1432,11 +1727,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B3942E-9FC7-4237-A72A-436C0A2724D2}">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1779,242 +2074,317 @@
       </c>
       <c r="F14" s="24"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F15" s="24"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="15" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+    </row>
+    <row r="16" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="27">
+        <f>B11</f>
+        <v>5780</v>
+      </c>
+      <c r="C16" s="27">
+        <f>SUM(C11:E11)</f>
+        <v>239</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="34">
+        <f>B16/SUM(B16:C16)</f>
+        <v>0.96029240737664068</v>
+      </c>
+      <c r="G16" s="36">
+        <f>2*F16*F17/(F16+F17)</f>
+        <v>0.93301049233252631</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+    </row>
+    <row r="17" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="27">
+        <f>SUM(B12:B14)</f>
+        <v>591</v>
+      </c>
+      <c r="C17" s="27">
+        <f>SUM(C12:E14)</f>
+        <v>17414</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="34">
+        <f>B16/SUM(B16:B17)</f>
+        <v>0.90723591272955584</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>3</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B19" s="27">
         <v>3338</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C19" s="27">
         <v>525</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D19" s="27">
         <v>41</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E19" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="27">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="27">
         <v>1072</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C20" s="27">
         <v>1591</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D20" s="27">
         <v>759</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E20" s="27">
         <v>583</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="27">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="27">
         <v>274</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C21" s="27">
         <v>1036</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D21" s="27">
         <v>1056</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E21" s="27">
         <v>1662</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="27">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="27">
         <v>84</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C22" s="27">
         <v>496</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D22" s="27">
         <v>821</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E22" s="27">
         <v>2640</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>4</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B24" s="27">
         <v>3319</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C24" s="27">
         <v>554</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D24" s="27">
         <v>35</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E24" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="27">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B25" s="27">
         <v>1124</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C25" s="27">
         <v>1780</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D25" s="27">
         <v>528</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E25" s="27">
         <v>573</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="27">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B26" s="27">
         <v>291</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C26" s="27">
         <v>1267</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D26" s="27">
         <v>802</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E26" s="27">
         <v>1668</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="27">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B27" s="27">
         <v>87</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C27" s="27">
         <v>665</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D27" s="27">
         <v>656</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E27" s="27">
         <v>2633</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>5</v>
       </c>
-      <c r="B26" s="27">
+      <c r="B29" s="27">
         <v>5651</v>
       </c>
-      <c r="C26" s="27">
+      <c r="C29" s="27">
         <v>345</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D29" s="27">
         <v>13</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E29" s="27">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="27">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B30" s="27">
         <v>568</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C30" s="27">
         <v>4265</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D30" s="27">
         <v>1088</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E30" s="27">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="27">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B31" s="27">
         <v>26</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C31" s="27">
         <v>1387</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D31" s="27">
         <v>3164</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E31" s="27">
         <v>1449</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="27">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B32" s="27">
         <v>3</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C32" s="27">
         <v>194</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D32" s="27">
         <v>1653</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E32" s="27">
         <v>4147</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>6</v>
       </c>
-      <c r="B31" s="27">
+      <c r="B34" s="27">
         <v>5512</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C34" s="27">
         <v>616</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D34" s="27">
         <v>51</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E34" s="27">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="27">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="27">
         <v>1627</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C35" s="27">
         <v>2671</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D35" s="27">
         <v>1095</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E35" s="27">
         <v>820</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="27">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="27">
         <v>392</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C36" s="27">
         <v>1703</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D36" s="27">
         <v>1525</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E36" s="27">
         <v>2701</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="27">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="27">
         <v>85</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C37" s="27">
         <v>851</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D37" s="27">
         <v>1125</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E37" s="27">
         <v>4196</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added script for trimming input file.
</commit_message>
<xml_diff>
--- a/model_building/summary_speaker_counting.xlsx
+++ b/model_building/summary_speaker_counting.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C81F0102-49D2-43B4-A79E-5E20FD35E015}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92356B43-9DCF-4C26-82FF-2004B84C2923}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="75">
   <si>
     <t>Metric</t>
   </si>
@@ -233,6 +233,21 @@
   </si>
   <si>
     <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [16, 8, 4]. Max pooling 1D of [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.5]. After convolutional blocks, dropout is 0.75. Batch normalization after convolutional blocks.</t>
+  </si>
+  <si>
+    <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [8, 6, 4]. Max pooling 1D [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256]. No dropout. Batch normalization after convolutional blocks._x0000_</t>
+  </si>
+  <si>
+    <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [8, 6, 4]. Max pooling 1D [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.5]. After convolutional blocks dropout is 0.75. Batch normalization after convolutional blocks._x0000_</t>
+  </si>
+  <si>
+    <t>500ms_mfcc_env_hist/model2</t>
+  </si>
+  <si>
+    <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [16, 8, 4]. Max pooling 1D of [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.25]. After convolutional blocks, dropout is 0.5. Batch normalization after convolutional blocks.</t>
+  </si>
+  <si>
+    <t>100ms_fft_env_hist\model3</t>
   </si>
 </sst>
 </file>
@@ -347,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -464,6 +479,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -752,18 +788,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
-    <col min="2" max="8" width="25.77734375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="7" width="25.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.77734375" style="17" customWidth="1"/>
+    <col min="9" max="9" width="25.77734375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -785,11 +823,14 @@
       <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="I1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
@@ -811,11 +852,14 @@
       <c r="G2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="43" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -837,11 +881,14 @@
       <c r="G3" s="2">
         <v>500</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="17">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -863,11 +910,14 @@
       <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -889,11 +939,14 @@
       <c r="G5" s="2">
         <v>35</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="17">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -915,11 +968,14 @@
       <c r="G6" s="2">
         <v>600000</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="17">
         <v>600000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="2">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -946,11 +1002,14 @@
       <c r="G7" s="2">
         <v>24000</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="17">
         <v>24000</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="2">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -972,21 +1031,24 @@
       <c r="G8" s="2">
         <v>2351</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="17">
         <v>1955</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="2">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1008,11 +1070,14 @@
       <c r="G11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="17" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1035,9 +1100,10 @@
         <f>G13*F12/F13</f>
         <v>21.102726063829788</v>
       </c>
-      <c r="H12" s="37"/>
-    </row>
-    <row r="13" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="44"/>
+      <c r="I12" s="37"/>
+    </row>
+    <row r="13" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -1065,12 +1131,16 @@
         <f t="shared" si="1"/>
         <v>5.254894495010376</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="35">
         <f>H8*H6*4/1024/1024/1024</f>
         <v>4.3697655200958252</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="I13" s="13">
+        <f>I8*I6*4/1024/1024/1024</f>
+        <v>4.3697655200958252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1092,11 +1162,14 @@
       <c r="G14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="17" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1118,11 +1191,14 @@
       <c r="G15" s="2">
         <v>64</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="17">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1144,11 +1220,14 @@
       <c r="G16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1170,11 +1249,14 @@
       <c r="G17" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="17">
         <v>5.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -1196,11 +1278,14 @@
       <c r="G18" s="38">
         <v>0.8397</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="28">
         <v>0.88619999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="38">
+        <v>0.96260000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1222,11 +1307,14 @@
       <c r="G19" s="38">
         <v>0.67979999999999996</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="45">
         <v>0.74980000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="39">
+        <v>0.74060000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1241,24 +1329,25 @@
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="19"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -1277,7 +1366,10 @@
       <c r="G24" s="2">
         <v>1500</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="17">
+        <v>1365</v>
+      </c>
+      <c r="I24" s="2">
         <v>1365</v>
       </c>
     </row>
@@ -1435,7 +1527,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE1B5DB-A7CE-4976-BA44-166DD16E4014}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1444,10 +1536,11 @@
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
     <col min="2" max="3" width="25.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" style="17" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="7" width="25.77734375" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1460,8 +1553,15 @@
       <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
@@ -1474,8 +1574,13 @@
       <c r="D2" s="16" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1488,8 +1593,14 @@
       <c r="D3" s="17">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="7">
+        <v>100</v>
+      </c>
+      <c r="F3" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1502,8 +1613,14 @@
       <c r="D4" s="17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1516,8 +1633,14 @@
       <c r="D5" s="17">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="7">
+        <v>40</v>
+      </c>
+      <c r="F5" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1530,8 +1653,14 @@
       <c r="D6" s="17">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="7">
+        <v>600000</v>
+      </c>
+      <c r="F6" s="7">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1545,18 +1674,25 @@
         <f>0.025*D6</f>
         <v>25000</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="7">
+        <f>0.04*E6</f>
+        <v>24000</v>
+      </c>
+      <c r="F7" s="7">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1569,8 +1705,14 @@
       <c r="D10" s="17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1583,8 +1725,14 @@
       <c r="D11" s="17">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="E11" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="F11" s="7">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1597,8 +1745,14 @@
       <c r="D12" s="17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1611,8 +1765,14 @@
       <c r="D13" s="17">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="7">
+        <v>64</v>
+      </c>
+      <c r="F13" s="7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1625,8 +1785,14 @@
       <c r="D14" s="17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1639,8 +1805,14 @@
       <c r="D15" s="17">
         <v>5.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F15" s="7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1653,8 +1825,15 @@
       <c r="D16" s="18">
         <v>0.54349999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="11">
+        <v>0.70740000000000003</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0.54069999999999996</v>
+      </c>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1667,8 +1846,15 @@
       <c r="D17" s="18">
         <v>0.55620000000000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="11">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0.54630000000000001</v>
+      </c>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1681,16 +1867,22 @@
       <c r="D18" s="19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="28">
         <v>0.53539999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1698,7 +1890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
@@ -1706,8 +1898,11 @@
         <f>'confusion matrices'!O8</f>
         <v>0.75891996142719376</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1719,6 +1914,12 @@
       </c>
       <c r="D22" s="17">
         <v>986</v>
+      </c>
+      <c r="E22" s="7">
+        <v>932</v>
+      </c>
+      <c r="F22" s="7">
+        <v>950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more metrics to inference script.
</commit_message>
<xml_diff>
--- a/model_building/summary_speaker_counting.xlsx
+++ b/model_building/summary_speaker_counting.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92356B43-9DCF-4C26-82FF-2004B84C2923}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A53594-247B-42B7-A635-609D1D53C1EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="500ms" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="80">
   <si>
     <t>Metric</t>
   </si>
@@ -248,12 +248,30 @@
   </si>
   <si>
     <t>100ms_fft_env_hist\model3</t>
+  </si>
+  <si>
+    <t>100ms_specgram_env_hist\model1</t>
+  </si>
+  <si>
+    <t>spectrogram in 25ms frames, with 10ms spectral frame, 4000Hz magnitude, clipped between (-3 and -40 db), envelope of signal (Hilbert) at 2000 Hz, histogram with 50 bins between 0 and 0.5</t>
+  </si>
+  <si>
+    <t>100ms_specgram_env_hist\model2</t>
+  </si>
+  <si>
+    <t>ID7</t>
+  </si>
+  <si>
+    <t>librispeech test-clean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -499,7 +517,10 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -790,7 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1383,7 +1404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE69C90-D583-4A21-B578-829C81F8277B}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1404,32 +1425,47 @@
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="29">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="2">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B6" s="2">
+        <v>600000</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B7" s="2">
+        <f>0.04*B6</f>
+        <v>24000</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1446,15 +1482,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B12" s="2">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1462,37 +1504,53 @@
       </c>
       <c r="B13" s="13"/>
     </row>
-    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="180" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B15" s="2">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B17" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3">
+        <v>0.83940000000000003</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4">
+        <v>0.64019999999999999</v>
+      </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1517,6 +1575,9 @@
     <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3300</v>
       </c>
     </row>
   </sheetData>
@@ -1527,7 +1588,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE1B5DB-A7CE-4976-BA44-166DD16E4014}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1536,11 +1597,11 @@
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
     <col min="2" max="3" width="25.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" style="17" customWidth="1"/>
-    <col min="5" max="7" width="25.77734375" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="8" width="25.77734375" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1559,9 +1620,14 @@
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="46"/>
-    </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
@@ -1578,9 +1644,14 @@
       <c r="F2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1599,8 +1670,14 @@
       <c r="F3" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="7">
+        <v>100</v>
+      </c>
+      <c r="H3" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1619,8 +1696,14 @@
       <c r="F4" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1639,8 +1722,14 @@
       <c r="F5" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="7">
+        <v>40</v>
+      </c>
+      <c r="H5" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1654,13 +1743,19 @@
         <v>1000000</v>
       </c>
       <c r="E6" s="7">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="F6" s="7">
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1000000</v>
+      </c>
+      <c r="G6" s="7">
+        <v>200000</v>
+      </c>
+      <c r="H6" s="7">
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1676,23 +1771,37 @@
       </c>
       <c r="E7" s="7">
         <f>0.04*E6</f>
-        <v>24000</v>
+        <v>40000</v>
       </c>
       <c r="F7" s="7">
         <v>24000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="7">
+        <f>0.04*G6</f>
+        <v>8000</v>
+      </c>
+      <c r="H7" s="7">
+        <f>0.04*H6</f>
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="17">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1711,8 +1820,14 @@
       <c r="F10" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1732,7 +1847,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1751,8 +1866,14 @@
       <c r="F12" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1771,8 +1892,14 @@
       <c r="F13" s="7">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="7">
+        <v>64</v>
+      </c>
+      <c r="H13" s="7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1791,8 +1918,14 @@
       <c r="F14" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1811,8 +1944,14 @@
       <c r="F15" s="7">
         <v>5.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H15" s="7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1832,8 +1971,11 @@
         <v>0.54069999999999996</v>
       </c>
       <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="11">
+        <v>0.61040000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1852,9 +1994,14 @@
       <c r="F17" s="11">
         <v>0.54630000000000001</v>
       </c>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="11">
+        <v>0.54349999999999998</v>
+      </c>
+      <c r="H17" s="46">
+        <v>0.5575</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1870,8 +2017,11 @@
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
       <c r="G18" s="40"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1881,16 +2031,22 @@
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
       <c r="G19" s="41"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="41">
+        <v>0.53129999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
@@ -1901,8 +2057,11 @@
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
       <c r="G21" s="42"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="42">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1930,9 +2089,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B3942E-9FC7-4237-A72A-436C0A2724D2}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2229,6 +2390,29 @@
         <v>8</v>
       </c>
       <c r="F11" s="24"/>
+      <c r="I11" s="2">
+        <v>2</v>
+      </c>
+      <c r="J11" s="26">
+        <v>20937</v>
+      </c>
+      <c r="K11" s="26">
+        <v>3500</v>
+      </c>
+      <c r="L11" s="26">
+        <v>347</v>
+      </c>
+      <c r="M11" s="26">
+        <v>214</v>
+      </c>
+      <c r="N11" s="24">
+        <f>J11/SUM(J11:M11)</f>
+        <v>0.83754700376030078</v>
+      </c>
+      <c r="O11" s="25">
+        <f>AVERAGE(N11:N14)</f>
+        <v>0.53129880080702363</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" s="27">
@@ -2244,6 +2428,22 @@
         <v>108</v>
       </c>
       <c r="F12" s="24"/>
+      <c r="J12" s="26">
+        <v>7417</v>
+      </c>
+      <c r="K12" s="26">
+        <v>9798</v>
+      </c>
+      <c r="L12" s="26">
+        <v>4755</v>
+      </c>
+      <c r="M12" s="26">
+        <v>3047</v>
+      </c>
+      <c r="N12" s="24">
+        <f>K12/SUM(J12:M12)</f>
+        <v>0.39165367550065955</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="27">
@@ -2259,6 +2459,22 @@
         <v>1842</v>
       </c>
       <c r="F13" s="24"/>
+      <c r="J13" s="26">
+        <v>2016</v>
+      </c>
+      <c r="K13" s="26">
+        <v>6705</v>
+      </c>
+      <c r="L13" s="26">
+        <v>6555</v>
+      </c>
+      <c r="M13" s="26">
+        <v>9671</v>
+      </c>
+      <c r="N13" s="24">
+        <f>L13/SUM(J13:M13)</f>
+        <v>0.26275704493526275</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="27">
@@ -2274,6 +2490,22 @@
         <v>4488</v>
       </c>
       <c r="F14" s="24"/>
+      <c r="J14" s="26">
+        <v>505</v>
+      </c>
+      <c r="K14" s="26">
+        <v>3184</v>
+      </c>
+      <c r="L14" s="26">
+        <v>5494</v>
+      </c>
+      <c r="M14" s="26">
+        <v>15855</v>
+      </c>
+      <c r="N14" s="24">
+        <f>M14/SUM(J14:M14)</f>
+        <v>0.63323747903187155</v>
+      </c>
     </row>
     <row r="15" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
@@ -2316,12 +2548,26 @@
         <v>0.93301049233252631</v>
       </c>
       <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
+      <c r="J16" s="26">
+        <f>J11</f>
+        <v>20937</v>
+      </c>
+      <c r="K16" s="26">
+        <f>SUM(K11:M11)</f>
+        <v>4061</v>
+      </c>
       <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
+      <c r="M16" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="N16" s="47">
+        <f>J16/SUM(J16:K16)</f>
+        <v>0.83754700376030078</v>
+      </c>
+      <c r="O16" s="34">
+        <f>2*N16*N17/(N17+N16)</f>
+        <v>0.74944964473001274</v>
+      </c>
     </row>
     <row r="17" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
@@ -2343,12 +2589,23 @@
       </c>
       <c r="G17" s="31"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
+      <c r="J17" s="26">
+        <f>SUM(J12:J14)</f>
+        <v>9938</v>
+      </c>
+      <c r="K17" s="26">
+        <f>SUM(K12:M14)</f>
+        <v>65064</v>
+      </c>
       <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
+      <c r="M17" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="N17" s="47">
+        <f>J16/SUM(J16:J17)</f>
+        <v>0.67812145748987851</v>
+      </c>
+      <c r="O17" s="34"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F18" s="24"/>
@@ -2587,6 +2844,65 @@
       </c>
       <c r="E37" s="27">
         <v>4196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>7</v>
+      </c>
+      <c r="B39" s="27">
+        <v>2937</v>
+      </c>
+      <c r="C39" s="27">
+        <v>492</v>
+      </c>
+      <c r="D39" s="27">
+        <v>42</v>
+      </c>
+      <c r="E39" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="27">
+        <v>791</v>
+      </c>
+      <c r="C40" s="27">
+        <v>1425</v>
+      </c>
+      <c r="D40" s="27">
+        <v>755</v>
+      </c>
+      <c r="E40" s="27">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="27">
+        <v>159</v>
+      </c>
+      <c r="C41" s="27">
+        <v>799</v>
+      </c>
+      <c r="D41" s="27">
+        <v>925</v>
+      </c>
+      <c r="E41" s="27">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="27">
+        <v>46</v>
+      </c>
+      <c r="C42" s="27">
+        <v>303</v>
+      </c>
+      <c r="D42" s="27">
+        <v>638</v>
+      </c>
+      <c r="E42" s="27">
+        <v>2546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest changes to windows branch.
</commit_message>
<xml_diff>
--- a/model_building/summary_speaker_counting.xlsx
+++ b/model_building/summary_speaker_counting.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A53594-247B-42B7-A635-609D1D53C1EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7139736-95B5-4E73-8471-D4F03995D63F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="500ms" sheetId="1" r:id="rId1"/>
-    <sheet name="300ms" sheetId="4" r:id="rId2"/>
-    <sheet name="100ms" sheetId="3" r:id="rId3"/>
-    <sheet name="confusion matrices" sheetId="2" r:id="rId4"/>
+    <sheet name="Summary" sheetId="8" r:id="rId1"/>
+    <sheet name="1000ms" sheetId="7" r:id="rId2"/>
+    <sheet name="500ms" sheetId="1" r:id="rId3"/>
+    <sheet name="400ms" sheetId="6" r:id="rId4"/>
+    <sheet name="300ms" sheetId="4" r:id="rId5"/>
+    <sheet name="200ms" sheetId="5" r:id="rId6"/>
+    <sheet name="100ms" sheetId="3" r:id="rId7"/>
+    <sheet name="confusion matrices" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="99">
   <si>
     <t>Metric</t>
   </si>
@@ -263,6 +267,63 @@
   </si>
   <si>
     <t>librispeech test-clean</t>
+  </si>
+  <si>
+    <t>100ms_specgram_env_hist\model3</t>
+  </si>
+  <si>
+    <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [12, 8, 6]. Max pooling 1D [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.5]. After convolutional blocks dropout is 0.75. Batch normalization after convolutional blocks._x0000_</t>
+  </si>
+  <si>
+    <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [16, 8, 4]. Max pooling 1D [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.25]. After convolutional blocks dropout is 0.5. Batch normalization after convolutional blocks._x0000_</t>
+  </si>
+  <si>
+    <t>spectrogram in 25ms frames, with 10ms spectral frame, 4000Hz magnitude, clipped between (-3 and -40 db), envelope of signal (Hilbert) at 2000 Hz, histogram with 100 bins between 0 and 0.5</t>
+  </si>
+  <si>
+    <t>4 x 1D convolutional blocks with [3, 3, 3, 3] layers per block with [32, 64, 128, 256] filters of [16, 8, 4, 4]. Max pooling 1D [1, 2, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.25]. After convolutional blocks dropout is 0.5. Batch normalization after convolutional blocks._x0000_</t>
+  </si>
+  <si>
+    <t>300ms_specgram_env_hist/model1</t>
+  </si>
+  <si>
+    <t>300ms_specgram_env_hist/model2</t>
+  </si>
+  <si>
+    <t>300ms_specgram_env_hist/model3</t>
+  </si>
+  <si>
+    <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [16, 8, 4]. Max pooling 1D [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.5]. After convolutional blocks dropout is 0.75. Batch normalization after convolutional blocks._x0000_</t>
+  </si>
+  <si>
+    <t>200ms_specgram_env_hist/model1</t>
+  </si>
+  <si>
+    <t>1000ms_specgram_env_hist/model1</t>
+  </si>
+  <si>
+    <t>12mfcc per frame "E0" melcepst, envelope of signal (Hilbert) at 2000 Hz, histogram with 100 bins between 0 and 0.5</t>
+  </si>
+  <si>
+    <t>400ms_specgram_env_hist/model1</t>
+  </si>
+  <si>
+    <t>Inference Cat Accuracy (%)</t>
+  </si>
+  <si>
+    <t>OS Precision</t>
+  </si>
+  <si>
+    <t>OS Recall</t>
+  </si>
+  <si>
+    <t>OS F-Score</t>
+  </si>
+  <si>
+    <t>Confusion Matrix ID</t>
+  </si>
+  <si>
+    <t>Duration (ms)</t>
   </si>
 </sst>
 </file>
@@ -270,9 +331,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +385,19 @@
       <color rgb="FF00B050"/>
       <name val="MS Reference Sans Serif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -380,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -517,10 +591,28 @@
     <xf numFmtId="10" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -808,10 +900,272 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D627365-F01A-4583-8FA0-E181B91C71DE}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="12.77734375" style="52" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="52"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="52">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="52">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="52">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="52">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="52">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C0A8CF-24A5-41AD-B8F9-22B8D89DACCE}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="29">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="42"/>
+    </row>
+    <row r="14" spans="1:2" ht="180" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.79669999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.81159999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="7">
+        <v>3973</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1161,7 +1515,7 @@
         <v>4.3697655200958252</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1282,10 +1636,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="3">
-        <v>0.91149999999999998</v>
+        <v>0.89829999999999999</v>
       </c>
       <c r="C18" s="3">
-        <v>0.73929999999999996</v>
+        <v>0.72430000000000005</v>
       </c>
       <c r="D18" s="10">
         <v>0.7218</v>
@@ -1294,16 +1648,16 @@
         <v>0.69969999999999999</v>
       </c>
       <c r="F18" s="10">
-        <v>0.74939999999999996</v>
+        <v>0.72070000000000001</v>
       </c>
       <c r="G18" s="38">
-        <v>0.8397</v>
+        <v>0.7621</v>
       </c>
       <c r="H18" s="28">
-        <v>0.88619999999999999</v>
+        <v>0.79020000000000001</v>
       </c>
       <c r="I18" s="38">
-        <v>0.96260000000000001</v>
+        <v>0.74199999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1400,8 +1754,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE69C90-D583-4A21-B578-829C81F8277B}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3C7494-2EAC-4FFC-8C4B-1EEE10737F24}">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0"/>
@@ -1409,7 +1763,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" style="17" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
@@ -1417,7 +1771,7 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1425,20 +1779,23 @@
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="B2" s="49" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29">
-        <v>100</v>
+      <c r="B3" s="50">
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="17" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1446,7 +1803,7 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="17">
         <v>40</v>
       </c>
     </row>
@@ -1454,7 +1811,7 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="17">
         <v>600000</v>
       </c>
     </row>
@@ -1462,8 +1819,7 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
-        <f>0.04*B6</f>
+      <c r="B7" s="17">
         <v>24000</v>
       </c>
     </row>
@@ -1471,6 +1827,9 @@
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B8" s="17">
+        <v>5797</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1486,37 +1845,37 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>76</v>
+      <c r="B11" s="17" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="2">
-        <v>38</v>
+      <c r="B12" s="17">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="35"/>
     </row>
     <row r="14" spans="1:2" ht="180" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>71</v>
+      <c r="B14" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="17">
         <v>64</v>
       </c>
     </row>
@@ -1524,7 +1883,7 @@
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="17" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1532,7 +1891,7 @@
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="17">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
@@ -1540,16 +1899,16 @@
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3">
-        <v>0.83940000000000003</v>
+      <c r="B18" s="51">
+        <v>0.70740000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="4">
-        <v>0.64019999999999999</v>
+      <c r="B19" s="51">
+        <v>0.69110000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1576,8 +1935,8 @@
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="2">
-        <v>3300</v>
+      <c r="B24" s="17">
+        <v>5949</v>
       </c>
     </row>
   </sheetData>
@@ -1586,9 +1945,486 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE69C90-D583-4A21-B578-829C81F8277B}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="29">
+        <v>300</v>
+      </c>
+      <c r="C3" s="50">
+        <v>300</v>
+      </c>
+      <c r="D3" s="29">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>40</v>
+      </c>
+      <c r="C5" s="17">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>600000</v>
+      </c>
+      <c r="C6" s="17">
+        <v>600000</v>
+      </c>
+      <c r="D6" s="2">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <f>0.04*B6</f>
+        <v>24000</v>
+      </c>
+      <c r="C7" s="17">
+        <v>24000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="2">
+        <v>38</v>
+      </c>
+      <c r="C12" s="17">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:4" ht="190.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>64</v>
+      </c>
+      <c r="C15" s="17">
+        <v>64</v>
+      </c>
+      <c r="D15" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C17" s="17">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.83940000000000003</v>
+      </c>
+      <c r="C18" s="51">
+        <v>0.68289999999999995</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.64309000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.64019999999999999</v>
+      </c>
+      <c r="C19" s="51">
+        <v>0.6583</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.63729999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3300</v>
+      </c>
+      <c r="C24" s="17">
+        <v>4499</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2626C802-DDDB-45F4-B350-C34EEA285F2A}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="50">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="17">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="17">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="35"/>
+    </row>
+    <row r="14" spans="1:2" ht="180" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="17">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="51">
+        <v>0.63029999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="51">
+        <v>0.61629999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="17">
+        <v>2300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE1B5DB-A7CE-4976-BA44-166DD16E4014}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1597,11 +2433,12 @@
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
     <col min="2" max="3" width="25.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" style="17" customWidth="1"/>
-    <col min="5" max="8" width="25.77734375" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="7" width="25.77734375" style="7" customWidth="1"/>
+    <col min="8" max="9" width="25.77734375" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1623,11 +2460,14 @@
       <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="I1" s="15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
@@ -1647,11 +2487,14 @@
       <c r="G2" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="16" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1673,11 +2516,14 @@
       <c r="G3" s="7">
         <v>100</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="17">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1699,11 +2545,14 @@
       <c r="G4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1725,11 +2574,14 @@
       <c r="G5" s="7">
         <v>40</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="17">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1751,11 +2603,14 @@
       <c r="G6" s="7">
         <v>200000</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="17">
         <v>350000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="17">
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1780,12 +2635,15 @@
         <f>0.04*G6</f>
         <v>8000</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="17">
         <f>0.04*H6</f>
         <v>14000</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="17">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1793,7 +2651,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1801,7 +2659,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1823,11 +2681,14 @@
       <c r="G10" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1847,7 +2708,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1869,11 +2730,14 @@
       <c r="G12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="17" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1895,11 +2759,14 @@
       <c r="G13" s="7">
         <v>64</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="17">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1921,11 +2788,14 @@
       <c r="G14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1947,11 +2817,14 @@
       <c r="G15" s="7">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="17">
         <v>5.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="17">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1971,11 +2844,14 @@
         <v>0.54069999999999996</v>
       </c>
       <c r="G16" s="11"/>
-      <c r="H16" s="11">
+      <c r="H16" s="18">
         <v>0.61040000000000005</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="18">
+        <v>0.55889999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1997,11 +2873,14 @@
       <c r="G17" s="11">
         <v>0.54349999999999998</v>
       </c>
-      <c r="H17" s="46">
+      <c r="H17" s="18">
         <v>0.5575</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="47">
+        <v>0.55820000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2017,11 +2896,12 @@
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
       <c r="G18" s="40"/>
-      <c r="H18" s="40" t="s">
+      <c r="H18" s="19" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2031,22 +2911,28 @@
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
       <c r="G19" s="41"/>
-      <c r="H19" s="41">
+      <c r="H19" s="28">
         <v>0.53129999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="28">
+        <v>0.53539999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
@@ -2057,11 +2943,14 @@
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
       <c r="G21" s="42"/>
-      <c r="H21" s="42">
+      <c r="H21" s="35">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="35">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -2087,13 +2976,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B3942E-9FC7-4237-A72A-436C0A2724D2}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2157,7 +3044,7 @@
       </c>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
-      <c r="I3" s="2">
+      <c r="I3" s="23">
         <v>1</v>
       </c>
       <c r="J3" s="26">
@@ -2390,7 +3277,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="24"/>
-      <c r="I11" s="2">
+      <c r="I11" s="23">
         <v>2</v>
       </c>
       <c r="J11" s="26">
@@ -2560,7 +3447,7 @@
       <c r="M16" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="47">
+      <c r="N16" s="46">
         <f>J16/SUM(J16:K16)</f>
         <v>0.83754700376030078</v>
       </c>
@@ -2601,7 +3488,7 @@
       <c r="M17" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="N17" s="47">
+      <c r="N17" s="46">
         <f>J16/SUM(J16:J17)</f>
         <v>0.67812145748987851</v>
       </c>
@@ -2626,6 +3513,25 @@
       <c r="E19" s="27">
         <v>22</v>
       </c>
+      <c r="I19" s="23">
+        <v>3</v>
+      </c>
+      <c r="J19" s="26">
+        <v>21753</v>
+      </c>
+      <c r="K19" s="26">
+        <v>2852</v>
+      </c>
+      <c r="L19" s="26">
+        <v>258</v>
+      </c>
+      <c r="M19" s="26">
+        <v>135</v>
+      </c>
+      <c r="N19" s="24">
+        <f>J19/SUM(J19:M19)</f>
+        <v>0.87018961516921356</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20" s="27">
@@ -2640,6 +3546,22 @@
       <c r="E20" s="27">
         <v>583</v>
       </c>
+      <c r="J20" s="26">
+        <v>7729</v>
+      </c>
+      <c r="K20" s="26">
+        <v>10704</v>
+      </c>
+      <c r="L20" s="26">
+        <v>4647</v>
+      </c>
+      <c r="M20" s="26">
+        <v>1937</v>
+      </c>
+      <c r="N20" s="24">
+        <f>K20/SUM(J20:M20)</f>
+        <v>0.4278690490466483</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="27">
@@ -2654,6 +3576,22 @@
       <c r="E21" s="27">
         <v>1662</v>
       </c>
+      <c r="J21" s="26">
+        <v>2170</v>
+      </c>
+      <c r="K21" s="26">
+        <v>7687</v>
+      </c>
+      <c r="L21" s="26">
+        <v>7838</v>
+      </c>
+      <c r="M21" s="26">
+        <v>7252</v>
+      </c>
+      <c r="N21" s="24">
+        <f>L21/SUM(J21:M21)</f>
+        <v>0.31418607447789315</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="27">
@@ -2668,6 +3606,22 @@
       <c r="E22" s="27">
         <v>2640</v>
       </c>
+      <c r="J22" s="26">
+        <v>570</v>
+      </c>
+      <c r="K22" s="26">
+        <v>3963</v>
+      </c>
+      <c r="L22" s="26">
+        <v>7249</v>
+      </c>
+      <c r="M22" s="26">
+        <v>13256</v>
+      </c>
+      <c r="N22" s="24">
+        <f>M22/SUM(J22:M22)</f>
+        <v>0.52943525840722105</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
@@ -2685,6 +3639,25 @@
       <c r="E24" s="27">
         <v>18</v>
       </c>
+      <c r="J24" s="26">
+        <f>J19</f>
+        <v>21753</v>
+      </c>
+      <c r="K24" s="26">
+        <f>SUM(K19:M19)</f>
+        <v>3245</v>
+      </c>
+      <c r="M24" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="N24" s="46">
+        <f>J24/SUM(J24:K24)</f>
+        <v>0.87018961516921356</v>
+      </c>
+      <c r="O24" s="34">
+        <f>2*N24*N25/(N25+N24)</f>
+        <v>0.76032855644879416</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B25" s="27">
@@ -2699,6 +3672,22 @@
       <c r="E25" s="27">
         <v>573</v>
       </c>
+      <c r="J25" s="26">
+        <f>SUM(J20:J22)</f>
+        <v>10469</v>
+      </c>
+      <c r="K25" s="26">
+        <f>SUM(K20:M22)</f>
+        <v>64533</v>
+      </c>
+      <c r="M25" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="N25" s="46">
+        <f>J24/SUM(J24:J25)</f>
+        <v>0.67509775929489169</v>
+      </c>
+      <c r="O25" s="34"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B26" s="27">

</xml_diff>

<commit_message>
Added latest version of summary spreadsheet.
</commit_message>
<xml_diff>
--- a/model_building/summary_speaker_counting.xlsx
+++ b/model_building/summary_speaker_counting.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7139736-95B5-4E73-8471-D4F03995D63F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E20BE6-C146-41E4-ADFC-7CDB5C35362B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="8" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="113">
   <si>
     <t>Metric</t>
   </si>
@@ -233,9 +233,6 @@
     <t>500ms_mfcc_env_hist/model1</t>
   </si>
   <si>
-    <t>12mfcc per frame "E0" melcepst, signal envelope (Hilbert) at 2000 Hz, 100 bins of histogram between 0 and 1</t>
-  </si>
-  <si>
     <t>3 x 1D convolutional blocks with [3, 3, 3] layers per block with [32, 64, 128] filters of [16, 8, 4]. Max pooling 1D of [1, 2, 2]. 3 x 1D Dense Layers of [1024, 512, 256] with dropouts of [0.1, 0.1, 0.5]. After convolutional blocks, dropout is 0.75. Batch normalization after convolutional blocks.</t>
   </si>
   <si>
@@ -324,6 +321,51 @@
   </si>
   <si>
     <t>Duration (ms)</t>
+  </si>
+  <si>
+    <t>Model Parameters</t>
+  </si>
+  <si>
+    <t>Input Features</t>
+  </si>
+  <si>
+    <t>Inference Time (Seconds)</t>
+  </si>
+  <si>
+    <t>Aggressive Regularization</t>
+  </si>
+  <si>
+    <t>50% More Training Examples</t>
+  </si>
+  <si>
+    <t>Higher Order Filters</t>
+  </si>
+  <si>
+    <t>Extra Convolutional Layer</t>
+  </si>
+  <si>
+    <t>2D Features (Specgram)</t>
+  </si>
+  <si>
+    <t>1D Features</t>
+  </si>
+  <si>
+    <t>1D + 2D Features Combined</t>
+  </si>
+  <si>
+    <t>Cat Accuracy Drop (%)</t>
+  </si>
+  <si>
+    <t>Class Errors</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>12mfcc per frame "E0" melcepst, signal envelope (Hilbert) at 2000 Hz, 100 bins of histogram between 0 and 0.5</t>
+  </si>
+  <si>
+    <t>ID8</t>
   </si>
 </sst>
 </file>
@@ -333,7 +375,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,17 +429,23 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="MS Reference Sans Serif"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -426,7 +474,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -449,12 +497,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -582,15 +656,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -609,11 +674,80 @@
     <xf numFmtId="10" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -901,71 +1035,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D627365-F01A-4583-8FA0-E181B91C71DE}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="12.77734375" style="52" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="52"/>
+    <col min="1" max="1" width="15.77734375" style="66" customWidth="1"/>
+    <col min="2" max="6" width="12.77734375" style="73" customWidth="1"/>
+    <col min="7" max="17" width="12.77734375" style="66" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="66"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:13" ht="45.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="53" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="52">
+      <c r="K1" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="67">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="52">
+      <c r="B2" s="68">
+        <f>'100ms'!I16</f>
+        <v>0.55889999999999995</v>
+      </c>
+      <c r="C2" s="68">
+        <f>'100ms'!I17</f>
+        <v>0.55820000000000003</v>
+      </c>
+      <c r="D2" s="68">
+        <f>'100ms'!I19</f>
+        <v>0.53539999999999999</v>
+      </c>
+      <c r="E2" s="68">
+        <f>1-D2/C2</f>
+        <v>4.0845575062701589E-2</v>
+      </c>
+      <c r="F2" s="69">
+        <f>'confusion matrices'!N8</f>
+        <v>0.82097576632964209</v>
+      </c>
+      <c r="G2" s="69">
+        <f>'confusion matrices'!N9</f>
+        <v>0.70558620689655172</v>
+      </c>
+      <c r="H2" s="69">
+        <f>'confusion matrices'!O8</f>
+        <v>0.75891996142719376</v>
+      </c>
+      <c r="I2" s="67">
+        <f>'confusion matrices'!I3</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="67">
+        <v>14032964</v>
+      </c>
+      <c r="K2" s="67">
+        <v>1000000</v>
+      </c>
+      <c r="L2" s="67">
+        <v>100000</v>
+      </c>
+      <c r="M2" s="67">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="67">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="52">
+      <c r="B3" s="70">
+        <f>'200ms'!B18</f>
+        <v>0.63029999999999997</v>
+      </c>
+      <c r="C3" s="70">
+        <f>'200ms'!B19</f>
+        <v>0.61629999999999996</v>
+      </c>
+      <c r="D3" s="70">
+        <v>0.59389999999999998</v>
+      </c>
+      <c r="E3" s="68">
+        <f>1-D3/C3</f>
+        <v>3.6345935421061126E-2</v>
+      </c>
+      <c r="F3" s="69">
+        <f>'confusion matrices'!N48</f>
+        <v>0.89714080917489647</v>
+      </c>
+      <c r="G3" s="69">
+        <f>'confusion matrices'!N49</f>
+        <v>0.76294490162213413</v>
+      </c>
+      <c r="H3" s="69">
+        <f>'confusion matrices'!O48</f>
+        <v>0.82461887593565264</v>
+      </c>
+      <c r="I3" s="67">
+        <v>6</v>
+      </c>
+      <c r="J3" s="67">
+        <v>88888996</v>
+      </c>
+      <c r="K3" s="67">
+        <v>600000</v>
+      </c>
+      <c r="L3" s="67">
+        <v>100000</v>
+      </c>
+      <c r="M3" s="67">
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="67">
         <v>300</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="52">
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="67">
         <v>400</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="52">
+      <c r="B5" s="70">
+        <f>'400ms'!B18</f>
+        <v>0.70740000000000003</v>
+      </c>
+      <c r="C5" s="70">
+        <f>'400ms'!B19</f>
+        <v>0.69110000000000005</v>
+      </c>
+      <c r="D5" s="70">
+        <f>'confusion matrices'!O35</f>
+        <v>0.66514904109764728</v>
+      </c>
+      <c r="E5" s="68">
+        <f>1-D5/C5</f>
+        <v>3.7550222691872026E-2</v>
+      </c>
+      <c r="F5" s="69">
+        <f>'confusion matrices'!N40</f>
+        <v>0.92923522548980164</v>
+      </c>
+      <c r="G5" s="69">
+        <f>'confusion matrices'!N41</f>
+        <v>0.84722884495470052</v>
+      </c>
+      <c r="H5" s="69">
+        <f>'confusion matrices'!O40</f>
+        <v>0.88633921719109754</v>
+      </c>
+      <c r="I5" s="67">
+        <f>'confusion matrices'!I35</f>
+        <v>5</v>
+      </c>
+      <c r="J5" s="67">
+        <v>185095844</v>
+      </c>
+      <c r="K5" s="67">
+        <v>600000</v>
+      </c>
+      <c r="L5" s="67">
+        <v>100000</v>
+      </c>
+      <c r="M5" s="67">
+        <v>5727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="67">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="52">
+      <c r="B6" s="70">
+        <f>'500ms'!H18</f>
+        <v>0.79020000000000001</v>
+      </c>
+      <c r="C6" s="70">
+        <f>'500ms'!H19</f>
+        <v>0.74980000000000002</v>
+      </c>
+      <c r="D6" s="70">
+        <f>'500ms'!H21</f>
+        <v>0.69498631436402913</v>
+      </c>
+      <c r="E6" s="68">
+        <f>1-D6/C6</f>
+        <v>7.3104408690278566E-2</v>
+      </c>
+      <c r="F6" s="69">
+        <f>'confusion matrices'!N64</f>
+        <v>0.82962119980490978</v>
+      </c>
+      <c r="G6" s="69">
+        <f>'confusion matrices'!N65</f>
+        <v>0.93667400881057272</v>
+      </c>
+      <c r="H6" s="69">
+        <f>'confusion matrices'!O64</f>
+        <v>0.87990343995171993</v>
+      </c>
+      <c r="I6" s="67">
+        <v>8</v>
+      </c>
+      <c r="J6" s="67">
+        <v>62149028</v>
+      </c>
+      <c r="K6" s="67">
+        <v>600000</v>
+      </c>
+      <c r="L6" s="67">
+        <v>50000</v>
+      </c>
+      <c r="M6" s="67">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="67">
         <v>1000</v>
       </c>
+      <c r="B7" s="70">
+        <f>'1000ms'!B18</f>
+        <v>0.79669999999999996</v>
+      </c>
+      <c r="C7" s="70">
+        <f>'1000ms'!B19</f>
+        <v>0.81159999999999999</v>
+      </c>
+      <c r="D7" s="70">
+        <f>'confusion matrices'!O27</f>
+        <v>0.77364353565212951</v>
+      </c>
+      <c r="E7" s="68">
+        <f>1-D7/C7</f>
+        <v>4.6767452375394925E-2</v>
+      </c>
+      <c r="F7" s="69">
+        <f>'confusion matrices'!N32</f>
+        <v>0.86464790971228744</v>
+      </c>
+      <c r="G7" s="69">
+        <f>'confusion matrices'!N33</f>
+        <v>0.97055937193326791</v>
+      </c>
+      <c r="H7" s="69">
+        <f>'confusion matrices'!O32</f>
+        <v>0.91454751796897993</v>
+      </c>
+      <c r="I7" s="67">
+        <f>'confusion matrices'!I27</f>
+        <v>4</v>
+      </c>
+      <c r="J7" s="67">
+        <v>123229860</v>
+      </c>
+      <c r="K7" s="67">
+        <v>600000</v>
+      </c>
+      <c r="L7" s="67">
+        <v>100000</v>
+      </c>
+      <c r="M7" s="67">
+        <v>3837</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="67">
+        <v>2000</v>
+      </c>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -998,8 +1395,8 @@
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="48" t="s">
-        <v>90</v>
+      <c r="B2" s="45" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1062,7 +1459,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1084,7 +1481,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1136,10 +1533,16 @@
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B21" s="49">
+        <v>0.77</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1163,7 +1566,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1171,7 +1574,7 @@
   <cols>
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
     <col min="2" max="7" width="25.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.77734375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="25.77734375" style="7" customWidth="1"/>
     <col min="9" max="9" width="25.77734375" style="2" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -1198,7 +1601,7 @@
       <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="6" t="s">
@@ -1227,11 +1630,11 @@
       <c r="G2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="14" t="s">
         <v>67</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1256,7 +1659,7 @@
       <c r="G3" s="2">
         <v>500</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="7">
         <v>500</v>
       </c>
       <c r="I3" s="2">
@@ -1285,7 +1688,7 @@
       <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1314,7 +1717,7 @@
       <c r="G5" s="2">
         <v>35</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="7">
         <v>40</v>
       </c>
       <c r="I5" s="2">
@@ -1343,7 +1746,7 @@
       <c r="G6" s="2">
         <v>600000</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="7">
         <v>600000</v>
       </c>
       <c r="I6" s="2">
@@ -1377,7 +1780,7 @@
       <c r="G7" s="2">
         <v>24000</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="7">
         <v>24000</v>
       </c>
       <c r="I7" s="2">
@@ -1406,7 +1809,7 @@
       <c r="G8" s="2">
         <v>2351</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="7">
         <v>1955</v>
       </c>
       <c r="I8" s="2">
@@ -1445,11 +1848,11 @@
       <c r="G11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="17" t="s">
-        <v>68</v>
+      <c r="H11" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1475,7 +1878,7 @@
         <f>G13*F12/F13</f>
         <v>21.102726063829788</v>
       </c>
-      <c r="H12" s="44"/>
+      <c r="H12" s="51"/>
       <c r="I12" s="37"/>
     </row>
     <row r="13" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1506,7 +1909,7 @@
         <f t="shared" si="1"/>
         <v>5.254894495010376</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H13" s="42">
         <f>H8*H6*4/1024/1024/1024</f>
         <v>4.3697655200958252</v>
       </c>
@@ -1537,11 +1940,11 @@
       <c r="G14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="17" t="s">
-        <v>69</v>
+      <c r="H14" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1566,7 +1969,7 @@
       <c r="G15" s="2">
         <v>64</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="7">
         <v>64</v>
       </c>
       <c r="I15" s="2">
@@ -1595,7 +1998,7 @@
       <c r="G16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -1624,7 +2027,7 @@
       <c r="G17" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="7">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="I17" s="2">
@@ -1636,7 +2039,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="3">
-        <v>0.89829999999999999</v>
+        <v>0.753</v>
       </c>
       <c r="C18" s="3">
         <v>0.72430000000000005</v>
@@ -1653,7 +2056,7 @@
       <c r="G18" s="38">
         <v>0.7621</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="41">
         <v>0.79020000000000001</v>
       </c>
       <c r="I18" s="38">
@@ -1665,7 +2068,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="4">
-        <v>0.67989999999999995</v>
+        <v>0.67549999999999999</v>
       </c>
       <c r="C19" s="3">
         <v>0.70209999999999995</v>
@@ -1682,7 +2085,7 @@
       <c r="G19" s="38">
         <v>0.67979999999999996</v>
       </c>
-      <c r="H19" s="45">
+      <c r="H19" s="52">
         <v>0.74980000000000002</v>
       </c>
       <c r="I19" s="39">
@@ -1704,18 +2107,25 @@
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
-      <c r="H20" s="19"/>
+      <c r="H20" s="40"/>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="H21" s="49">
+        <f>'confusion matrices'!O59</f>
+        <v>0.69498631436402913</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H22" s="7" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1741,11 +2151,38 @@
       <c r="G24" s="2">
         <v>1500</v>
       </c>
-      <c r="H24" s="17">
+      <c r="H24" s="7">
         <v>1365</v>
       </c>
       <c r="I24" s="2">
         <v>1365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="63" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="A25" s="62"/>
+      <c r="B25" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" s="63" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1756,9 +2193,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3C7494-2EAC-4FFC-8C4B-1EEE10737F24}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1779,15 +2216,15 @@
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>92</v>
+      <c r="B2" s="46" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="50">
+      <c r="B3" s="47">
         <v>400</v>
       </c>
     </row>
@@ -1846,7 +2283,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1868,7 +2305,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1899,7 +2336,7 @@
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="51">
+      <c r="B18" s="48">
         <v>0.70740000000000003</v>
       </c>
     </row>
@@ -1907,7 +2344,7 @@
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="51">
+      <c r="B19" s="48">
         <v>0.69110000000000005</v>
       </c>
     </row>
@@ -1920,11 +2357,18 @@
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B21" s="50">
+        <f>'confusion matrices'!O35</f>
+        <v>0.66514904109764728</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B22" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1937,6 +2381,22 @@
       </c>
       <c r="B24" s="17">
         <v>5949</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="17">
+        <v>377.28800000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="17">
+        <v>185095844</v>
       </c>
     </row>
   </sheetData>
@@ -1949,7 +2409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE69C90-D583-4A21-B578-829C81F8277B}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1978,14 +2440,14 @@
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="D2" s="45" t="s">
         <v>86</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1995,7 +2457,7 @@
       <c r="B3" s="29">
         <v>300</v>
       </c>
-      <c r="C3" s="50">
+      <c r="C3" s="47">
         <v>300</v>
       </c>
       <c r="D3" s="29">
@@ -2079,13 +2541,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2115,13 +2577,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2173,7 +2635,7 @@
       <c r="B18" s="3">
         <v>0.83940000000000003</v>
       </c>
-      <c r="C18" s="51">
+      <c r="C18" s="48">
         <v>0.68289999999999995</v>
       </c>
       <c r="D18" s="3">
@@ -2187,7 +2649,7 @@
       <c r="B19" s="4">
         <v>0.64019999999999999</v>
       </c>
-      <c r="C19" s="51">
+      <c r="C19" s="48">
         <v>0.6583</v>
       </c>
       <c r="D19" s="4">
@@ -2238,7 +2700,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2626C802-DDDB-45F4-B350-C34EEA285F2A}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2259,15 +2723,15 @@
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>89</v>
+      <c r="B2" s="46" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="50">
+      <c r="B3" s="47">
         <v>200</v>
       </c>
     </row>
@@ -2323,7 +2787,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2345,7 +2809,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2376,7 +2840,7 @@
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="51">
+      <c r="B18" s="48">
         <v>0.63029999999999997</v>
       </c>
     </row>
@@ -2384,7 +2848,7 @@
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="51">
+      <c r="B19" s="48">
         <v>0.61629999999999996</v>
       </c>
     </row>
@@ -2397,10 +2861,16 @@
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B21" s="48">
+        <v>0.59389999999999998</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2424,15 +2894,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE1B5DB-A7CE-4976-BA44-166DD16E4014}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
     <col min="2" max="3" width="25.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" style="26" customWidth="1"/>
     <col min="5" max="7" width="25.77734375" style="7" customWidth="1"/>
     <col min="8" max="9" width="25.77734375" style="17" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="2"/>
@@ -2445,13 +2917,13 @@
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="54" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="55" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -2477,21 +2949,21 @@
       <c r="C2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="56" t="s">
         <v>46</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="H2" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2504,7 +2976,7 @@
       <c r="C3" s="2">
         <v>100</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="26">
         <v>100</v>
       </c>
       <c r="E3" s="7">
@@ -2533,7 +3005,7 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="26" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -2562,7 +3034,7 @@
       <c r="C5" s="2">
         <v>35</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="26">
         <v>40</v>
       </c>
       <c r="E5" s="7">
@@ -2591,7 +3063,7 @@
       <c r="C6" s="2">
         <v>400000</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="26">
         <v>1000000</v>
       </c>
       <c r="E6" s="7">
@@ -2620,7 +3092,7 @@
       <c r="C7" s="2">
         <v>16000</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="26">
         <f>0.025*D6</f>
         <v>25000</v>
       </c>
@@ -2647,15 +3119,15 @@
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>79</v>
+      <c r="D8" s="26" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="26">
         <v>100000</v>
       </c>
     </row>
@@ -2669,7 +3141,7 @@
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -2679,13 +3151,13 @@
         <v>31</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2698,7 +3170,7 @@
       <c r="C11" s="2">
         <v>2.8</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="26">
         <v>6.8</v>
       </c>
       <c r="E11" s="7">
@@ -2718,23 +3190,23 @@
       <c r="C12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="26" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="G12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2747,7 +3219,7 @@
       <c r="C13" s="2">
         <v>64</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="26">
         <v>64</v>
       </c>
       <c r="E13" s="7">
@@ -2776,7 +3248,7 @@
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -2805,7 +3277,7 @@
       <c r="C15" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="26">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="E15" s="7">
@@ -2834,7 +3306,7 @@
       <c r="C16" s="10">
         <v>0.54039999999999999</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="57">
         <v>0.54349999999999998</v>
       </c>
       <c r="E16" s="11">
@@ -2861,7 +3333,7 @@
       <c r="C17" s="11">
         <v>0.5343</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="57">
         <v>0.55620000000000003</v>
       </c>
       <c r="E17" s="11">
@@ -2876,7 +3348,7 @@
       <c r="H17" s="18">
         <v>0.5575</v>
       </c>
-      <c r="I17" s="47">
+      <c r="I17" s="44">
         <v>0.55820000000000003</v>
       </c>
     </row>
@@ -2890,14 +3362,14 @@
       <c r="C18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="58" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
       <c r="G18" s="40"/>
       <c r="H18" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I18" s="19"/>
     </row>
@@ -2905,11 +3377,13 @@
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="59">
         <v>0.53539999999999999</v>
       </c>
       <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
+      <c r="F19" s="41">
+        <v>0.53359999999999996</v>
+      </c>
       <c r="G19" s="41"/>
       <c r="H19" s="28">
         <v>0.53129999999999999</v>
@@ -2922,7 +3396,7 @@
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="26" t="s">
         <v>25</v>
       </c>
       <c r="H20" s="17" t="s">
@@ -2936,7 +3410,7 @@
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="60">
         <f>'confusion matrices'!O8</f>
         <v>0.75891996142719376</v>
       </c>
@@ -2960,7 +3434,7 @@
       <c r="C22" s="2">
         <v>629</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="26">
         <v>986</v>
       </c>
       <c r="E22" s="7">
@@ -2968,6 +3442,34 @@
       </c>
       <c r="F22" s="7">
         <v>950</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="26">
+        <v>31.221</v>
+      </c>
+      <c r="H23" s="17">
+        <v>90.97</v>
+      </c>
+      <c r="I23" s="17">
+        <v>94.905000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="26">
+        <v>14032964</v>
+      </c>
+      <c r="H24" s="17">
+        <v>40616100</v>
+      </c>
+      <c r="I24" s="17">
+        <v>39989540</v>
       </c>
     </row>
   </sheetData>
@@ -2978,9 +3480,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B3942E-9FC7-4237-A72A-436C0A2724D2}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C43" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2989,10 +3493,11 @@
     <col min="8" max="8" width="12.77734375" style="21" customWidth="1"/>
     <col min="9" max="13" width="12.77734375" style="2" customWidth="1"/>
     <col min="14" max="15" width="12.77734375" style="24" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="21"/>
+    <col min="16" max="21" width="12.77734375" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>48</v>
       </c>
@@ -3000,7 +3505,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>24</v>
       </c>
@@ -3025,8 +3530,14 @@
       <c r="O2" s="24" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -3067,8 +3578,27 @@
         <f>AVERAGE(N3:N6)</f>
         <v>0.53541498568106682</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="61">
+        <f>K3</f>
+        <v>3797</v>
+      </c>
+      <c r="R3" s="61">
+        <f>L3*2</f>
+        <v>952</v>
+      </c>
+      <c r="S3" s="61">
+        <f>M3*3</f>
+        <v>567</v>
+      </c>
+      <c r="T3" s="38">
+        <f>SUM(P3:S6)/SUM(J3:M6)</f>
+        <v>0.56755999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B4" s="27">
         <v>186</v>
       </c>
@@ -3098,8 +3628,23 @@
         <f>K4/SUM(J4:M4)</f>
         <v>0.41851275296371693</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="61">
+        <f>J4</f>
+        <v>6431</v>
+      </c>
+      <c r="Q4" s="61">
+        <v>0</v>
+      </c>
+      <c r="R4" s="61">
+        <f>L4</f>
+        <v>4562</v>
+      </c>
+      <c r="S4" s="61">
+        <f>M4*2</f>
+        <v>7150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B5" s="27">
         <v>7</v>
       </c>
@@ -3129,8 +3674,23 @@
         <f>L5/SUM(J5:M5)</f>
         <v>0.23378860095325829</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="61">
+        <f>J5*2</f>
+        <v>3370</v>
+      </c>
+      <c r="Q5" s="61">
+        <f>K5</f>
+        <v>6912</v>
+      </c>
+      <c r="R5" s="61">
+        <v>0</v>
+      </c>
+      <c r="S5" s="61">
+        <f>M5</f>
+        <v>10533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B6" s="27">
         <v>1</v>
       </c>
@@ -3160,8 +3720,24 @@
         <f>M6/SUM(J6:M6)</f>
         <v>0.66838282247765002</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="61">
+        <f>J6*3</f>
+        <v>1266</v>
+      </c>
+      <c r="Q6" s="61">
+        <f>K6*2</f>
+        <v>6658</v>
+      </c>
+      <c r="R6" s="61">
+        <f>L6</f>
+        <v>4558</v>
+      </c>
+      <c r="S6" s="61">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
@@ -3182,8 +3758,14 @@
       <c r="O7" s="30" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+    </row>
+    <row r="8" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
@@ -3214,8 +3796,14 @@
         <f>2*N8*N9/(N8+N9)</f>
         <v>0.75891996142719376</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+    </row>
+    <row r="9" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
@@ -3243,8 +3831,14 @@
         <v>0.70558620689655172</v>
       </c>
       <c r="O9" s="30"/>
-    </row>
-    <row r="10" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" spans="1:21" s="32" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
@@ -3259,8 +3853,18 @@
       <c r="M10" s="29"/>
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="U10" s="7"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -3276,7 +3880,14 @@
       <c r="E11" s="27">
         <v>8</v>
       </c>
-      <c r="F11" s="24"/>
+      <c r="F11" s="24">
+        <f>B11/SUM(B11:E11)</f>
+        <v>0.96029240737664068</v>
+      </c>
+      <c r="G11" s="53">
+        <f>AVERAGE(F11:F14)</f>
+        <v>0.72283648809504553</v>
+      </c>
       <c r="I11" s="23">
         <v>2</v>
       </c>
@@ -3300,8 +3911,27 @@
         <f>AVERAGE(N11:N14)</f>
         <v>0.53129880080702363</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="61">
+        <f>K11</f>
+        <v>3500</v>
+      </c>
+      <c r="R11" s="61">
+        <f>L11*2</f>
+        <v>694</v>
+      </c>
+      <c r="S11" s="61">
+        <f>M11*3</f>
+        <v>642</v>
+      </c>
+      <c r="T11" s="38">
+        <f>SUM(P11:S14)/SUM(J11:M14)</f>
+        <v>0.56886999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B12" s="27">
         <v>553</v>
       </c>
@@ -3314,7 +3944,10 @@
       <c r="E12" s="27">
         <v>108</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" s="24">
+        <f>C12/SUM(B12:E12)</f>
+        <v>0.6551320628552324</v>
+      </c>
       <c r="J12" s="26">
         <v>7417</v>
       </c>
@@ -3331,8 +3964,23 @@
         <f>K12/SUM(J12:M12)</f>
         <v>0.39165367550065955</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12" s="61">
+        <f>J12</f>
+        <v>7417</v>
+      </c>
+      <c r="Q12" s="61">
+        <v>0</v>
+      </c>
+      <c r="R12" s="61">
+        <f>L12</f>
+        <v>4755</v>
+      </c>
+      <c r="S12" s="61">
+        <f>M12*2</f>
+        <v>6094</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B13" s="27">
         <v>36</v>
       </c>
@@ -3345,7 +3993,10 @@
       <c r="E13" s="27">
         <v>1842</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="24">
+        <f>D13/SUM(B13:E13)</f>
+        <v>0.52754729505476272</v>
+      </c>
       <c r="J13" s="26">
         <v>2016</v>
       </c>
@@ -3362,8 +4013,23 @@
         <f>L13/SUM(J13:M13)</f>
         <v>0.26275704493526275</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="61">
+        <f>J13*2</f>
+        <v>4032</v>
+      </c>
+      <c r="Q13" s="61">
+        <f>K13</f>
+        <v>6705</v>
+      </c>
+      <c r="R13" s="61">
+        <v>0</v>
+      </c>
+      <c r="S13" s="61">
+        <f>M13</f>
+        <v>9671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B14" s="27">
         <v>2</v>
       </c>
@@ -3376,7 +4042,10 @@
       <c r="E14" s="27">
         <v>4488</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="24">
+        <f>E14/SUM(B14:E14)</f>
+        <v>0.74837418709354675</v>
+      </c>
       <c r="J14" s="26">
         <v>505</v>
       </c>
@@ -3393,8 +4062,24 @@
         <f>M14/SUM(J14:M14)</f>
         <v>0.63323747903187155</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P14" s="61">
+        <f>J14*3</f>
+        <v>1515</v>
+      </c>
+      <c r="Q14" s="61">
+        <f>K14*2</f>
+        <v>6368</v>
+      </c>
+      <c r="R14" s="61">
+        <f>L14</f>
+        <v>5494</v>
+      </c>
+      <c r="S14" s="61">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -3411,8 +4096,14 @@
       <c r="M15" s="7"/>
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
-    </row>
-    <row r="16" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+    </row>
+    <row r="16" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="27">
         <f>B11</f>
@@ -3447,7 +4138,7 @@
       <c r="M16" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="46">
+      <c r="N16" s="43">
         <f>J16/SUM(J16:K16)</f>
         <v>0.83754700376030078</v>
       </c>
@@ -3455,8 +4146,14 @@
         <f>2*N16*N17/(N17+N16)</f>
         <v>0.74944964473001274</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+    </row>
+    <row r="17" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="27">
         <f>SUM(B12:B14)</f>
@@ -3488,16 +4185,28 @@
       <c r="M17" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="N17" s="46">
+      <c r="N17" s="43">
         <f>J16/SUM(J16:J17)</f>
         <v>0.67812145748987851</v>
       </c>
       <c r="O17" s="34"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+    </row>
+    <row r="18" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F18" s="24"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="T18" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>3</v>
       </c>
@@ -3532,8 +4241,27 @@
         <f>J19/SUM(J19:M19)</f>
         <v>0.87018961516921356</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="61">
+        <f>K19</f>
+        <v>2852</v>
+      </c>
+      <c r="R19" s="61">
+        <f>L19*2</f>
+        <v>516</v>
+      </c>
+      <c r="S19" s="61">
+        <f>M19*3</f>
+        <v>405</v>
+      </c>
+      <c r="T19" s="38">
+        <f>SUM(P19:S22)/SUM(J19:M22)</f>
+        <v>0.56186999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B20" s="27">
         <v>1072</v>
       </c>
@@ -3562,8 +4290,23 @@
         <f>K20/SUM(J20:M20)</f>
         <v>0.4278690490466483</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20" s="61">
+        <f>J20</f>
+        <v>7729</v>
+      </c>
+      <c r="Q20" s="61">
+        <v>0</v>
+      </c>
+      <c r="R20" s="61">
+        <f>L20</f>
+        <v>4647</v>
+      </c>
+      <c r="S20" s="61">
+        <f>M20*2</f>
+        <v>3874</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B21" s="27">
         <v>274</v>
       </c>
@@ -3592,8 +4335,23 @@
         <f>L21/SUM(J21:M21)</f>
         <v>0.31418607447789315</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21" s="61">
+        <f>J21*2</f>
+        <v>4340</v>
+      </c>
+      <c r="Q21" s="61">
+        <f>K21</f>
+        <v>7687</v>
+      </c>
+      <c r="R21" s="61">
+        <v>0</v>
+      </c>
+      <c r="S21" s="61">
+        <f>M21</f>
+        <v>7252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B22" s="27">
         <v>84</v>
       </c>
@@ -3622,23 +4380,24 @@
         <f>M22/SUM(J22:M22)</f>
         <v>0.52943525840722105</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>4</v>
-      </c>
-      <c r="B24" s="27">
-        <v>3319</v>
-      </c>
-      <c r="C24" s="27">
-        <v>554</v>
-      </c>
-      <c r="D24" s="27">
-        <v>35</v>
-      </c>
-      <c r="E24" s="27">
-        <v>18</v>
-      </c>
+      <c r="P22" s="61">
+        <f>J22*3</f>
+        <v>1710</v>
+      </c>
+      <c r="Q22" s="61">
+        <f>K22*2</f>
+        <v>7926</v>
+      </c>
+      <c r="R22" s="61">
+        <f>L22</f>
+        <v>7249</v>
+      </c>
+      <c r="S22" s="61">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J24" s="26">
         <f>J19</f>
         <v>21753</v>
@@ -3650,7 +4409,7 @@
       <c r="M24" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="N24" s="46">
+      <c r="N24" s="43">
         <f>J24/SUM(J24:K24)</f>
         <v>0.87018961516921356</v>
       </c>
@@ -3659,19 +4418,7 @@
         <v>0.76032855644879416</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="27">
-        <v>1124</v>
-      </c>
-      <c r="C25" s="27">
-        <v>1780</v>
-      </c>
-      <c r="D25" s="27">
-        <v>528</v>
-      </c>
-      <c r="E25" s="27">
-        <v>573</v>
-      </c>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J25" s="26">
         <f>SUM(J20:J22)</f>
         <v>10469</v>
@@ -3683,216 +4430,1172 @@
       <c r="M25" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="N25" s="46">
+      <c r="N25" s="43">
         <f>J24/SUM(J24:J25)</f>
         <v>0.67509775929489169</v>
       </c>
       <c r="O25" s="34"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="27">
+    <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P26" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="T26" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>4</v>
+      </c>
+      <c r="B27" s="27">
+        <v>3319</v>
+      </c>
+      <c r="C27" s="27">
+        <v>554</v>
+      </c>
+      <c r="D27" s="27">
+        <v>35</v>
+      </c>
+      <c r="E27" s="27">
+        <v>18</v>
+      </c>
+      <c r="I27" s="23">
+        <v>4</v>
+      </c>
+      <c r="J27" s="26">
+        <v>21758</v>
+      </c>
+      <c r="K27" s="26">
+        <v>3332</v>
+      </c>
+      <c r="L27" s="26">
+        <v>53</v>
+      </c>
+      <c r="M27" s="26">
+        <v>21</v>
+      </c>
+      <c r="N27" s="24">
+        <f>J27/SUM(J27:M27)</f>
+        <v>0.86464790971228744</v>
+      </c>
+      <c r="O27" s="24">
+        <f>AVERAGE(N27:N30)</f>
+        <v>0.77364353565212951</v>
+      </c>
+      <c r="P27" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="61">
+        <f>K27</f>
+        <v>3332</v>
+      </c>
+      <c r="R27" s="61">
+        <f>L27*2</f>
+        <v>106</v>
+      </c>
+      <c r="S27" s="61">
+        <f>M27*3</f>
+        <v>63</v>
+      </c>
+      <c r="T27" s="38">
+        <f>SUM(P27:S30)/SUM(J27:M30)</f>
+        <v>0.22989000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B28" s="27">
+        <v>1124</v>
+      </c>
+      <c r="C28" s="27">
+        <v>1780</v>
+      </c>
+      <c r="D28" s="27">
+        <v>528</v>
+      </c>
+      <c r="E28" s="27">
+        <v>573</v>
+      </c>
+      <c r="J28" s="26">
+        <v>653</v>
+      </c>
+      <c r="K28" s="26">
+        <v>19602</v>
+      </c>
+      <c r="L28" s="26">
+        <v>4670</v>
+      </c>
+      <c r="M28" s="26">
+        <v>127</v>
+      </c>
+      <c r="N28" s="24">
+        <f>K28/SUM(J28:M28)</f>
+        <v>0.78245249880249079</v>
+      </c>
+      <c r="P28" s="61">
+        <f>J28</f>
+        <v>653</v>
+      </c>
+      <c r="Q28" s="61">
+        <v>0</v>
+      </c>
+      <c r="R28" s="61">
+        <f>L28</f>
+        <v>4670</v>
+      </c>
+      <c r="S28" s="61">
+        <f>M28*2</f>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B29" s="27">
         <v>291</v>
       </c>
-      <c r="C26" s="27">
+      <c r="C29" s="27">
         <v>1267</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D29" s="27">
         <v>802</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E29" s="27">
         <v>1668</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="27">
+      <c r="J29" s="26">
+        <v>6</v>
+      </c>
+      <c r="K29" s="26">
+        <v>2847</v>
+      </c>
+      <c r="L29" s="26">
+        <v>15044</v>
+      </c>
+      <c r="M29" s="26">
+        <v>7206</v>
+      </c>
+      <c r="N29" s="24">
+        <f>L29/SUM(J29:M29)</f>
+        <v>0.59929092140381623</v>
+      </c>
+      <c r="P29" s="61">
+        <f>J29*2</f>
+        <v>12</v>
+      </c>
+      <c r="Q29" s="61">
+        <f>K29</f>
+        <v>2847</v>
+      </c>
+      <c r="R29" s="61">
+        <v>0</v>
+      </c>
+      <c r="S29" s="61">
+        <f>M29</f>
+        <v>7206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B30" s="27">
         <v>87</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C30" s="27">
         <v>665</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D30" s="27">
         <v>656</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E30" s="27">
         <v>2633</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+      <c r="J30" s="26">
+        <v>1</v>
+      </c>
+      <c r="K30" s="26">
+        <v>97</v>
+      </c>
+      <c r="L30" s="26">
+        <v>3649</v>
+      </c>
+      <c r="M30" s="26">
+        <v>20934</v>
+      </c>
+      <c r="N30" s="24">
+        <f>M30/SUM(J30:M30)</f>
+        <v>0.84818281268992346</v>
+      </c>
+      <c r="P30" s="61">
+        <f>J30*3</f>
+        <v>3</v>
+      </c>
+      <c r="Q30" s="61">
+        <f>K30*2</f>
+        <v>194</v>
+      </c>
+      <c r="R30" s="61">
+        <f>L30</f>
+        <v>3649</v>
+      </c>
+      <c r="S30" s="61">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>5</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B32" s="27">
         <v>5651</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C32" s="27">
         <v>345</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D32" s="27">
         <v>13</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E32" s="27">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B30" s="27">
+      <c r="J32" s="26">
+        <f>J27</f>
+        <v>21758</v>
+      </c>
+      <c r="K32" s="26">
+        <f>SUM(K27:M27)</f>
+        <v>3406</v>
+      </c>
+      <c r="M32" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="N32" s="43">
+        <f>J32/SUM(J32:K32)</f>
+        <v>0.86464790971228744</v>
+      </c>
+      <c r="O32" s="34">
+        <f>2*N32*N33/(N33+N32)</f>
+        <v>0.91454751796897993</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B33" s="27">
         <v>568</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C33" s="27">
         <v>4265</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D33" s="27">
         <v>1088</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E33" s="27">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B31" s="27">
+      <c r="J33" s="26">
+        <f>SUM(J28:J30)</f>
+        <v>660</v>
+      </c>
+      <c r="K33" s="26">
+        <f>SUM(K28:M30)</f>
+        <v>74176</v>
+      </c>
+      <c r="M33" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="N33" s="43">
+        <f>J32/SUM(J32:J33)</f>
+        <v>0.97055937193326791</v>
+      </c>
+      <c r="O33" s="34"/>
+    </row>
+    <row r="34" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B34" s="27">
         <v>26</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C34" s="27">
         <v>1387</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D34" s="27">
         <v>3164</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E34" s="27">
         <v>1449</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B32" s="27">
+      <c r="P34" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="T34" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B35" s="27">
         <v>3</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C35" s="27">
         <v>194</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D35" s="27">
         <v>1653</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E35" s="27">
         <v>4147</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+      <c r="I35" s="23">
+        <v>5</v>
+      </c>
+      <c r="J35" s="26">
+        <v>23098</v>
+      </c>
+      <c r="K35" s="26">
+        <v>1645</v>
+      </c>
+      <c r="L35" s="26">
+        <v>72</v>
+      </c>
+      <c r="M35" s="26">
+        <v>42</v>
+      </c>
+      <c r="N35" s="24">
+        <f>J35/SUM(J35:M35)</f>
+        <v>0.92923522548980164</v>
+      </c>
+      <c r="O35" s="24">
+        <f>AVERAGE(N35:N38)</f>
+        <v>0.66514904109764728</v>
+      </c>
+      <c r="P35" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="61">
+        <f>K35</f>
+        <v>1645</v>
+      </c>
+      <c r="R35" s="61">
+        <f>L35*2</f>
+        <v>144</v>
+      </c>
+      <c r="S35" s="61">
+        <f>M35*3</f>
+        <v>126</v>
+      </c>
+      <c r="T35" s="38">
+        <f>SUM(P35:S38)/SUM(J35:M38)</f>
+        <v>0.36002000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J36" s="26">
+        <v>3798</v>
+      </c>
+      <c r="K36" s="26">
+        <v>17658</v>
+      </c>
+      <c r="L36" s="26">
+        <v>3606</v>
+      </c>
+      <c r="M36" s="26">
+        <v>197</v>
+      </c>
+      <c r="N36" s="24">
+        <f>K36/SUM(J36:M36)</f>
+        <v>0.69907755651450965</v>
+      </c>
+      <c r="P36" s="61">
+        <f>J36</f>
+        <v>3798</v>
+      </c>
+      <c r="Q36" s="61">
+        <v>0</v>
+      </c>
+      <c r="R36" s="61">
+        <f>L36</f>
+        <v>3606</v>
+      </c>
+      <c r="S36" s="61">
+        <f>M36*2</f>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>6</v>
       </c>
-      <c r="B34" s="27">
+      <c r="B37" s="27">
         <v>5512</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C37" s="27">
         <v>616</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D37" s="27">
         <v>51</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E37" s="27">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="27">
+      <c r="J37" s="26">
+        <v>334</v>
+      </c>
+      <c r="K37" s="26">
+        <v>7959</v>
+      </c>
+      <c r="L37" s="26">
+        <v>12535</v>
+      </c>
+      <c r="M37" s="26">
+        <v>4040</v>
+      </c>
+      <c r="N37" s="24">
+        <f>L37/SUM(J37:M37)</f>
+        <v>0.5040614444265723</v>
+      </c>
+      <c r="P37" s="61">
+        <f>J37*2</f>
+        <v>668</v>
+      </c>
+      <c r="Q37" s="61">
+        <f>K37</f>
+        <v>7959</v>
+      </c>
+      <c r="R37" s="61">
+        <v>0</v>
+      </c>
+      <c r="S37" s="61">
+        <f>M37</f>
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B38" s="27">
         <v>1627</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C38" s="27">
         <v>2671</v>
       </c>
-      <c r="D35" s="27">
+      <c r="D38" s="27">
         <v>1095</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E38" s="27">
         <v>820</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="27">
+      <c r="J38" s="26">
+        <v>33</v>
+      </c>
+      <c r="K38" s="26">
+        <v>1754</v>
+      </c>
+      <c r="L38" s="26">
+        <v>10015</v>
+      </c>
+      <c r="M38" s="26">
+        <v>13214</v>
+      </c>
+      <c r="N38" s="24">
+        <f>M38/SUM(J38:M38)</f>
+        <v>0.52822193795970573</v>
+      </c>
+      <c r="P38" s="61">
+        <f>J38*3</f>
+        <v>99</v>
+      </c>
+      <c r="Q38" s="61">
+        <f>K38*2</f>
+        <v>3508</v>
+      </c>
+      <c r="R38" s="61">
+        <f>L38</f>
+        <v>10015</v>
+      </c>
+      <c r="S38" s="61">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B39" s="27">
         <v>392</v>
       </c>
-      <c r="C36" s="27">
+      <c r="C39" s="27">
         <v>1703</v>
       </c>
-      <c r="D36" s="27">
+      <c r="D39" s="27">
         <v>1525</v>
       </c>
-      <c r="E36" s="27">
+      <c r="E39" s="27">
         <v>2701</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="27">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B40" s="27">
         <v>85</v>
       </c>
-      <c r="C37" s="27">
+      <c r="C40" s="27">
         <v>851</v>
       </c>
-      <c r="D37" s="27">
+      <c r="D40" s="27">
         <v>1125</v>
       </c>
-      <c r="E37" s="27">
+      <c r="E40" s="27">
         <v>4196</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
+      <c r="J40" s="26">
+        <f>J35</f>
+        <v>23098</v>
+      </c>
+      <c r="K40" s="26">
+        <f>SUM(K35:M35)</f>
+        <v>1759</v>
+      </c>
+      <c r="M40" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="N40" s="43">
+        <f>J40/SUM(J40:K40)</f>
+        <v>0.92923522548980164</v>
+      </c>
+      <c r="O40" s="34">
+        <f>2*N40*N41/(N41+N40)</f>
+        <v>0.88633921719109754</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J41" s="26">
+        <f>SUM(J36:J38)</f>
+        <v>4165</v>
+      </c>
+      <c r="K41" s="26">
+        <f>SUM(K36:M38)</f>
+        <v>70978</v>
+      </c>
+      <c r="M41" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="N41" s="43">
+        <f>J40/SUM(J40:J41)</f>
+        <v>0.84722884495470052</v>
+      </c>
+      <c r="O41" s="34"/>
+    </row>
+    <row r="42" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>7</v>
       </c>
-      <c r="B39" s="27">
+      <c r="B42" s="27">
         <v>2937</v>
       </c>
-      <c r="C39" s="27">
+      <c r="C42" s="27">
         <v>492</v>
       </c>
-      <c r="D39" s="27">
+      <c r="D42" s="27">
         <v>42</v>
       </c>
-      <c r="E39" s="27">
+      <c r="E42" s="27">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="27">
+      <c r="P42" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="T42" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B43" s="27">
         <v>791</v>
       </c>
-      <c r="C40" s="27">
+      <c r="C43" s="27">
         <v>1425</v>
       </c>
-      <c r="D40" s="27">
+      <c r="D43" s="27">
         <v>755</v>
       </c>
-      <c r="E40" s="27">
+      <c r="E43" s="27">
         <v>547</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="27">
+      <c r="I43" s="23">
+        <v>6</v>
+      </c>
+      <c r="J43" s="26">
+        <v>22529</v>
+      </c>
+      <c r="K43" s="26">
+        <v>2401</v>
+      </c>
+      <c r="L43" s="26">
+        <v>103</v>
+      </c>
+      <c r="M43" s="26">
+        <v>79</v>
+      </c>
+      <c r="N43" s="24">
+        <f>J43/SUM(J43:M43)</f>
+        <v>0.89714080917489647</v>
+      </c>
+      <c r="O43" s="24">
+        <f>AVERAGE(N43:N46)</f>
+        <v>0.59392449034441019</v>
+      </c>
+      <c r="P43" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="61">
+        <f>K43</f>
+        <v>2401</v>
+      </c>
+      <c r="R43" s="61">
+        <f>L43*2</f>
+        <v>206</v>
+      </c>
+      <c r="S43" s="61">
+        <f>M43*3</f>
+        <v>237</v>
+      </c>
+      <c r="T43" s="38">
+        <f>SUM(P43:S46)/SUM(J43:M46)</f>
+        <v>0.46977999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B44" s="27">
         <v>159</v>
       </c>
-      <c r="C41" s="27">
+      <c r="C44" s="27">
         <v>799</v>
       </c>
-      <c r="D41" s="27">
+      <c r="D44" s="27">
         <v>925</v>
       </c>
-      <c r="E41" s="27">
+      <c r="E44" s="27">
         <v>1624</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="27">
+      <c r="J44" s="26">
+        <v>5857</v>
+      </c>
+      <c r="K44" s="26">
+        <v>14824</v>
+      </c>
+      <c r="L44" s="26">
+        <v>3215</v>
+      </c>
+      <c r="M44" s="26">
+        <v>1098</v>
+      </c>
+      <c r="N44" s="24">
+        <f>K44/SUM(J44:M44)</f>
+        <v>0.59310234456269506</v>
+      </c>
+      <c r="P44" s="61">
+        <f>J44</f>
+        <v>5857</v>
+      </c>
+      <c r="Q44" s="61">
+        <v>0</v>
+      </c>
+      <c r="R44" s="61">
+        <f>L44</f>
+        <v>3215</v>
+      </c>
+      <c r="S44" s="61">
+        <f>M44*2</f>
+        <v>2196</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B45" s="27">
         <v>46</v>
       </c>
-      <c r="C42" s="27">
+      <c r="C45" s="27">
         <v>303</v>
       </c>
-      <c r="D42" s="27">
+      <c r="D45" s="27">
         <v>638</v>
       </c>
-      <c r="E42" s="27">
+      <c r="E45" s="27">
         <v>2546</v>
       </c>
+      <c r="J45" s="26">
+        <v>972</v>
+      </c>
+      <c r="K45" s="26">
+        <v>9432</v>
+      </c>
+      <c r="L45" s="26">
+        <v>7232</v>
+      </c>
+      <c r="M45" s="26">
+        <v>7250</v>
+      </c>
+      <c r="N45" s="24">
+        <f>L45/SUM(J45:M45)</f>
+        <v>0.29060515952744514</v>
+      </c>
+      <c r="P45" s="61">
+        <f>J45*2</f>
+        <v>1944</v>
+      </c>
+      <c r="Q45" s="61">
+        <f>K45</f>
+        <v>9432</v>
+      </c>
+      <c r="R45" s="61">
+        <v>0</v>
+      </c>
+      <c r="S45" s="61">
+        <f>M45</f>
+        <v>7250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J46" s="26">
+        <v>171</v>
+      </c>
+      <c r="K46" s="26">
+        <v>3766</v>
+      </c>
+      <c r="L46" s="26">
+        <v>6195</v>
+      </c>
+      <c r="M46" s="26">
+        <v>14876</v>
+      </c>
+      <c r="N46" s="24">
+        <f>M46/SUM(J46:M46)</f>
+        <v>0.59484964811260399</v>
+      </c>
+      <c r="P46" s="61">
+        <f>J46*3</f>
+        <v>513</v>
+      </c>
+      <c r="Q46" s="61">
+        <f>K46*2</f>
+        <v>7532</v>
+      </c>
+      <c r="R46" s="61">
+        <f>L46</f>
+        <v>6195</v>
+      </c>
+      <c r="S46" s="61">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J48" s="26">
+        <f>J43</f>
+        <v>22529</v>
+      </c>
+      <c r="K48" s="26">
+        <f>SUM(K43:M43)</f>
+        <v>2583</v>
+      </c>
+      <c r="M48" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="N48" s="43">
+        <f>J48/SUM(J48:K48)</f>
+        <v>0.89714080917489647</v>
+      </c>
+      <c r="O48" s="34">
+        <f>2*N48*N49/(N49+N48)</f>
+        <v>0.82461887593565264</v>
+      </c>
+    </row>
+    <row r="49" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J49" s="26">
+        <f>SUM(J44:J46)</f>
+        <v>7000</v>
+      </c>
+      <c r="K49" s="26">
+        <f>SUM(K44:M46)</f>
+        <v>67888</v>
+      </c>
+      <c r="M49" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="N49" s="43">
+        <f>J48/SUM(J48:J49)</f>
+        <v>0.76294490162213413</v>
+      </c>
+      <c r="O49" s="34"/>
+    </row>
+    <row r="50" spans="9:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P50" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="T50" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I51" s="23">
+        <v>7</v>
+      </c>
+      <c r="J51" s="26">
+        <v>21124</v>
+      </c>
+      <c r="K51" s="26">
+        <v>3139</v>
+      </c>
+      <c r="L51" s="26">
+        <v>423</v>
+      </c>
+      <c r="M51" s="26">
+        <v>238</v>
+      </c>
+      <c r="N51" s="24">
+        <f>J51/SUM(J51:M51)</f>
+        <v>0.84753651099341998</v>
+      </c>
+      <c r="O51" s="24">
+        <f>AVERAGE(N51:N54)</f>
+        <v>0.53355537426088451</v>
+      </c>
+      <c r="P51" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="61">
+        <f>K51</f>
+        <v>3139</v>
+      </c>
+      <c r="R51" s="61">
+        <f>L51*2</f>
+        <v>846</v>
+      </c>
+      <c r="S51" s="61">
+        <f>M51*3</f>
+        <v>714</v>
+      </c>
+      <c r="T51" s="38">
+        <f>SUM(P51:S54)/SUM(J51:M54)</f>
+        <v>0.56971000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J52" s="26">
+        <v>7134</v>
+      </c>
+      <c r="K52" s="26">
+        <v>8705</v>
+      </c>
+      <c r="L52" s="26">
+        <v>5513</v>
+      </c>
+      <c r="M52" s="26">
+        <v>3701</v>
+      </c>
+      <c r="N52" s="24">
+        <f>K52/SUM(J52:M52)</f>
+        <v>0.34746337763940444</v>
+      </c>
+      <c r="P52" s="61">
+        <f>J52</f>
+        <v>7134</v>
+      </c>
+      <c r="Q52" s="61">
+        <v>0</v>
+      </c>
+      <c r="R52" s="61">
+        <f>L52</f>
+        <v>5513</v>
+      </c>
+      <c r="S52" s="61">
+        <f>M52*2</f>
+        <v>7402</v>
+      </c>
+    </row>
+    <row r="53" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J53" s="26">
+        <v>2036</v>
+      </c>
+      <c r="K53" s="26">
+        <v>5537</v>
+      </c>
+      <c r="L53" s="26">
+        <v>6771</v>
+      </c>
+      <c r="M53" s="26">
+        <v>10623</v>
+      </c>
+      <c r="N53" s="24">
+        <f>L53/SUM(J53:M53)</f>
+        <v>0.27119798133536266</v>
+      </c>
+      <c r="P53" s="61">
+        <f>J53*2</f>
+        <v>4072</v>
+      </c>
+      <c r="Q53" s="61">
+        <f>K53</f>
+        <v>5537</v>
+      </c>
+      <c r="R53" s="61">
+        <v>0</v>
+      </c>
+      <c r="S53" s="61">
+        <f>M53</f>
+        <v>10623</v>
+      </c>
+    </row>
+    <row r="54" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J54" s="26">
+        <v>544</v>
+      </c>
+      <c r="K54" s="26">
+        <v>2585</v>
+      </c>
+      <c r="L54" s="26">
+        <v>5189</v>
+      </c>
+      <c r="M54" s="26">
+        <v>16738</v>
+      </c>
+      <c r="N54" s="24">
+        <f>M54/SUM(J54:M54)</f>
+        <v>0.66802362707535123</v>
+      </c>
+      <c r="P54" s="61">
+        <f>J54*3</f>
+        <v>1632</v>
+      </c>
+      <c r="Q54" s="61">
+        <f>K54*2</f>
+        <v>5170</v>
+      </c>
+      <c r="R54" s="61">
+        <f>L54</f>
+        <v>5189</v>
+      </c>
+      <c r="S54" s="61">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J56" s="26">
+        <f>J51</f>
+        <v>21124</v>
+      </c>
+      <c r="K56" s="26">
+        <f>SUM(K51:M51)</f>
+        <v>3800</v>
+      </c>
+      <c r="M56" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="N56" s="43">
+        <f>J56/SUM(J56:K56)</f>
+        <v>0.84753651099341998</v>
+      </c>
+      <c r="O56" s="34">
+        <f>2*N56*N57/(N57+N56)</f>
+        <v>0.75764857788458084</v>
+      </c>
+    </row>
+    <row r="57" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J57" s="26">
+        <f>SUM(J52:J54)</f>
+        <v>9714</v>
+      </c>
+      <c r="K57" s="26">
+        <f>SUM(K52:M54)</f>
+        <v>65362</v>
+      </c>
+      <c r="M57" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="N57" s="43">
+        <f>J56/SUM(J56:J57)</f>
+        <v>0.68499902717426553</v>
+      </c>
+      <c r="O57" s="34"/>
+    </row>
+    <row r="58" spans="9:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P58" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="T58" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I59" s="23">
+        <v>8</v>
+      </c>
+      <c r="J59" s="26">
+        <v>10206</v>
+      </c>
+      <c r="K59" s="26">
+        <v>2035</v>
+      </c>
+      <c r="L59" s="26">
+        <v>35</v>
+      </c>
+      <c r="M59" s="26">
+        <v>26</v>
+      </c>
+      <c r="N59" s="24">
+        <f>J59/SUM(J59:M59)</f>
+        <v>0.82962119980490978</v>
+      </c>
+      <c r="O59" s="25">
+        <f>AVERAGE(N59:N62)</f>
+        <v>0.69498631436402913</v>
+      </c>
+      <c r="P59" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="61">
+        <f>K59</f>
+        <v>2035</v>
+      </c>
+      <c r="R59" s="61">
+        <f>L59*2</f>
+        <v>70</v>
+      </c>
+      <c r="S59" s="61">
+        <f>M59*3</f>
+        <v>78</v>
+      </c>
+      <c r="T59" s="38">
+        <f>SUM(P59:S62)/SUM(J59:M62)</f>
+        <v>0.31603999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J60" s="26">
+        <v>665</v>
+      </c>
+      <c r="K60" s="26">
+        <v>7820</v>
+      </c>
+      <c r="L60" s="26">
+        <v>3774</v>
+      </c>
+      <c r="M60" s="26">
+        <v>265</v>
+      </c>
+      <c r="N60" s="24">
+        <f>K60/SUM(J60:M60)</f>
+        <v>0.62440114979239858</v>
+      </c>
+      <c r="P60" s="61">
+        <f>J60</f>
+        <v>665</v>
+      </c>
+      <c r="Q60" s="61">
+        <v>0</v>
+      </c>
+      <c r="R60" s="61">
+        <f>L60</f>
+        <v>3774</v>
+      </c>
+      <c r="S60" s="61">
+        <f>M60*2</f>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="61" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J61" s="26">
+        <v>24</v>
+      </c>
+      <c r="K61" s="26">
+        <v>1382</v>
+      </c>
+      <c r="L61" s="26">
+        <v>6540</v>
+      </c>
+      <c r="M61" s="26">
+        <v>4704</v>
+      </c>
+      <c r="N61" s="24">
+        <f>L61/SUM(J61:M61)</f>
+        <v>0.51699604743083005</v>
+      </c>
+      <c r="P61" s="61">
+        <f>J61*2</f>
+        <v>48</v>
+      </c>
+      <c r="Q61" s="61">
+        <f>K61</f>
+        <v>1382</v>
+      </c>
+      <c r="R61" s="61">
+        <v>0</v>
+      </c>
+      <c r="S61" s="61">
+        <f>M61</f>
+        <v>4704</v>
+      </c>
+    </row>
+    <row r="62" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J62" s="26">
+        <v>1</v>
+      </c>
+      <c r="K62" s="26">
+        <v>121</v>
+      </c>
+      <c r="L62" s="26">
+        <v>2271</v>
+      </c>
+      <c r="M62" s="26">
+        <v>10131</v>
+      </c>
+      <c r="N62" s="24">
+        <f>M62/SUM(J62:M62)</f>
+        <v>0.80892686042797823</v>
+      </c>
+      <c r="P62" s="61">
+        <f>J62*3</f>
+        <v>3</v>
+      </c>
+      <c r="Q62" s="61">
+        <f>K62*2</f>
+        <v>242</v>
+      </c>
+      <c r="R62" s="61">
+        <f>L62</f>
+        <v>2271</v>
+      </c>
+      <c r="S62" s="61">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J64" s="26">
+        <f>J59</f>
+        <v>10206</v>
+      </c>
+      <c r="K64" s="26">
+        <f>SUM(K59:M59)</f>
+        <v>2096</v>
+      </c>
+      <c r="M64" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="N64" s="43">
+        <f>J64/SUM(J64:K64)</f>
+        <v>0.82962119980490978</v>
+      </c>
+      <c r="O64" s="34">
+        <f>2*N64*N65/(N65+N64)</f>
+        <v>0.87990343995171993</v>
+      </c>
+    </row>
+    <row r="65" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="J65" s="26">
+        <f>SUM(J60:J62)</f>
+        <v>690</v>
+      </c>
+      <c r="K65" s="26">
+        <f>SUM(K60:M62)</f>
+        <v>37008</v>
+      </c>
+      <c r="M65" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="N65" s="43">
+        <f>J64/SUM(J64:J65)</f>
+        <v>0.93667400881057272</v>
+      </c>
+      <c r="O65" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New data in the summary spreadsheet.
</commit_message>
<xml_diff>
--- a/model_building/summary_speaker_counting.xlsx
+++ b/model_building/summary_speaker_counting.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CF00B1-9957-4DC1-890A-FEC4B7A94A4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA26D673-562E-45D4-A64E-B2C7BE49D0B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="126">
   <si>
     <t>Metric</t>
   </si>
@@ -404,6 +404,9 @@
   </si>
   <si>
     <t>Number of Features</t>
+  </si>
+  <si>
+    <t>4 x 1D convolutional blocks with [3, 3, 3, 3] layers per block with [32, 64, 128, 256] filters of [16, 8, 4, 4]. Max pooling 1D [1, 2, 2, 2]. 3 x 1D Dense Layers of [1024, 1024, 512] with dropouts of [0.1, 0.1, 0.25]. After convolutional blocks dropout is 0.5. Batch normalization after convolutional blocks.</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,8 +488,15 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,6 +524,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,7 +568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -766,6 +788,39 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1053,7 +1108,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D627365-F01A-4583-8FA0-E181B91C71DE}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1130,7 +1185,7 @@
         <v>0.44829999999999998</v>
       </c>
       <c r="E2" s="36">
-        <f>1-D2/C2</f>
+        <f t="shared" ref="E2:E7" si="0">1-D2/C2</f>
         <v>4.9809241203899957E-2</v>
       </c>
       <c r="F2" s="37">
@@ -1157,7 +1212,7 @@
         <v>1000000</v>
       </c>
       <c r="L2" s="35">
-        <f t="shared" ref="L2:L10" si="0">0.04*K2</f>
+        <f t="shared" ref="L2:L9" si="1">0.04*K2</f>
         <v>40000</v>
       </c>
       <c r="M2" s="35">
@@ -1175,58 +1230,20 @@
       <c r="A3" s="35">
         <v>50</v>
       </c>
-      <c r="B3" s="36">
-        <f>'50ms'!B18</f>
-        <v>0.54410000000000003</v>
-      </c>
-      <c r="C3" s="36">
-        <f>'50ms'!B19</f>
-        <v>0.52410000000000001</v>
-      </c>
-      <c r="D3" s="36">
-        <f>'50ms'!B21</f>
-        <v>0.46760000000000002</v>
-      </c>
-      <c r="E3" s="36">
-        <f>1-D3/C3</f>
-        <v>0.10780385422629268</v>
-      </c>
-      <c r="F3" s="37">
-        <f>'confusion matrices'!N72</f>
-        <v>0.60120737216647346</v>
-      </c>
-      <c r="G3" s="37">
-        <f>'confusion matrices'!N73</f>
-        <v>0.68106884057971018</v>
-      </c>
-      <c r="H3" s="37">
-        <f>'confusion matrices'!O72</f>
-        <v>0.6386511795808294</v>
-      </c>
-      <c r="I3" s="35">
-        <v>9</v>
-      </c>
-      <c r="J3" s="35">
-        <f>'50ms'!B25</f>
-        <v>17576228</v>
-      </c>
-      <c r="K3" s="35">
-        <f>'100ms'!I3</f>
-        <v>350000</v>
-      </c>
-      <c r="L3" s="35">
-        <f t="shared" si="0"/>
-        <v>14000</v>
-      </c>
-      <c r="M3" s="35">
-        <v>100000</v>
-      </c>
-      <c r="N3" s="35">
-        <v>582</v>
-      </c>
-      <c r="O3" s="72" t="s">
-        <v>122</v>
-      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="72"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="35">
@@ -1245,7 +1262,7 @@
         <v>0.53539999999999999</v>
       </c>
       <c r="E4" s="36">
-        <f>1-D4/C4</f>
+        <f t="shared" si="0"/>
         <v>4.0845575062701589E-2</v>
       </c>
       <c r="F4" s="37">
@@ -1271,7 +1288,7 @@
         <v>600000</v>
       </c>
       <c r="L4" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24000</v>
       </c>
       <c r="M4" s="35">
@@ -1300,7 +1317,7 @@
         <v>0.59389999999999998</v>
       </c>
       <c r="E5" s="36">
-        <f>1-D5/C5</f>
+        <f t="shared" si="0"/>
         <v>3.6345935421061126E-2</v>
       </c>
       <c r="F5" s="37">
@@ -1325,7 +1342,7 @@
         <v>600000</v>
       </c>
       <c r="L5" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24000</v>
       </c>
       <c r="M5" s="35">
@@ -1342,19 +1359,56 @@
       <c r="A6" s="35">
         <v>300</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
+      <c r="B6" s="38">
+        <f>'300ms'!C18</f>
+        <v>0.68289999999999995</v>
+      </c>
+      <c r="C6" s="38">
+        <f>'300ms'!C19</f>
+        <v>0.6583</v>
+      </c>
+      <c r="D6" s="38">
+        <f>'confusion matrices'!O83</f>
+        <v>0.63865926423613417</v>
+      </c>
+      <c r="E6" s="36">
+        <f t="shared" si="0"/>
+        <v>2.9835539668640165E-2</v>
+      </c>
+      <c r="F6" s="37">
+        <f>'confusion matrices'!N88</f>
+        <v>0.93323669163243939</v>
+      </c>
+      <c r="G6" s="37">
+        <f>'confusion matrices'!N89</f>
+        <v>0.80643028637043734</v>
+      </c>
+      <c r="H6" s="37">
+        <f>'confusion matrices'!O88</f>
+        <v>0.86521195378268911</v>
+      </c>
+      <c r="I6" s="35">
+        <v>11</v>
+      </c>
+      <c r="J6" s="35">
+        <f>'300ms'!C25</f>
+        <v>137123492</v>
+      </c>
+      <c r="K6" s="35">
+        <f>'300ms'!C6</f>
+        <v>600000</v>
+      </c>
+      <c r="L6" s="35">
+        <f t="shared" si="1"/>
+        <v>24000</v>
+      </c>
+      <c r="M6" s="35">
+        <v>100000</v>
+      </c>
+      <c r="N6" s="35">
+        <f>'300ms'!C8</f>
+        <v>4258</v>
+      </c>
       <c r="O6" s="72" t="s">
         <v>122</v>
       </c>
@@ -1376,7 +1430,7 @@
         <v>0.66514904109764728</v>
       </c>
       <c r="E7" s="36">
-        <f>1-D7/C7</f>
+        <f t="shared" si="0"/>
         <v>3.7550222691872026E-2</v>
       </c>
       <c r="F7" s="37">
@@ -1402,7 +1456,7 @@
         <v>600000</v>
       </c>
       <c r="L7" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24000</v>
       </c>
       <c r="M7" s="35">
@@ -1419,56 +1473,20 @@
       <c r="A8" s="35">
         <v>500</v>
       </c>
-      <c r="B8" s="38">
-        <f>'500ms'!J18</f>
-        <v>0.79020000000000001</v>
-      </c>
-      <c r="C8" s="38">
-        <f>'500ms'!J19</f>
-        <v>0.74980000000000002</v>
-      </c>
-      <c r="D8" s="38">
-        <f>'500ms'!J21</f>
-        <v>0.69498631436402913</v>
-      </c>
-      <c r="E8" s="36">
-        <f>1-D8/C8</f>
-        <v>7.3104408690278566E-2</v>
-      </c>
-      <c r="F8" s="37">
-        <f>'confusion matrices'!N64</f>
-        <v>0.82962119980490978</v>
-      </c>
-      <c r="G8" s="37">
-        <f>'confusion matrices'!N65</f>
-        <v>0.93667400881057272</v>
-      </c>
-      <c r="H8" s="37">
-        <f>'confusion matrices'!O64</f>
-        <v>0.87990343995171993</v>
-      </c>
-      <c r="I8" s="35">
-        <v>8</v>
-      </c>
-      <c r="J8" s="35">
-        <v>62149028</v>
-      </c>
-      <c r="K8" s="35">
-        <v>600000</v>
-      </c>
-      <c r="L8" s="35">
-        <f t="shared" si="0"/>
-        <v>24000</v>
-      </c>
-      <c r="M8" s="35">
-        <v>50000</v>
-      </c>
-      <c r="N8" s="35">
-        <v>1955</v>
-      </c>
-      <c r="O8" s="72" t="s">
-        <v>123</v>
-      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="72"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="35">
@@ -1513,7 +1531,7 @@
         <v>600000</v>
       </c>
       <c r="L9" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24000</v>
       </c>
       <c r="M9" s="35">
@@ -1526,60 +1544,189 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="35">
+    <row r="10" spans="1:15" s="83" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="78"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="82"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="35">
+        <v>50</v>
+      </c>
+      <c r="B11" s="36">
+        <f>'50ms'!B18</f>
+        <v>0.54410000000000003</v>
+      </c>
+      <c r="C11" s="36">
+        <f>'50ms'!B19</f>
+        <v>0.52410000000000001</v>
+      </c>
+      <c r="D11" s="36">
+        <f>'50ms'!B21</f>
+        <v>0.46760000000000002</v>
+      </c>
+      <c r="E11" s="84">
+        <f>1-D11/C11</f>
+        <v>0.10780385422629268</v>
+      </c>
+      <c r="F11" s="37">
+        <f>'confusion matrices'!N72</f>
+        <v>0.60120737216647346</v>
+      </c>
+      <c r="G11" s="37">
+        <f>'confusion matrices'!N73</f>
+        <v>0.68106884057971018</v>
+      </c>
+      <c r="H11" s="37">
+        <f>'confusion matrices'!O72</f>
+        <v>0.6386511795808294</v>
+      </c>
+      <c r="I11" s="35">
+        <v>9</v>
+      </c>
+      <c r="J11" s="35">
+        <f>'50ms'!B25</f>
+        <v>17576228</v>
+      </c>
+      <c r="K11" s="35">
+        <f>'100ms'!I3</f>
+        <v>350000</v>
+      </c>
+      <c r="L11" s="35">
+        <f>0.04*K11</f>
+        <v>14000</v>
+      </c>
+      <c r="M11" s="35">
+        <v>100000</v>
+      </c>
+      <c r="N11" s="35">
+        <v>582</v>
+      </c>
+      <c r="O11" s="72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="35">
         <v>100</v>
       </c>
-      <c r="B10" s="36">
-        <f>'100ms'!I13</f>
-        <v>0.55889999999999995</v>
-      </c>
-      <c r="C10" s="36">
-        <f>'100ms'!I14</f>
-        <v>0.55820000000000003</v>
-      </c>
-      <c r="D10" s="36">
+      <c r="B12" s="36">
+        <f>'100ms'!D13</f>
+        <v>0.54349999999999998</v>
+      </c>
+      <c r="C12" s="36">
+        <f>'100ms'!D14</f>
+        <v>0.55620000000000003</v>
+      </c>
+      <c r="D12" s="36">
         <f>'100ms'!I16</f>
         <v>0.53539999999999999</v>
       </c>
-      <c r="E10" s="36">
-        <f>1-D10/C10</f>
-        <v>4.0845575062701589E-2</v>
-      </c>
-      <c r="F10" s="37">
+      <c r="E12" s="36">
+        <f>1-D12/C12</f>
+        <v>3.7396619920891827E-2</v>
+      </c>
+      <c r="F12" s="37">
         <f>'confusion matrices'!N8</f>
         <v>0.82097576632964209</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G12" s="37">
         <f>'confusion matrices'!N9</f>
         <v>0.70558620689655172</v>
       </c>
-      <c r="H10" s="37">
+      <c r="H12" s="37">
         <f>'confusion matrices'!O8</f>
         <v>0.75891996142719376</v>
       </c>
-      <c r="I10" s="35">
+      <c r="I12" s="35">
         <f>'confusion matrices'!I3</f>
         <v>1</v>
       </c>
-      <c r="J10" s="35">
+      <c r="J12" s="35">
         <v>14032964</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K12" s="35">
         <v>1000000</v>
       </c>
-      <c r="L10" s="35">
-        <f t="shared" si="0"/>
+      <c r="L12" s="35">
+        <f>0.04*K12</f>
         <v>40000</v>
       </c>
-      <c r="M10" s="35">
+      <c r="M12" s="35">
         <v>100000</v>
       </c>
-      <c r="N10" s="35">
+      <c r="N12" s="35">
         <v>451</v>
       </c>
-      <c r="O10" s="72" t="s">
+      <c r="O12" s="72" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="35">
+        <v>500</v>
+      </c>
+      <c r="B13" s="38">
+        <f>'500ms'!K18</f>
+        <v>0.79020000000000001</v>
+      </c>
+      <c r="C13" s="38">
+        <f>'500ms'!K19</f>
+        <v>0.74980000000000002</v>
+      </c>
+      <c r="D13" s="38">
+        <f>'500ms'!K21</f>
+        <v>0.69498631436402913</v>
+      </c>
+      <c r="E13" s="36">
+        <f>1-D13/C13</f>
+        <v>7.3104408690278566E-2</v>
+      </c>
+      <c r="F13" s="37">
+        <f>'confusion matrices'!N64</f>
+        <v>0.82962119980490978</v>
+      </c>
+      <c r="G13" s="37">
+        <f>'confusion matrices'!N65</f>
+        <v>0.93667400881057272</v>
+      </c>
+      <c r="H13" s="37">
+        <f>'confusion matrices'!O64</f>
+        <v>0.87990343995171993</v>
+      </c>
+      <c r="I13" s="35">
+        <v>8</v>
+      </c>
+      <c r="J13" s="35">
+        <v>62149028</v>
+      </c>
+      <c r="K13" s="35">
+        <v>600000</v>
+      </c>
+      <c r="L13" s="35">
+        <f>0.04*K13</f>
+        <v>24000</v>
+      </c>
+      <c r="M13" s="35">
+        <v>50000</v>
+      </c>
+      <c r="N13" s="35">
+        <v>1955</v>
+      </c>
+      <c r="O13" s="72" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1590,9 +1737,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B3942E-9FC7-4237-A72A-436C0A2724D2}">
-  <dimension ref="A1:U81"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0"/>
+    <sheetView topLeftCell="A67" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4070,7 +4217,7 @@
         <v>0.62963816547591611</v>
       </c>
     </row>
-    <row r="81" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="9:20" x14ac:dyDescent="0.3">
       <c r="J81" s="14">
         <f>SUM(J76:J78)</f>
         <v>13660</v>
@@ -4087,6 +4234,197 @@
         <v>0.56521739130434778</v>
       </c>
       <c r="O81" s="21"/>
+    </row>
+    <row r="82" spans="9:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P82" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="T82" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I83" s="11">
+        <v>11</v>
+      </c>
+      <c r="J83" s="14">
+        <v>23176</v>
+      </c>
+      <c r="K83" s="14">
+        <v>1555</v>
+      </c>
+      <c r="L83" s="14">
+        <v>56</v>
+      </c>
+      <c r="M83" s="14">
+        <v>47</v>
+      </c>
+      <c r="N83" s="12">
+        <f>J83/SUM(J83:M83)</f>
+        <v>0.93323669163243939</v>
+      </c>
+      <c r="O83" s="13">
+        <f>AVERAGE(N83:N86)</f>
+        <v>0.63865926423613417</v>
+      </c>
+      <c r="P83" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="31">
+        <f>K83</f>
+        <v>1555</v>
+      </c>
+      <c r="R83" s="31">
+        <f>L83*2</f>
+        <v>112</v>
+      </c>
+      <c r="S83" s="31">
+        <f>M83*3</f>
+        <v>141</v>
+      </c>
+      <c r="T83" s="23">
+        <f>SUM(P83:S86)/SUM(J83:M86)</f>
+        <v>0.39834000000000003</v>
+      </c>
+    </row>
+    <row r="84" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J84" s="14">
+        <v>4907</v>
+      </c>
+      <c r="K84" s="14">
+        <v>15996</v>
+      </c>
+      <c r="L84" s="14">
+        <v>3744</v>
+      </c>
+      <c r="M84" s="14">
+        <v>544</v>
+      </c>
+      <c r="N84" s="12">
+        <f>K84/SUM(J84:M84)</f>
+        <v>0.63498868643563178</v>
+      </c>
+      <c r="P84" s="31">
+        <f>J84</f>
+        <v>4907</v>
+      </c>
+      <c r="Q84" s="31">
+        <v>0</v>
+      </c>
+      <c r="R84" s="31">
+        <f>L84</f>
+        <v>3744</v>
+      </c>
+      <c r="S84" s="31">
+        <f>M84*2</f>
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="85" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J85" s="14">
+        <v>595</v>
+      </c>
+      <c r="K85" s="14">
+        <v>8331</v>
+      </c>
+      <c r="L85" s="14">
+        <v>9833</v>
+      </c>
+      <c r="M85" s="14">
+        <v>6193</v>
+      </c>
+      <c r="N85" s="12">
+        <f>L85/SUM(J85:M85)</f>
+        <v>0.3940766271240782</v>
+      </c>
+      <c r="P85" s="31">
+        <f>J85*2</f>
+        <v>1190</v>
+      </c>
+      <c r="Q85" s="31">
+        <f>K85</f>
+        <v>8331</v>
+      </c>
+      <c r="R85" s="31">
+        <v>0</v>
+      </c>
+      <c r="S85" s="31">
+        <f>M85</f>
+        <v>6193</v>
+      </c>
+    </row>
+    <row r="86" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J86" s="14">
+        <v>61</v>
+      </c>
+      <c r="K86" s="14">
+        <v>2250</v>
+      </c>
+      <c r="L86" s="14">
+        <v>7890</v>
+      </c>
+      <c r="M86" s="14">
+        <v>14822</v>
+      </c>
+      <c r="N86" s="12">
+        <f>M86/SUM(J86:M86)</f>
+        <v>0.59233505175238776</v>
+      </c>
+      <c r="P86" s="31">
+        <f>J86*3</f>
+        <v>183</v>
+      </c>
+      <c r="Q86" s="31">
+        <f>K86*2</f>
+        <v>4500</v>
+      </c>
+      <c r="R86" s="31">
+        <f>L86</f>
+        <v>7890</v>
+      </c>
+      <c r="S86" s="31">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J88" s="14">
+        <f>J83</f>
+        <v>23176</v>
+      </c>
+      <c r="K88" s="14">
+        <f>SUM(K83:M83)</f>
+        <v>1658</v>
+      </c>
+      <c r="M88" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="N88" s="24">
+        <f>J88/SUM(J88:K88)</f>
+        <v>0.93323669163243939</v>
+      </c>
+      <c r="O88" s="21">
+        <f>2*N88*N89/(N89+N88)</f>
+        <v>0.86521195378268911</v>
+      </c>
+    </row>
+    <row r="89" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="J89" s="14">
+        <f>SUM(J84:J86)</f>
+        <v>5563</v>
+      </c>
+      <c r="K89" s="14">
+        <f>SUM(K84:M86)</f>
+        <v>69603</v>
+      </c>
+      <c r="M89" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N89" s="24">
+        <f>J88/SUM(J88:J89)</f>
+        <v>0.80643028637043734</v>
+      </c>
+      <c r="O89" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4098,7 +4436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C0A8CF-24A5-41AD-B8F9-22B8D89DACCE}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4295,20 +4633,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
-    <col min="2" max="9" width="25.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.77734375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="25.77734375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="10" width="25.77734375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="25.77734375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="25.77734375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4336,14 +4674,17 @@
       <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>32</v>
       </c>
@@ -4371,14 +4712,15 @@
       <c r="I2" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="59"/>
+      <c r="K2" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="59" t="s">
+      <c r="L2" s="59" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
         <v>2</v>
       </c>
@@ -4406,14 +4748,17 @@
       <c r="I3" s="31">
         <v>500</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="31">
         <v>500</v>
       </c>
-      <c r="K3" s="31">
+      <c r="K3" s="14">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="31">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>4</v>
       </c>
@@ -4441,14 +4786,17 @@
       <c r="I4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
         <v>3</v>
       </c>
@@ -4476,14 +4824,17 @@
       <c r="I5" s="31">
         <v>50</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="31">
+        <v>50</v>
+      </c>
+      <c r="K5" s="14">
         <v>40</v>
       </c>
-      <c r="K5" s="31">
+      <c r="L5" s="31">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="46" t="s">
         <v>8</v>
       </c>
@@ -4511,14 +4862,17 @@
       <c r="I6" s="31">
         <v>600000</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="31">
         <v>600000</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="14">
         <v>600000</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="31">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
         <v>7</v>
       </c>
@@ -4552,14 +4906,18 @@
         <f>0.04*I6</f>
         <v>24000</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="31">
+        <f>0.04*J6</f>
         <v>24000</v>
       </c>
-      <c r="K7" s="31">
+      <c r="K7" s="14">
         <v>24000</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="31">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
         <v>43</v>
       </c>
@@ -4587,14 +4945,17 @@
       <c r="I8" s="31">
         <v>7197</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="31">
+        <v>7197</v>
+      </c>
+      <c r="K8" s="14">
         <v>1955</v>
       </c>
-      <c r="K8" s="31">
+      <c r="L8" s="31">
         <v>1955</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>5</v>
       </c>
@@ -4606,10 +4967,11 @@
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
       <c r="I9" s="31"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="31"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J9" s="31"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
         <v>6</v>
       </c>
@@ -4621,10 +4983,11 @@
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="31"/>
-    </row>
-    <row r="11" spans="1:11" ht="139.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="31"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" ht="139.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="46" t="s">
         <v>9</v>
       </c>
@@ -4652,14 +5015,17 @@
       <c r="I11" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="K11" s="31" t="s">
+      <c r="L11" s="31" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
         <v>30</v>
       </c>
@@ -4688,10 +5054,13 @@
       <c r="I12" s="60">
         <v>64</v>
       </c>
-      <c r="J12" s="68"/>
-      <c r="K12" s="60"/>
-    </row>
-    <row r="13" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="60">
+        <v>64</v>
+      </c>
+      <c r="K12" s="68"/>
+      <c r="L12" s="60"/>
+    </row>
+    <row r="13" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
         <v>44</v>
       </c>
@@ -4727,16 +5096,20 @@
         <f t="shared" si="1"/>
         <v>16.086548566818237</v>
       </c>
-      <c r="J13" s="30">
-        <f>J8*J6*4/1024/1024/1024</f>
-        <v>4.3697655200958252</v>
-      </c>
-      <c r="K13" s="55">
+      <c r="J13" s="55">
+        <f t="shared" ref="J13" si="2">J6*J8*4/1024/1024/1024</f>
+        <v>16.086548566818237</v>
+      </c>
+      <c r="K13" s="30">
         <f>K8*K6*4/1024/1024/1024</f>
         <v>4.3697655200958252</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="L13" s="55">
+        <f>L8*L6*4/1024/1024/1024</f>
+        <v>4.3697655200958252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A14" s="46" t="s">
         <v>10</v>
       </c>
@@ -4764,14 +5137,17 @@
       <c r="I14" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="K14" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="31" t="s">
+      <c r="L14" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="46" t="s">
         <v>19</v>
       </c>
@@ -4799,14 +5175,17 @@
       <c r="I15" s="31">
         <v>64</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="31">
         <v>64</v>
       </c>
-      <c r="K15" s="31">
+      <c r="K15" s="14">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" s="31">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="46" t="s">
         <v>20</v>
       </c>
@@ -4834,14 +5213,17 @@
       <c r="I16" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="31" t="s">
+      <c r="K16" s="14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="46" t="s">
         <v>22</v>
       </c>
@@ -4869,14 +5251,17 @@
       <c r="I17" s="31">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="31">
+        <v>1E-4</v>
+      </c>
+      <c r="K17" s="14">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="K17" s="31">
+      <c r="L17" s="31">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
         <v>11</v>
       </c>
@@ -4901,15 +5286,18 @@
       <c r="H18" s="62">
         <v>0.69669999999999999</v>
       </c>
-      <c r="I18" s="62"/>
-      <c r="J18" s="29">
+      <c r="I18" s="62">
+        <v>0.77070000000000005</v>
+      </c>
+      <c r="J18" s="62"/>
+      <c r="K18" s="29">
         <v>0.79020000000000001</v>
       </c>
-      <c r="K18" s="62">
+      <c r="L18" s="62">
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
         <v>12</v>
       </c>
@@ -4934,15 +5322,18 @@
       <c r="H19" s="62">
         <v>0.69789999999999996</v>
       </c>
-      <c r="I19" s="62"/>
-      <c r="J19" s="69">
+      <c r="I19" s="62">
+        <v>0.71050000000000002</v>
+      </c>
+      <c r="J19" s="62"/>
+      <c r="K19" s="69">
         <v>0.74980000000000002</v>
       </c>
-      <c r="K19" s="63">
+      <c r="L19" s="63">
         <v>0.74060000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
         <v>15</v>
       </c>
@@ -4960,10 +5351,11 @@
       <c r="G20" s="50"/>
       <c r="H20" s="50"/>
       <c r="I20" s="50"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="50"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J20" s="50"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="50"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="46" t="s">
         <v>16</v>
       </c>
@@ -4975,13 +5367,14 @@
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
       <c r="I21" s="31"/>
-      <c r="J21" s="58">
+      <c r="J21" s="31"/>
+      <c r="K21" s="58">
         <f>'confusion matrices'!O59</f>
         <v>0.69498631436402913</v>
       </c>
-      <c r="K21" s="31"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" s="31"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
         <v>17</v>
       </c>
@@ -4993,12 +5386,13 @@
       <c r="G22" s="31"/>
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="31"/>
+      <c r="K22" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K22" s="31"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="31"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="46" t="s">
         <v>26</v>
       </c>
@@ -5010,10 +5404,11 @@
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="31"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J23" s="31"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="31"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="46" t="s">
         <v>28</v>
       </c>
@@ -5039,14 +5434,17 @@
       <c r="I24" s="31">
         <v>4710</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="31">
+        <v>4710</v>
+      </c>
+      <c r="K24" s="14">
         <v>1365</v>
       </c>
-      <c r="K24" s="31">
+      <c r="L24" s="31">
         <v>1365</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.3">
       <c r="A25" s="65"/>
       <c r="B25" s="66" t="s">
         <v>105</v>
@@ -5072,10 +5470,13 @@
       <c r="I25" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="J25" s="70" t="s">
+      <c r="J25" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="K25" s="66" t="s">
+      <c r="L25" s="66" t="s">
         <v>101</v>
       </c>
     </row>
@@ -5089,7 +5490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3C7494-2EAC-4FFC-8C4B-1EEE10737F24}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5305,7 +5706,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE69C90-D583-4A21-B578-829C81F8277B}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5422,7 +5823,9 @@
         <v>43</v>
       </c>
       <c r="B8" s="31"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="14">
+        <v>4258</v>
+      </c>
       <c r="D8" s="31"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5533,31 +5936,31 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="s">
+    <row r="18" spans="1:4" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="56">
+      <c r="B18" s="77">
         <v>0.83940000000000003</v>
       </c>
-      <c r="C18" s="53">
+      <c r="C18" s="77">
         <v>0.68289999999999995</v>
       </c>
-      <c r="D18" s="56">
+      <c r="D18" s="77">
         <v>0.64309000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46" t="s">
+    <row r="19" spans="1:4" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="57">
+      <c r="B19" s="77">
         <v>0.64019999999999999</v>
       </c>
-      <c r="C19" s="53">
+      <c r="C19" s="77">
         <v>0.6583</v>
       </c>
-      <c r="D19" s="57">
+      <c r="D19" s="77">
         <v>0.63729999999999998</v>
       </c>
     </row>
@@ -5569,13 +5972,15 @@
       <c r="C20" s="14"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="46" t="s">
+    <row r="21" spans="1:4" s="76" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="31"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="77">
+        <v>0.63870000000000005</v>
+      </c>
+      <c r="D21" s="75"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
@@ -5606,6 +6011,16 @@
       <c r="D24" s="31">
         <v>3300</v>
       </c>
+    </row>
+    <row r="25" spans="1:4" s="76" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75">
+        <v>137123492</v>
+      </c>
+      <c r="D25" s="75"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5824,7 +6239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE1B5DB-A7CE-4976-BA44-166DD16E4014}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B10" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -6374,7 +6789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A5FAF3-C0D2-4D79-B23C-18AD251D1D2D}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Continued working at the paper's sketch.
</commit_message>
<xml_diff>
--- a/model_building/summary_speaker_counting.xlsx
+++ b/model_building/summary_speaker_counting.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4431C2B-C9D7-41B9-B76A-D4CAF41F554D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56C4AB4-8F51-49C1-B5DC-CDB2AD91B9AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="775" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="158">
   <si>
     <t>Metric</t>
   </si>
@@ -492,6 +492,18 @@
   </si>
   <si>
     <t>2D Features + Extra Convolutional Layer</t>
+  </si>
+  <si>
+    <t>1D Features (FFT, Envelope, Histogram)</t>
+  </si>
+  <si>
+    <t>1D Features + 2.5X More Training Examples</t>
+  </si>
+  <si>
+    <t>1D Features + 2D Features (Spectrogram, Envelope, Histogram)</t>
+  </si>
+  <si>
+    <t>1D Features + 2D Features + Higher Order Filters</t>
   </si>
 </sst>
 </file>
@@ -1001,15 +1013,6 @@
     <xf numFmtId="9" fontId="14" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1051,6 +1054,15 @@
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3440,7 +3452,7 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1D Features</c:v>
+                  <c:v>1D Features (FFT, Envelope, Histogram)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2D Features (Spectrogram)</c:v>
@@ -3541,7 +3553,7 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1D Features</c:v>
+                  <c:v>1D Features (FFT, Envelope, Histogram)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2D Features (Spectrogram)</c:v>
@@ -3700,7 +3712,7 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1D Features</c:v>
+                  <c:v>1D Features (FFT, Envelope, Histogram)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2D Features (Spectrogram)</c:v>
@@ -3747,6 +3759,588 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2527-47E3-AC23-357F835C9BC9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1715300960"/>
+        <c:axId val="1489637024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1715300960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1489637024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1489637024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1715300960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Converging</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> to the right model for 100ms frame duration</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100ms'!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training Categorical Accuracy (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'100ms'!$A$25:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1D Features (FFT, Envelope, Histogram)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1D Features + 2.5X More Training Examples</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1D Features + 2D Features (Spectrogram, Envelope, Histogram)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1D Features + 2D Features + Higher Order Filters</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100ms'!$B$25:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.54859999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54349999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61040000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55889999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-10B6-474E-90F1-1FD689F83941}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100ms'!$C$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Validation Categorical Accuracy (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'100ms'!$A$25:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1D Features (FFT, Envelope, Histogram)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1D Features + 2.5X More Training Examples</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1D Features + 2D Features (Spectrogram, Envelope, Histogram)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1D Features + 2D Features + Higher Order Filters</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100ms'!$C$25:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.53910000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55620000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5575</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55820000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-10B6-474E-90F1-1FD689F83941}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100ms'!$D$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inference Categorical Accuracy (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="31EF99"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'100ms'!$A$25:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1D Features (FFT, Envelope, Histogram)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1D Features + 2.5X More Training Examples</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1D Features + 2D Features (Spectrogram, Envelope, Histogram)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1D Features + 2D Features + Higher Order Filters</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100ms'!$D$25:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>0.53539999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53539999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-10B6-474E-90F1-1FD689F83941}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4184,6 +4778,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6236,6 +6870,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6916,6 +8053,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBCE1E61-47C3-4611-B370-8D2537A0FB6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -11097,50 +12277,50 @@
       <c r="A1" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="91" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="96" t="s">
+      <c r="E1" s="93" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="97"/>
+      <c r="F1" s="94"/>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="91" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="92" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="96" t="s">
+      <c r="E2" s="93" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="90" t="s">
+      <c r="F2" s="94"/>
+      <c r="G2" s="104" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="90" t="s">
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="104" t="s">
         <v>144</v>
       </c>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="85">
@@ -11178,7 +12358,7 @@
         <f t="shared" si="0"/>
         <v>5.4004320345627651E-3</v>
       </c>
-      <c r="K3" s="92"/>
+      <c r="K3" s="106"/>
       <c r="L3" s="86">
         <v>0.92954060474292388</v>
       </c>
@@ -11228,7 +12408,7 @@
         <f t="shared" si="0"/>
         <v>7.7427349402406365E-2</v>
       </c>
-      <c r="K4" s="92"/>
+      <c r="K4" s="106"/>
       <c r="L4" s="89">
         <v>0.10252684265762493</v>
       </c>
@@ -11275,7 +12455,7 @@
         <f t="shared" si="0"/>
         <v>0.29069627610534332</v>
       </c>
-      <c r="K5" s="92"/>
+      <c r="K5" s="106"/>
       <c r="L5" s="86">
         <v>6.608543333731438E-3</v>
       </c>
@@ -11322,7 +12502,7 @@
         <f t="shared" si="0"/>
         <v>0.52943525840722105</v>
       </c>
-      <c r="K6" s="92"/>
+      <c r="K6" s="106"/>
       <c r="L6" s="86">
         <v>6.7273446774831819E-4</v>
       </c>
@@ -11337,19 +12517,19 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G7" s="91" t="s">
+      <c r="G7" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="91" t="s">
+      <c r="H7" s="105"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="105" t="s">
         <v>145</v>
       </c>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
-      <c r="O7" s="91"/>
+      <c r="M7" s="105"/>
+      <c r="N7" s="105"/>
+      <c r="O7" s="105"/>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="85">
@@ -11387,7 +12567,7 @@
         <f t="shared" ref="J8:J11" si="5">E8/$F8</f>
         <v>1.8925666425062414E-3</v>
       </c>
-      <c r="K8" s="92"/>
+      <c r="K8" s="106"/>
       <c r="L8" s="86">
         <v>0.86464790971228744</v>
       </c>
@@ -11437,7 +12617,7 @@
         <f t="shared" si="5"/>
         <v>2.1595014092334563E-2</v>
       </c>
-      <c r="K9" s="92"/>
+      <c r="K9" s="106"/>
       <c r="L9" s="86">
         <v>2.606578317100431E-2</v>
       </c>
@@ -11484,7 +12664,7 @@
         <f t="shared" si="5"/>
         <v>0.24819653735171529</v>
       </c>
-      <c r="K10" s="92"/>
+      <c r="K10" s="106"/>
       <c r="L10" s="86">
         <v>2.390152571405808E-4</v>
       </c>
@@ -11531,7 +12711,7 @@
         <f t="shared" si="5"/>
         <v>0.59233505175238776</v>
       </c>
-      <c r="K11" s="92"/>
+      <c r="K11" s="106"/>
       <c r="L11" s="86">
         <v>4.0516996880191239E-5</v>
       </c>
@@ -11710,19 +12890,19 @@
         <v>25164</v>
       </c>
       <c r="G18" s="86">
-        <f>B18/$F18</f>
+        <f t="shared" ref="G18:J21" si="13">B18/$F18</f>
         <v>0.86464790971228744</v>
       </c>
       <c r="H18" s="89">
-        <f>C18/$F18</f>
+        <f t="shared" si="13"/>
         <v>0.13241138133841995</v>
       </c>
       <c r="I18" s="86">
-        <f>D18/$F18</f>
+        <f t="shared" si="13"/>
         <v>2.1061834366555396E-3</v>
       </c>
       <c r="J18" s="86">
-        <f>E18/$F18</f>
+        <f t="shared" si="13"/>
         <v>8.3452551263710065E-4</v>
       </c>
     </row>
@@ -11743,23 +12923,23 @@
         <v>127</v>
       </c>
       <c r="F19" s="84">
-        <f t="shared" ref="F19:F21" si="13">SUM(B19:E19)</f>
+        <f t="shared" ref="F19:F21" si="14">SUM(B19:E19)</f>
         <v>25052</v>
       </c>
       <c r="G19" s="86">
-        <f>B19/$F19</f>
+        <f t="shared" si="13"/>
         <v>2.606578317100431E-2</v>
       </c>
       <c r="H19" s="89">
-        <f>C19/$F19</f>
+        <f t="shared" si="13"/>
         <v>0.78245249880249079</v>
       </c>
       <c r="I19" s="87">
-        <f>D19/$F19</f>
+        <f t="shared" si="13"/>
         <v>0.18641226249401247</v>
       </c>
       <c r="J19" s="86">
-        <f>E19/$F19</f>
+        <f t="shared" si="13"/>
         <v>5.0694555324924161E-3</v>
       </c>
     </row>
@@ -11777,23 +12957,23 @@
         <v>7206</v>
       </c>
       <c r="F20" s="84">
+        <f t="shared" si="14"/>
+        <v>25103</v>
+      </c>
+      <c r="G20" s="86">
         <f t="shared" si="13"/>
-        <v>25103</v>
-      </c>
-      <c r="G20" s="86">
-        <f>B20/$F20</f>
         <v>2.390152571405808E-4</v>
       </c>
       <c r="H20" s="89">
-        <f>C20/$F20</f>
+        <f t="shared" si="13"/>
         <v>0.11341273951320559</v>
       </c>
       <c r="I20" s="89">
-        <f>D20/$F20</f>
+        <f t="shared" si="13"/>
         <v>0.59929092140381623</v>
       </c>
       <c r="J20" s="87">
-        <f>E20/$F20</f>
+        <f t="shared" si="13"/>
         <v>0.28705732382583754</v>
       </c>
     </row>
@@ -11811,23 +12991,23 @@
         <v>20934</v>
       </c>
       <c r="F21" s="84">
+        <f t="shared" si="14"/>
+        <v>24681</v>
+      </c>
+      <c r="G21" s="86">
         <f t="shared" si="13"/>
-        <v>24681</v>
-      </c>
-      <c r="G21" s="86">
-        <f>B21/$F21</f>
         <v>4.0516996880191239E-5</v>
       </c>
       <c r="H21" s="86">
-        <f>C21/$F21</f>
+        <f t="shared" si="13"/>
         <v>3.9301486973785504E-3</v>
       </c>
       <c r="I21" s="89">
-        <f>D21/$F21</f>
+        <f t="shared" si="13"/>
         <v>0.14784652161581782</v>
       </c>
       <c r="J21" s="86">
-        <f>E21/$F21</f>
+        <f t="shared" si="13"/>
         <v>0.84818281268992346</v>
       </c>
     </row>
@@ -12046,13 +13226,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
-    </sheetView>
+    <sheetView topLeftCell="A34" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.77734375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="49.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="25.77734375" style="2" customWidth="1"/>
     <col min="10" max="11" width="25.77734375" style="7" customWidth="1"/>
     <col min="12" max="12" width="25.77734375" style="2" customWidth="1"/>
@@ -12060,7 +13238,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -12098,7 +13276,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="96" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="38" t="s">
@@ -12136,7 +13314,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="97" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="30">
@@ -12174,7 +13352,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="97" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="30" t="s">
@@ -12212,7 +13390,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="97" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="30">
@@ -12250,7 +13428,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="97" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="30">
@@ -12288,7 +13466,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="97" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="30">
@@ -12333,7 +13511,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="100" t="s">
+      <c r="A8" s="97" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="30">
@@ -12371,7 +13549,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="97" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="30"/>
@@ -12387,7 +13565,7 @@
       <c r="L9" s="30"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="100" t="s">
+      <c r="A10" s="97" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="30"/>
@@ -12403,7 +13581,7 @@
       <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12" ht="139.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="97" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="30" t="s">
@@ -12441,7 +13619,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="97" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="30">
@@ -12476,7 +13654,7 @@
       <c r="L12" s="57"/>
     </row>
     <row r="13" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="97" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="53">
@@ -12525,7 +13703,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="97" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="30" t="s">
@@ -12563,7 +13741,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="97" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="30">
@@ -12601,7 +13779,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="97" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="30" t="s">
@@ -12639,7 +13817,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="97" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="30">
@@ -12677,7 +13855,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="101" t="s">
+      <c r="A18" s="98" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="52">
@@ -12715,7 +13893,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="98" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="52">
@@ -12753,7 +13931,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="100" t="s">
+      <c r="A20" s="97" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="30" t="s">
@@ -12775,7 +13953,7 @@
       <c r="L20" s="48"/>
     </row>
     <row r="21" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="101" t="s">
+      <c r="A21" s="98" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="49"/>
@@ -12796,7 +13974,7 @@
       <c r="L21" s="49"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="100" t="s">
+      <c r="A22" s="97" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="30"/>
@@ -12816,7 +13994,7 @@
       <c r="L22" s="30"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="100" t="s">
+      <c r="A23" s="97" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="30"/>
@@ -12832,7 +14010,7 @@
       <c r="L23" s="30"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="100" t="s">
+      <c r="A24" s="97" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="30"/>
@@ -12868,7 +14046,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="101" t="s">
+      <c r="A25" s="98" t="s">
         <v>97</v>
       </c>
       <c r="B25" s="49"/>
@@ -12886,13 +14064,13 @@
       <c r="L25" s="49"/>
     </row>
     <row r="26" spans="1:12" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.3">
-      <c r="A26" s="102" t="s">
+      <c r="A26" s="99" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="105" t="s">
+      <c r="C26" s="102" t="s">
         <v>150</v>
       </c>
       <c r="D26" s="59" t="s">
@@ -12924,7 +14102,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="100"/>
+      <c r="A28" s="97"/>
       <c r="B28" s="30" t="s">
         <v>126</v>
       </c>
@@ -12936,141 +14114,141 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="100" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="103">
+      <c r="A29" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="100">
         <f>G18</f>
         <v>0.7621</v>
       </c>
-      <c r="C29" s="103">
+      <c r="C29" s="100">
         <f>G19</f>
         <v>0.67979999999999996</v>
       </c>
       <c r="D29" s="30"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="100" t="str">
+      <c r="A30" s="97" t="str">
         <f>B26</f>
         <v>2D Features (Spectrogram)</v>
       </c>
-      <c r="B30" s="103">
+      <c r="B30" s="100">
         <f>B18</f>
         <v>0.753</v>
       </c>
-      <c r="C30" s="103">
+      <c r="C30" s="100">
         <f>B19</f>
         <v>0.67549999999999999</v>
       </c>
       <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="100" t="str">
+      <c r="A31" s="97" t="str">
         <f>C26</f>
         <v>2D Features + Aggressive Regularization</v>
       </c>
-      <c r="B31" s="103">
+      <c r="B31" s="100">
         <f>C18</f>
         <v>0.72430000000000005</v>
       </c>
-      <c r="C31" s="103">
+      <c r="C31" s="100">
         <f>C19</f>
         <v>0.70209999999999995</v>
       </c>
       <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="100" t="str">
+      <c r="A32" s="97" t="str">
         <f>D26</f>
         <v>2D Features + 50% More Training Examples</v>
       </c>
-      <c r="B32" s="103">
+      <c r="B32" s="100">
         <f>D18</f>
         <v>0.7218</v>
       </c>
-      <c r="C32" s="103">
+      <c r="C32" s="100">
         <f>D19</f>
         <v>0.72289999999999999</v>
       </c>
       <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="104" t="str">
+      <c r="A33" s="101" t="str">
         <f>E26</f>
         <v>2D Features + Higher Order Filters</v>
       </c>
-      <c r="B33" s="103">
+      <c r="B33" s="100">
         <f>E18</f>
         <v>0.69969999999999999</v>
       </c>
-      <c r="C33" s="103">
+      <c r="C33" s="100">
         <f>E19</f>
         <v>0.71699999999999997</v>
       </c>
       <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="100" t="str">
+      <c r="A34" s="97" t="str">
         <f>F26</f>
         <v>2D Features + Extra Convolutional Layer</v>
       </c>
-      <c r="B34" s="103">
+      <c r="B34" s="100">
         <f>F18</f>
         <v>0.72070000000000001</v>
       </c>
-      <c r="C34" s="103">
+      <c r="C34" s="100">
         <f>F19</f>
         <v>0.71289999999999998</v>
       </c>
       <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="100" t="str">
+      <c r="A35" s="97" t="str">
         <f>I26</f>
         <v>1D + 2D Features (Spectrogram, Envelope, Hist.)</v>
       </c>
-      <c r="B35" s="103">
+      <c r="B35" s="100">
         <f>I18</f>
         <v>0.77070000000000005</v>
       </c>
-      <c r="C35" s="103">
+      <c r="C35" s="100">
         <f>I19</f>
         <v>0.71050000000000002</v>
       </c>
       <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="100" t="str">
+      <c r="A36" s="97" t="str">
         <f>J26</f>
         <v>1D + 2D Features, Lower Learning Rate</v>
       </c>
-      <c r="B36" s="103">
+      <c r="B36" s="100">
         <f>J18</f>
         <v>0.75470000000000004</v>
       </c>
-      <c r="C36" s="103">
+      <c r="C36" s="100">
         <f>J19</f>
         <v>0.73480000000000001</v>
       </c>
-      <c r="D36" s="103">
+      <c r="D36" s="100">
         <f>J21</f>
         <v>0.70509999999999995</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="100" t="str">
+      <c r="A37" s="97" t="str">
         <f>K26</f>
         <v>MFCC Replaced Spectrogram</v>
       </c>
-      <c r="B37" s="103">
+      <c r="B37" s="100">
         <f>K18</f>
         <v>0.79020000000000001</v>
       </c>
-      <c r="C37" s="103">
+      <c r="C37" s="100">
         <f>K19</f>
         <v>0.74980000000000002</v>
       </c>
-      <c r="D37" s="106">
+      <c r="D37" s="103">
         <f>K21</f>
         <v>0.69498631436402913</v>
       </c>
@@ -13833,13 +15011,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE1B5DB-A7CE-4976-BA44-166DD16E4014}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="25.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" style="25" customWidth="1"/>
     <col min="5" max="7" width="25.77734375" style="5" customWidth="1"/>
@@ -14373,9 +15551,101 @@
         <v>39989540</v>
       </c>
     </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="25">
+        <v>2</v>
+      </c>
+      <c r="H22" s="7">
+        <v>3</v>
+      </c>
+      <c r="I22" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="44"/>
+      <c r="B24" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="100">
+        <f>B13</f>
+        <v>0.54859999999999998</v>
+      </c>
+      <c r="C25" s="100">
+        <f>B14</f>
+        <v>0.53910000000000002</v>
+      </c>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="100">
+        <f>D13</f>
+        <v>0.54349999999999998</v>
+      </c>
+      <c r="C26" s="100">
+        <f>D14</f>
+        <v>0.55620000000000003</v>
+      </c>
+      <c r="D26" s="51">
+        <f>D16</f>
+        <v>0.53539999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="100">
+        <f>H13</f>
+        <v>0.61040000000000005</v>
+      </c>
+      <c r="C27" s="100">
+        <f>H14</f>
+        <v>0.5575</v>
+      </c>
+      <c r="D27" s="51">
+        <f>H16</f>
+        <v>0.53129999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28" s="100">
+        <f>I13</f>
+        <v>0.55889999999999995</v>
+      </c>
+      <c r="C28" s="100">
+        <f>I14</f>
+        <v>0.55820000000000003</v>
+      </c>
+      <c r="D28" s="51">
+        <f>I16</f>
+        <v>0.53539999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added scripts for reruning perception experiment.
</commit_message>
<xml_diff>
--- a/model_building/summary_speaker_counting.xlsx
+++ b/model_building/summary_speaker_counting.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56C4AB4-8F51-49C1-B5DC-CDB2AD91B9AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D6F742-6A21-4EED-ADE5-646B550331F2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="775" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="162">
   <si>
     <t>Metric</t>
   </si>
@@ -401,12 +401,6 @@
     <t>ID13</t>
   </si>
   <si>
-    <t>MAE (%)</t>
-  </si>
-  <si>
-    <t>Inference Categorical Accuracy (%)</t>
-  </si>
-  <si>
     <t>Validation Categorical Accuracy (%)</t>
   </si>
   <si>
@@ -470,30 +464,6 @@
     <t>1000 ms</t>
   </si>
   <si>
-    <t>2D Features (Spectrogram)</t>
-  </si>
-  <si>
-    <t>1D + 2D Features (Spectrogram, Envelope, Hist.)</t>
-  </si>
-  <si>
-    <t>1D + 2D Features, Lower Learning Rate</t>
-  </si>
-  <si>
-    <t>MFCC Replaced Spectrogram</t>
-  </si>
-  <si>
-    <t>2D Features + Aggressive Regularization</t>
-  </si>
-  <si>
-    <t>2D Features + 50% More Training Examples</t>
-  </si>
-  <si>
-    <t>2D Features + Higher Order Filters</t>
-  </si>
-  <si>
-    <t>2D Features + Extra Convolutional Layer</t>
-  </si>
-  <si>
     <t>1D Features (FFT, Envelope, Histogram)</t>
   </si>
   <si>
@@ -505,6 +475,48 @@
   <si>
     <t>1D Features + 2D Features + Higher Order Filters</t>
   </si>
+  <si>
+    <t>FFT, Envelope, Histogram</t>
+  </si>
+  <si>
+    <t>Spectrogram</t>
+  </si>
+  <si>
+    <t>+Aggressive Regularization</t>
+  </si>
+  <si>
+    <t>+50% More Training Examples</t>
+  </si>
+  <si>
+    <t>+Higher Order Filters</t>
+  </si>
+  <si>
+    <t>+Extra Convolutional Layer</t>
+  </si>
+  <si>
+    <t>+Envelope and Histogram</t>
+  </si>
+  <si>
+    <t>Lower Learning Rate</t>
+  </si>
+  <si>
+    <t>+MFCC -Spectrogram</t>
+  </si>
+  <si>
+    <t>Training Error (%)</t>
+  </si>
+  <si>
+    <t>Validation Error (%)</t>
+  </si>
+  <si>
+    <t>Inference Error (%)</t>
+  </si>
+  <si>
+    <t>Error (%)</t>
+  </si>
+  <si>
+    <t>Categorical Accuracy (%)</t>
+  </si>
 </sst>
 </file>
 
@@ -513,7 +525,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +624,19 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -744,7 +769,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1055,13 +1080,28 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="16" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="16" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1103,62 +1143,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Inference categorical accuracy and MAE as function of frame duration</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1173,7 +1158,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inference Categorical Accuracy (%)</c:v>
+                  <c:v>Inference Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1242,28 +1227,28 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.44829999999999998</c:v>
+                  <c:v>0.55170000000000008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47960000000000003</c:v>
+                  <c:v>0.52039999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53539999999999999</c:v>
+                  <c:v>0.46460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59389999999999998</c:v>
+                  <c:v>0.40610000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63865926423613417</c:v>
+                  <c:v>0.36134073576386583</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66514904109764728</c:v>
+                  <c:v>0.33485095890235272</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70509999999999995</c:v>
+                  <c:v>0.29490000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.77364353565212951</c:v>
+                  <c:v>0.22635646434787049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1280,11 +1265,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$F$1</c:f>
+              <c:f>Summary!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MAE (%)</c:v>
+                  <c:v>Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1349,7 +1334,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$F$2:$F$9</c:f>
+              <c:f>Summary!$I$2:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1442,7 +1427,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1455,7 +1440,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
                   <a:t>Frame duration (ms)</a:t>
                 </a:r>
               </a:p>
@@ -1474,7 +1459,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1512,7 +1497,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1574,7 +1559,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1616,7 +1601,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1693,62 +1678,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Overlap detection F-Score as function of frame duration</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1759,7 +1689,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$I$1</c:f>
+              <c:f>Summary!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1769,9 +1699,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1779,12 +1709,12 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="25400">
                 <a:solidFill>
                   <a:srgbClr val="0070C0"/>
                 </a:solidFill>
@@ -1827,7 +1757,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$I$2:$I$9</c:f>
+              <c:f>Summary!$L$2:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1920,7 +1850,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1933,7 +1863,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
                   <a:t>Frame duration (ms)</a:t>
                 </a:r>
               </a:p>
@@ -1952,7 +1882,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1990,7 +1920,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2013,6 +1943,7 @@
         <c:axId val="1644280080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2052,7 +1983,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2140,67 +2071,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Categorical accuracy:</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> training, validation, inference</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -2215,7 +2086,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Training Categorical Accuracy (%)</c:v>
+                  <c:v>Training Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2284,28 +2155,28 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.47189999999999999</c:v>
+                  <c:v>0.52810000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51390000000000002</c:v>
+                  <c:v>0.48609999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55889999999999995</c:v>
+                  <c:v>0.44110000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63029999999999997</c:v>
+                  <c:v>0.36970000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.68289999999999995</c:v>
+                  <c:v>0.31710000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.70740000000000003</c:v>
+                  <c:v>0.29259999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75470000000000004</c:v>
+                  <c:v>0.24529999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.79669999999999996</c:v>
+                  <c:v>0.20330000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2326,7 +2197,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Validation Categorical Accuracy (%)</c:v>
+                  <c:v>Validation Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2396,28 +2267,28 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.4718</c:v>
+                  <c:v>0.5282</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.50249999999999995</c:v>
+                  <c:v>0.49750000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55820000000000003</c:v>
+                  <c:v>0.44179999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.61629999999999996</c:v>
+                  <c:v>0.38370000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6583</c:v>
+                  <c:v>0.3417</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.69110000000000005</c:v>
+                  <c:v>0.30889999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73480000000000001</c:v>
+                  <c:v>0.26519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.81159999999999999</c:v>
+                  <c:v>0.18840000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2438,7 +2309,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inference Categorical Accuracy (%)</c:v>
+                  <c:v>Inference Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2508,28 +2379,28 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.44829999999999998</c:v>
+                  <c:v>0.55170000000000008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47960000000000003</c:v>
+                  <c:v>0.52039999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53539999999999999</c:v>
+                  <c:v>0.46460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59389999999999998</c:v>
+                  <c:v>0.40610000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63865926423613417</c:v>
+                  <c:v>0.36134073576386583</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66514904109764728</c:v>
+                  <c:v>0.33485095890235272</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70509999999999995</c:v>
+                  <c:v>0.29490000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.77364353565212951</c:v>
+                  <c:v>0.22635646434787049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2596,7 +2467,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2609,7 +2480,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
                   <a:t>Frame duration (ms)</a:t>
                 </a:r>
               </a:p>
@@ -2628,7 +2499,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2666,7 +2537,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2689,7 +2560,6 @@
         <c:axId val="1644280080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2707,7 +2577,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
+                  <a:t>Error Rate (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2729,7 +2654,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2771,7 +2696,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2915,7 +2840,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$Q$1</c:f>
+              <c:f>Summary!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3027,7 +2952,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$Q$2:$Q$9</c:f>
+              <c:f>Summary!$T$2:$T$9</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3355,67 +3280,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Converging</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> to the right model for 500ms frame duration</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3431,7 +3296,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Training Categorical Accuracy (%)</c:v>
+                  <c:v>Training Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3452,31 +3317,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1D Features (FFT, Envelope, Histogram)</c:v>
+                  <c:v>FFT, Envelope, Histogram</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2D Features (Spectrogram)</c:v>
+                  <c:v>Spectrogram</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2D Features + Aggressive Regularization</c:v>
+                  <c:v>+Aggressive Regularization</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2D Features + 50% More Training Examples</c:v>
+                  <c:v>+50% More Training Examples</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2D Features + Higher Order Filters</c:v>
+                  <c:v>+Higher Order Filters</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2D Features + Extra Convolutional Layer</c:v>
+                  <c:v>+Extra Convolutional Layer</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1D + 2D Features (Spectrogram, Envelope, Hist.)</c:v>
+                  <c:v>+Envelope and Histogram</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1D + 2D Features, Lower Learning Rate</c:v>
+                  <c:v>Lower Learning Rate</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>MFCC Replaced Spectrogram</c:v>
+                  <c:v>+MFCC -Spectrogram</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3488,31 +3353,31 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.7621</c:v>
+                  <c:v>0.2379</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.753</c:v>
+                  <c:v>0.247</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.72430000000000005</c:v>
+                  <c:v>0.27569999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7218</c:v>
+                  <c:v>0.2782</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.69969999999999999</c:v>
+                  <c:v>0.30030000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.72070000000000001</c:v>
+                  <c:v>0.27929999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.77070000000000005</c:v>
+                  <c:v>0.22929999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.75470000000000004</c:v>
+                  <c:v>0.24529999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79020000000000001</c:v>
+                  <c:v>0.20979999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3532,7 +3397,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Validation Categorical Accuracy (%)</c:v>
+                  <c:v>Validation Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3553,31 +3418,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1D Features (FFT, Envelope, Histogram)</c:v>
+                  <c:v>FFT, Envelope, Histogram</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2D Features (Spectrogram)</c:v>
+                  <c:v>Spectrogram</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2D Features + Aggressive Regularization</c:v>
+                  <c:v>+Aggressive Regularization</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2D Features + 50% More Training Examples</c:v>
+                  <c:v>+50% More Training Examples</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2D Features + Higher Order Filters</c:v>
+                  <c:v>+Higher Order Filters</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2D Features + Extra Convolutional Layer</c:v>
+                  <c:v>+Extra Convolutional Layer</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1D + 2D Features (Spectrogram, Envelope, Hist.)</c:v>
+                  <c:v>+Envelope and Histogram</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1D + 2D Features, Lower Learning Rate</c:v>
+                  <c:v>Lower Learning Rate</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>MFCC Replaced Spectrogram</c:v>
+                  <c:v>+MFCC -Spectrogram</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3589,31 +3454,31 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.67979999999999996</c:v>
+                  <c:v>0.32020000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67549999999999999</c:v>
+                  <c:v>0.32450000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70209999999999995</c:v>
+                  <c:v>0.29790000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.72289999999999999</c:v>
+                  <c:v>0.27710000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.71699999999999997</c:v>
+                  <c:v>0.28300000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.71289999999999998</c:v>
+                  <c:v>0.28710000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.71050000000000002</c:v>
+                  <c:v>0.28949999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.73480000000000001</c:v>
+                  <c:v>0.26519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.74980000000000002</c:v>
+                  <c:v>0.25019999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3633,7 +3498,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inference Categorical Accuracy (%)</c:v>
+                  <c:v>Inference Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3664,7 +3529,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3712,31 +3577,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1D Features (FFT, Envelope, Histogram)</c:v>
+                  <c:v>FFT, Envelope, Histogram</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2D Features (Spectrogram)</c:v>
+                  <c:v>Spectrogram</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2D Features + Aggressive Regularization</c:v>
+                  <c:v>+Aggressive Regularization</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2D Features + 50% More Training Examples</c:v>
+                  <c:v>+50% More Training Examples</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2D Features + Higher Order Filters</c:v>
+                  <c:v>+Higher Order Filters</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2D Features + Extra Convolutional Layer</c:v>
+                  <c:v>+Extra Convolutional Layer</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1D + 2D Features (Spectrogram, Envelope, Hist.)</c:v>
+                  <c:v>+Envelope and Histogram</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1D + 2D Features, Lower Learning Rate</c:v>
+                  <c:v>Lower Learning Rate</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>MFCC Replaced Spectrogram</c:v>
+                  <c:v>+MFCC -Spectrogram</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3748,10 +3613,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="7" formatCode="0.00%">
-                  <c:v>0.70509999999999995</c:v>
+                  <c:v>0.29490000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0%">
-                  <c:v>0.69498631436402913</c:v>
+                  <c:v>0.30501368563597087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3832,7 +3697,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="1" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3858,6 +3723,8 @@
         <c:axId val="1489637024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.35000000000000003"/>
+          <c:min val="0.15000000000000002"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3875,6 +3742,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400" b="1"/>
+                  <a:t>Classification Error (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3891,7 +3813,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3933,7 +3855,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4010,67 +3932,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Converging</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> to the right model for 100ms frame duration</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -4086,7 +3948,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Training Categorical Accuracy (%)</c:v>
+                  <c:v>Training Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4128,16 +3990,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.54859999999999998</c:v>
+                  <c:v>0.45140000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54349999999999998</c:v>
+                  <c:v>0.45650000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.61040000000000005</c:v>
+                  <c:v>0.38959999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55889999999999995</c:v>
+                  <c:v>0.44110000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4157,7 +4019,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Validation Categorical Accuracy (%)</c:v>
+                  <c:v>Validation Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4199,16 +4061,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.53910000000000002</c:v>
+                  <c:v>0.46089999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55620000000000003</c:v>
+                  <c:v>0.44379999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5575</c:v>
+                  <c:v>0.4425</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55820000000000003</c:v>
+                  <c:v>0.44179999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4228,7 +4090,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Inference Categorical Accuracy (%)</c:v>
+                  <c:v>Inference Error (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4258,7 +4120,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -4327,13 +4189,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="1">
-                  <c:v>0.53539999999999999</c:v>
+                  <c:v>0.46460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53129999999999999</c:v>
+                  <c:v>0.46870000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53539999999999999</c:v>
+                  <c:v>0.46460000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4414,7 +4276,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2800" b="1" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4440,6 +4302,8 @@
         <c:axId val="1489637024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.60000000000000009"/>
+          <c:min val="0.30000000000000004"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4457,6 +4321,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400" b="1"/>
+                  <a:t>Classification Error (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4473,7 +4392,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4515,7 +4434,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -7921,8 +7840,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
@@ -8040,8 +7959,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1760220</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8081,8 +8000,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8375,610 +8294,700 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D627365-F01A-4583-8FA0-E181B91C71DE}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="M61" sqref="M61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" style="33" customWidth="1"/>
-    <col min="2" max="15" width="12.77734375" style="33" customWidth="1"/>
-    <col min="16" max="16" width="25.77734375" style="65" customWidth="1"/>
-    <col min="17" max="20" width="12.77734375" style="33" customWidth="1"/>
+    <col min="2" max="13" width="12.77734375" style="33" customWidth="1"/>
+    <col min="14" max="15" width="15.77734375" style="33" customWidth="1"/>
+    <col min="16" max="16" width="15.77734375" style="65" customWidth="1"/>
+    <col min="17" max="18" width="12.77734375" style="33" customWidth="1"/>
+    <col min="19" max="19" width="25.77734375" style="33" customWidth="1"/>
+    <col min="20" max="20" width="12.77734375" style="33" customWidth="1"/>
     <col min="21" max="16384" width="8.88671875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="57" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="57" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="D1" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>124</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>102</v>
       </c>
       <c r="F1" s="32" t="s">
         <v>123</v>
       </c>
       <c r="G1" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="P1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="Q1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="R1" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="63" t="s">
+      <c r="S1" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="81" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T1" s="81" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="34">
         <v>25</v>
       </c>
       <c r="B2" s="37">
-        <f>'25ms'!B18</f>
+        <f>1-E2</f>
+        <v>0.52810000000000001</v>
+      </c>
+      <c r="C2" s="37">
+        <f t="shared" ref="C2:D2" si="0">1-F2</f>
+        <v>0.5282</v>
+      </c>
+      <c r="D2" s="37">
+        <f t="shared" si="0"/>
+        <v>0.55170000000000008</v>
+      </c>
+      <c r="E2" s="37">
         <v>0.47189999999999999</v>
       </c>
-      <c r="C2" s="37">
-        <f>'25ms'!B19</f>
+      <c r="F2" s="37">
         <v>0.4718</v>
       </c>
-      <c r="D2" s="37">
-        <f>'25ms'!B21</f>
+      <c r="G2" s="37">
         <v>0.44829999999999998</v>
       </c>
-      <c r="E2" s="35">
-        <f t="shared" ref="E2:E8" si="0">1-D2/C2</f>
-        <v>4.9809241203899957E-2</v>
-      </c>
-      <c r="F2" s="35">
+      <c r="H2" s="35">
+        <f t="shared" ref="H2:H9" si="1">1-D2/C2</f>
+        <v>-4.4490723210905081E-2</v>
+      </c>
+      <c r="I2" s="35">
         <f>'confusion matrices'!T75</f>
         <v>0.74426999999999999</v>
       </c>
-      <c r="G2" s="36">
+      <c r="J2" s="36">
         <f>'confusion matrices'!N80</f>
         <v>0.71063267837848654</v>
       </c>
-      <c r="H2" s="36">
+      <c r="K2" s="36">
         <f>'confusion matrices'!N81</f>
         <v>0.56521739130434778</v>
       </c>
-      <c r="I2" s="36">
+      <c r="L2" s="36">
         <f>'confusion matrices'!O80</f>
         <v>0.62963816547591611</v>
       </c>
-      <c r="J2" s="34">
+      <c r="M2" s="34">
         <v>10</v>
       </c>
-      <c r="K2" s="34">
+      <c r="N2" s="34">
         <f>'25ms'!B26</f>
         <v>15954084</v>
       </c>
-      <c r="L2" s="34">
+      <c r="O2" s="34">
         <f>'25ms'!B6</f>
         <v>1000000</v>
       </c>
-      <c r="M2" s="34">
-        <f t="shared" ref="M2:M9" si="1">0.04*L2</f>
+      <c r="P2" s="34">
+        <f t="shared" ref="P2:P9" si="2">0.04*O2</f>
         <v>40000</v>
       </c>
-      <c r="N2" s="34">
+      <c r="Q2" s="34">
         <v>100000</v>
       </c>
-      <c r="O2" s="34">
+      <c r="R2" s="34">
         <f>'25ms'!B25</f>
         <v>278</v>
       </c>
-      <c r="P2" s="64" t="s">
+      <c r="S2" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="Q2" s="76">
-        <f>K2/O2</f>
+      <c r="T2" s="76">
+        <f>N2/R2</f>
         <v>57388.791366906473</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="34">
         <v>50</v>
       </c>
       <c r="B3" s="37">
-        <f>'50ms'!C18</f>
+        <f t="shared" ref="B3:B9" si="3">1-E3</f>
+        <v>0.48609999999999998</v>
+      </c>
+      <c r="C3" s="37">
+        <f t="shared" ref="C3:C9" si="4">1-F3</f>
+        <v>0.49750000000000005</v>
+      </c>
+      <c r="D3" s="37">
+        <f t="shared" ref="D3:D9" si="5">1-G3</f>
+        <v>0.52039999999999997</v>
+      </c>
+      <c r="E3" s="37">
         <v>0.51390000000000002</v>
       </c>
-      <c r="C3" s="37">
-        <f>'50ms'!C19</f>
+      <c r="F3" s="37">
         <v>0.50249999999999995</v>
       </c>
-      <c r="D3" s="37">
-        <f>'50ms'!C21</f>
+      <c r="G3" s="37">
         <v>0.47960000000000003</v>
       </c>
-      <c r="E3" s="35">
-        <f t="shared" si="0"/>
-        <v>4.5572139303482473E-2</v>
-      </c>
-      <c r="F3" s="35">
+      <c r="H3" s="35">
+        <f t="shared" si="1"/>
+        <v>-4.6030150753768595E-2</v>
+      </c>
+      <c r="I3" s="35">
         <f>'confusion matrices'!T91</f>
         <v>0.66876999999999998</v>
       </c>
-      <c r="G3" s="36">
+      <c r="J3" s="36">
         <f>'confusion matrices'!N96</f>
         <v>0.84574723690533393</v>
       </c>
-      <c r="H3" s="36">
+      <c r="K3" s="36">
         <f>'confusion matrices'!N97</f>
         <v>0.57889976153276868</v>
       </c>
-      <c r="I3" s="36">
+      <c r="L3" s="36">
         <f>'confusion matrices'!O96</f>
         <v>0.68733219428850378</v>
       </c>
-      <c r="J3" s="76">
+      <c r="M3" s="76">
         <v>12</v>
       </c>
-      <c r="K3" s="34">
+      <c r="N3" s="34">
         <f>'50ms'!C25</f>
         <v>35504292</v>
       </c>
-      <c r="L3" s="34">
+      <c r="O3" s="34">
         <f>'50ms'!C6</f>
         <v>600000</v>
       </c>
-      <c r="M3" s="34">
-        <f t="shared" si="1"/>
+      <c r="P3" s="34">
+        <f t="shared" si="2"/>
         <v>24000</v>
       </c>
-      <c r="N3" s="34">
+      <c r="Q3" s="34">
         <v>100000</v>
       </c>
-      <c r="O3" s="34">
+      <c r="R3" s="34">
         <f>'50ms'!C8</f>
         <v>582</v>
       </c>
-      <c r="P3" s="64" t="s">
+      <c r="S3" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="Q3" s="76">
-        <f t="shared" ref="Q3:Q13" si="2">K3/O3</f>
+      <c r="T3" s="76">
+        <f t="shared" ref="T3:T13" si="6">N3/R3</f>
         <v>61003.938144329899</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="34">
         <v>100</v>
       </c>
       <c r="B4" s="37">
-        <f>'100ms'!I13</f>
+        <f t="shared" si="3"/>
+        <v>0.44110000000000005</v>
+      </c>
+      <c r="C4" s="37">
+        <f t="shared" si="4"/>
+        <v>0.44179999999999997</v>
+      </c>
+      <c r="D4" s="37">
+        <f t="shared" si="5"/>
+        <v>0.46460000000000001</v>
+      </c>
+      <c r="E4" s="37">
         <v>0.55889999999999995</v>
       </c>
-      <c r="C4" s="37">
-        <f>'100ms'!I14</f>
+      <c r="F4" s="37">
         <v>0.55820000000000003</v>
       </c>
-      <c r="D4" s="37">
-        <f>'100ms'!I16</f>
+      <c r="G4" s="37">
         <v>0.53539999999999999</v>
       </c>
-      <c r="E4" s="35">
-        <f t="shared" si="0"/>
-        <v>4.0845575062701589E-2</v>
-      </c>
-      <c r="F4" s="35">
+      <c r="H4" s="35">
+        <f t="shared" si="1"/>
+        <v>-5.1607062019013217E-2</v>
+      </c>
+      <c r="I4" s="35">
         <f>'confusion matrices'!T19</f>
         <v>0.56186999999999998</v>
       </c>
-      <c r="G4" s="36">
+      <c r="J4" s="36">
         <f>'confusion matrices'!N24</f>
         <v>0.87018961516921356</v>
       </c>
-      <c r="H4" s="36">
+      <c r="K4" s="36">
         <f>'confusion matrices'!N25</f>
         <v>0.67509775929489169</v>
       </c>
-      <c r="I4" s="36">
+      <c r="L4" s="36">
         <f>'confusion matrices'!O24</f>
         <v>0.76032855644879416</v>
       </c>
-      <c r="J4" s="34">
+      <c r="M4" s="34">
         <v>3</v>
       </c>
-      <c r="K4" s="34">
+      <c r="N4" s="34">
         <f>'100ms'!I21</f>
         <v>39989540</v>
       </c>
-      <c r="L4" s="34">
+      <c r="O4" s="34">
         <v>600000</v>
       </c>
-      <c r="M4" s="34">
-        <f t="shared" si="1"/>
+      <c r="P4" s="34">
+        <f t="shared" si="2"/>
         <v>24000</v>
       </c>
-      <c r="N4" s="34">
+      <c r="Q4" s="34">
         <v>100000</v>
       </c>
-      <c r="O4" s="34">
+      <c r="R4" s="34">
         <v>1267</v>
       </c>
-      <c r="P4" s="64" t="s">
+      <c r="S4" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="Q4" s="76">
-        <f t="shared" si="2"/>
+      <c r="T4" s="76">
+        <f t="shared" si="6"/>
         <v>31562.383583267561</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="34">
         <v>200</v>
       </c>
       <c r="B5" s="37">
-        <f>'200ms'!B18</f>
+        <f t="shared" si="3"/>
+        <v>0.36970000000000003</v>
+      </c>
+      <c r="C5" s="37">
+        <f t="shared" si="4"/>
+        <v>0.38370000000000004</v>
+      </c>
+      <c r="D5" s="37">
+        <f t="shared" si="5"/>
+        <v>0.40610000000000002</v>
+      </c>
+      <c r="E5" s="37">
         <v>0.63029999999999997</v>
       </c>
-      <c r="C5" s="37">
-        <f>'200ms'!B19</f>
+      <c r="F5" s="37">
         <v>0.61629999999999996</v>
       </c>
-      <c r="D5" s="37">
+      <c r="G5" s="37">
         <v>0.59389999999999998</v>
       </c>
-      <c r="E5" s="35">
-        <f t="shared" si="0"/>
-        <v>3.6345935421061126E-2</v>
-      </c>
-      <c r="F5" s="35">
+      <c r="H5" s="35">
+        <f t="shared" si="1"/>
+        <v>-5.8378941881678248E-2</v>
+      </c>
+      <c r="I5" s="35">
         <f>'confusion matrices'!T43</f>
         <v>0.46977999999999998</v>
       </c>
-      <c r="G5" s="36">
+      <c r="J5" s="36">
         <f>'confusion matrices'!N48</f>
         <v>0.89714080917489647</v>
       </c>
-      <c r="H5" s="36">
+      <c r="K5" s="36">
         <f>'confusion matrices'!N49</f>
         <v>0.76294490162213413</v>
       </c>
-      <c r="I5" s="36">
+      <c r="L5" s="36">
         <f>'confusion matrices'!O48</f>
         <v>0.82461887593565264</v>
       </c>
-      <c r="J5" s="34">
+      <c r="M5" s="34">
         <v>6</v>
       </c>
-      <c r="K5" s="34">
+      <c r="N5" s="34">
         <v>88888996</v>
       </c>
-      <c r="L5" s="34">
+      <c r="O5" s="34">
         <v>600000</v>
       </c>
-      <c r="M5" s="34">
-        <f t="shared" si="1"/>
+      <c r="P5" s="34">
+        <f t="shared" si="2"/>
         <v>24000</v>
       </c>
-      <c r="N5" s="34">
+      <c r="Q5" s="34">
         <v>100000</v>
       </c>
-      <c r="O5" s="34">
+      <c r="R5" s="34">
         <v>2787</v>
       </c>
-      <c r="P5" s="64" t="s">
+      <c r="S5" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="Q5" s="76">
-        <f t="shared" si="2"/>
+      <c r="T5" s="76">
+        <f t="shared" si="6"/>
         <v>31894.149982059564</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="34">
         <v>300</v>
       </c>
       <c r="B6" s="37">
-        <f>'300ms'!C18</f>
+        <f t="shared" si="3"/>
+        <v>0.31710000000000005</v>
+      </c>
+      <c r="C6" s="37">
+        <f t="shared" si="4"/>
+        <v>0.3417</v>
+      </c>
+      <c r="D6" s="37">
+        <f t="shared" si="5"/>
+        <v>0.36134073576386583</v>
+      </c>
+      <c r="E6" s="37">
         <v>0.68289999999999995</v>
       </c>
-      <c r="C6" s="37">
-        <f>'300ms'!C19</f>
+      <c r="F6" s="37">
         <v>0.6583</v>
       </c>
-      <c r="D6" s="37">
-        <f>'confusion matrices'!O83</f>
+      <c r="G6" s="37">
         <v>0.63865926423613417</v>
       </c>
-      <c r="E6" s="35">
-        <f t="shared" si="0"/>
-        <v>2.9835539668640165E-2</v>
-      </c>
-      <c r="F6" s="35">
+      <c r="H6" s="35">
+        <f t="shared" si="1"/>
+        <v>-5.7479472531067666E-2</v>
+      </c>
+      <c r="I6" s="35">
         <f>'confusion matrices'!T83</f>
         <v>0.39834000000000003</v>
       </c>
-      <c r="G6" s="36">
+      <c r="J6" s="36">
         <f>'confusion matrices'!N88</f>
         <v>0.93323669163243939</v>
       </c>
-      <c r="H6" s="36">
+      <c r="K6" s="36">
         <f>'confusion matrices'!N89</f>
         <v>0.80643028637043734</v>
       </c>
-      <c r="I6" s="36">
+      <c r="L6" s="36">
         <f>'confusion matrices'!O88</f>
         <v>0.86521195378268911</v>
       </c>
-      <c r="J6" s="34">
+      <c r="M6" s="34">
         <v>11</v>
       </c>
-      <c r="K6" s="34">
+      <c r="N6" s="34">
         <f>'300ms'!C25</f>
         <v>137123492</v>
       </c>
-      <c r="L6" s="34">
+      <c r="O6" s="34">
         <f>'300ms'!C6</f>
         <v>600000</v>
       </c>
-      <c r="M6" s="34">
-        <f t="shared" si="1"/>
+      <c r="P6" s="34">
+        <f t="shared" si="2"/>
         <v>24000</v>
       </c>
-      <c r="N6" s="34">
+      <c r="Q6" s="34">
         <v>100000</v>
       </c>
-      <c r="O6" s="34">
+      <c r="R6" s="34">
         <f>'300ms'!C8</f>
         <v>4258</v>
       </c>
-      <c r="P6" s="64" t="s">
+      <c r="S6" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="Q6" s="76">
-        <f t="shared" si="2"/>
+      <c r="T6" s="76">
+        <f t="shared" si="6"/>
         <v>32203.732268670738</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="34">
         <v>400</v>
       </c>
       <c r="B7" s="37">
-        <f>'400ms'!B18</f>
+        <f t="shared" si="3"/>
+        <v>0.29259999999999997</v>
+      </c>
+      <c r="C7" s="37">
+        <f t="shared" si="4"/>
+        <v>0.30889999999999995</v>
+      </c>
+      <c r="D7" s="37">
+        <f t="shared" si="5"/>
+        <v>0.33485095890235272</v>
+      </c>
+      <c r="E7" s="37">
         <v>0.70740000000000003</v>
       </c>
-      <c r="C7" s="37">
-        <f>'400ms'!B19</f>
+      <c r="F7" s="37">
         <v>0.69110000000000005</v>
       </c>
-      <c r="D7" s="37">
-        <f>'confusion matrices'!O35</f>
+      <c r="G7" s="37">
         <v>0.66514904109764728</v>
       </c>
-      <c r="E7" s="35">
-        <f t="shared" si="0"/>
-        <v>3.7550222691872026E-2</v>
-      </c>
-      <c r="F7" s="35">
+      <c r="H7" s="35">
+        <f t="shared" si="1"/>
+        <v>-8.4010873753165294E-2</v>
+      </c>
+      <c r="I7" s="35">
         <f>'confusion matrices'!T35</f>
         <v>0.36002000000000001</v>
       </c>
-      <c r="G7" s="36">
+      <c r="J7" s="36">
         <f>'confusion matrices'!N40</f>
         <v>0.92923522548980164</v>
       </c>
-      <c r="H7" s="36">
+      <c r="K7" s="36">
         <f>'confusion matrices'!N41</f>
         <v>0.84722884495470052</v>
       </c>
-      <c r="I7" s="36">
+      <c r="L7" s="36">
         <f>'confusion matrices'!O40</f>
         <v>0.88633921719109754</v>
       </c>
-      <c r="J7" s="34">
+      <c r="M7" s="34">
         <f>'confusion matrices'!I35</f>
         <v>5</v>
       </c>
-      <c r="K7" s="34">
+      <c r="N7" s="34">
         <v>185095844</v>
       </c>
-      <c r="L7" s="34">
+      <c r="O7" s="34">
         <v>600000</v>
       </c>
-      <c r="M7" s="34">
-        <f t="shared" si="1"/>
+      <c r="P7" s="34">
+        <f t="shared" si="2"/>
         <v>24000</v>
       </c>
-      <c r="N7" s="34">
+      <c r="Q7" s="34">
         <v>100000</v>
       </c>
-      <c r="O7" s="34">
+      <c r="R7" s="34">
         <v>5727</v>
       </c>
-      <c r="P7" s="64" t="s">
+      <c r="S7" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="Q7" s="76">
-        <f t="shared" si="2"/>
+      <c r="T7" s="76">
+        <f t="shared" si="6"/>
         <v>32319.861009254408</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="34">
         <v>500</v>
       </c>
       <c r="B8" s="37">
-        <f>'500ms'!J18</f>
+        <f t="shared" si="3"/>
+        <v>0.24529999999999996</v>
+      </c>
+      <c r="C8" s="37">
+        <f t="shared" si="4"/>
+        <v>0.26519999999999999</v>
+      </c>
+      <c r="D8" s="37">
+        <f t="shared" si="5"/>
+        <v>0.29490000000000005</v>
+      </c>
+      <c r="E8" s="37">
         <v>0.75470000000000004</v>
       </c>
-      <c r="C8" s="37">
-        <f>'500ms'!J19</f>
+      <c r="F8" s="37">
         <v>0.73480000000000001</v>
       </c>
-      <c r="D8" s="37">
-        <f>'500ms'!J21</f>
+      <c r="G8" s="37">
         <v>0.70509999999999995</v>
       </c>
-      <c r="E8" s="35">
-        <f t="shared" si="0"/>
-        <v>4.0419161676646831E-2</v>
-      </c>
-      <c r="F8" s="35">
+      <c r="H8" s="35">
+        <f t="shared" si="1"/>
+        <v>-0.11199095022624461</v>
+      </c>
+      <c r="I8" s="35">
         <f>'confusion matrices'!T99</f>
         <v>0.31314999999999998</v>
       </c>
-      <c r="G8" s="36">
+      <c r="J8" s="36">
         <f>'confusion matrices'!N104</f>
         <v>0.92954060474292388</v>
       </c>
-      <c r="H8" s="36">
+      <c r="K8" s="36">
         <f>'confusion matrices'!N105</f>
         <v>0.89449825648973269</v>
       </c>
-      <c r="I8" s="36">
+      <c r="L8" s="36">
         <f>'confusion matrices'!O104</f>
         <v>0.91168282425415126</v>
       </c>
-      <c r="J8" s="34">
+      <c r="M8" s="34">
         <v>13</v>
       </c>
-      <c r="K8" s="34">
+      <c r="N8" s="34">
         <f>'500ms'!J25</f>
         <v>234249636</v>
       </c>
-      <c r="L8" s="34">
+      <c r="O8" s="34">
         <f>'500ms'!J6</f>
         <v>600000</v>
       </c>
-      <c r="M8" s="34">
-        <f t="shared" si="1"/>
+      <c r="P8" s="34">
+        <f t="shared" si="2"/>
         <v>24000</v>
       </c>
-      <c r="N8" s="34">
+      <c r="Q8" s="34">
         <v>100000</v>
       </c>
-      <c r="O8" s="34">
+      <c r="R8" s="34">
         <f>'500ms'!J8</f>
         <v>7197</v>
       </c>
-      <c r="P8" s="64" t="s">
+      <c r="S8" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="Q8" s="76">
-        <f t="shared" si="2"/>
+      <c r="T8" s="76">
+        <f t="shared" si="6"/>
         <v>32548.233430596083</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="34">
         <v>1000</v>
       </c>
       <c r="B9" s="37">
-        <f>'1000ms'!B18</f>
+        <f t="shared" si="3"/>
+        <v>0.20330000000000004</v>
+      </c>
+      <c r="C9" s="37">
+        <f t="shared" si="4"/>
+        <v>0.18840000000000001</v>
+      </c>
+      <c r="D9" s="37">
+        <f t="shared" si="5"/>
+        <v>0.22635646434787049</v>
+      </c>
+      <c r="E9" s="37">
         <v>0.79669999999999996</v>
       </c>
-      <c r="C9" s="37">
-        <f>'1000ms'!B19</f>
+      <c r="F9" s="37">
         <v>0.81159999999999999</v>
       </c>
-      <c r="D9" s="37">
-        <f>'confusion matrices'!O27</f>
+      <c r="G9" s="37">
         <v>0.77364353565212951</v>
       </c>
-      <c r="E9" s="35">
-        <f>1-D9/C9</f>
-        <v>4.6767452375394925E-2</v>
-      </c>
-      <c r="F9" s="35">
+      <c r="H9" s="35">
+        <f t="shared" si="1"/>
+        <v>-0.20146743284432311</v>
+      </c>
+      <c r="I9" s="35">
         <f>'confusion matrices'!T27</f>
         <v>0.22989000000000001</v>
       </c>
-      <c r="G9" s="36">
+      <c r="J9" s="36">
         <f>'confusion matrices'!N32</f>
         <v>0.86464790971228744</v>
       </c>
-      <c r="H9" s="36">
+      <c r="K9" s="36">
         <f>'confusion matrices'!N33</f>
         <v>0.97055937193326791</v>
       </c>
-      <c r="I9" s="36">
+      <c r="L9" s="36">
         <f>'confusion matrices'!O32</f>
         <v>0.91454751796897993</v>
       </c>
-      <c r="J9" s="34">
+      <c r="M9" s="34">
         <f>'confusion matrices'!I27</f>
         <v>4</v>
       </c>
-      <c r="K9" s="34">
+      <c r="N9" s="34">
         <v>123229860</v>
       </c>
-      <c r="L9" s="34">
+      <c r="O9" s="34">
         <v>600000</v>
       </c>
-      <c r="M9" s="34">
-        <f t="shared" si="1"/>
+      <c r="P9" s="34">
+        <f t="shared" si="2"/>
         <v>24000</v>
       </c>
-      <c r="N9" s="34">
+      <c r="Q9" s="34">
         <v>100000</v>
       </c>
-      <c r="O9" s="34">
+      <c r="R9" s="34">
         <v>3837</v>
       </c>
-      <c r="P9" s="64" t="s">
+      <c r="S9" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="Q9" s="76">
-        <f t="shared" si="2"/>
+      <c r="T9" s="76">
+        <f t="shared" si="6"/>
         <v>32116.200156372164</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" s="75" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="70"/>
       <c r="B10" s="71"/>
       <c r="C10" s="71"/>
       <c r="D10" s="71"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="70"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
       <c r="M10" s="70"/>
       <c r="N10" s="70"/>
       <c r="O10" s="70"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="82"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P10" s="70"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="82"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="34">
         <v>50</v>
       </c>
@@ -8994,56 +9003,68 @@
         <f>'50ms'!B21</f>
         <v>0.46760000000000002</v>
       </c>
-      <c r="E11" s="80">
+      <c r="E11" s="35">
+        <f>'50ms'!E18</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="35">
+        <f>'50ms'!E19</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="35">
+        <f>'50ms'!E21</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="80">
         <f>1-D11/C11</f>
         <v>0.10780385422629268</v>
       </c>
-      <c r="F11" s="79">
+      <c r="I11" s="79">
         <f>'confusion matrices'!T67</f>
         <v>0.67052</v>
       </c>
-      <c r="G11" s="36">
+      <c r="J11" s="36">
         <f>'confusion matrices'!N72</f>
         <v>0.60120737216647346</v>
       </c>
-      <c r="H11" s="36">
+      <c r="K11" s="36">
         <f>'confusion matrices'!N73</f>
         <v>0.68106884057971018</v>
       </c>
-      <c r="I11" s="36">
+      <c r="L11" s="36">
         <f>'confusion matrices'!O72</f>
         <v>0.6386511795808294</v>
       </c>
-      <c r="J11" s="34">
+      <c r="M11" s="34">
         <v>9</v>
       </c>
-      <c r="K11" s="34">
+      <c r="N11" s="34">
         <f>'50ms'!B25</f>
         <v>17576228</v>
       </c>
-      <c r="L11" s="34">
+      <c r="O11" s="34">
         <f>'100ms'!I3</f>
         <v>350000</v>
       </c>
-      <c r="M11" s="34">
-        <f>0.04*L11</f>
+      <c r="P11" s="34">
+        <f>0.04*O11</f>
         <v>14000</v>
       </c>
-      <c r="N11" s="34">
+      <c r="Q11" s="34">
         <v>100000</v>
       </c>
-      <c r="O11" s="34">
+      <c r="R11" s="34">
         <v>582</v>
       </c>
-      <c r="P11" s="64" t="s">
+      <c r="S11" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="Q11" s="76">
-        <f t="shared" si="2"/>
+      <c r="T11" s="76">
+        <f t="shared" si="6"/>
         <v>30199.704467353953</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="34">
         <v>100</v>
       </c>
@@ -9060,54 +9081,66 @@
         <v>0.53539999999999999</v>
       </c>
       <c r="E12" s="35">
+        <f>'100ms'!G13</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="35">
+        <f>'100ms'!G14</f>
+        <v>0.54349999999999998</v>
+      </c>
+      <c r="G12" s="35">
+        <f>'100ms'!L16</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="35">
         <f>1-D12/C12</f>
         <v>3.7396619920891827E-2</v>
       </c>
-      <c r="F12" s="80">
+      <c r="I12" s="80">
         <f>'confusion matrices'!T3</f>
         <v>0.56755999999999995</v>
       </c>
-      <c r="G12" s="36">
+      <c r="J12" s="36">
         <f>'confusion matrices'!N8</f>
         <v>0.82097576632964209</v>
       </c>
-      <c r="H12" s="36">
+      <c r="K12" s="36">
         <f>'confusion matrices'!N9</f>
         <v>0.70558620689655172</v>
       </c>
-      <c r="I12" s="36">
+      <c r="L12" s="36">
         <f>'confusion matrices'!O8</f>
         <v>0.75891996142719376</v>
       </c>
-      <c r="J12" s="34">
+      <c r="M12" s="34">
         <f>'confusion matrices'!I3</f>
         <v>1</v>
       </c>
-      <c r="K12" s="34">
+      <c r="N12" s="34">
         <v>14032964</v>
       </c>
-      <c r="L12" s="34">
+      <c r="O12" s="34">
         <v>1000000</v>
       </c>
-      <c r="M12" s="34">
-        <f>0.04*L12</f>
+      <c r="P12" s="34">
+        <f>0.04*O12</f>
         <v>40000</v>
       </c>
-      <c r="N12" s="34">
+      <c r="Q12" s="34">
         <v>100000</v>
       </c>
-      <c r="O12" s="34">
+      <c r="R12" s="34">
         <v>451</v>
       </c>
-      <c r="P12" s="64" t="s">
+      <c r="S12" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="Q12" s="76">
-        <f t="shared" si="2"/>
+      <c r="T12" s="76">
+        <f t="shared" si="6"/>
         <v>31115.219512195123</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="34">
         <v>500</v>
       </c>
@@ -9123,50 +9156,62 @@
         <f>'500ms'!K21</f>
         <v>0.69498631436402913</v>
       </c>
-      <c r="E13" s="80">
+      <c r="E13" s="37">
+        <f>'500ms'!N18</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="37">
+        <f>'500ms'!N19</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="37">
+        <f>'500ms'!N21</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="80">
         <f>1-D13/C13</f>
         <v>7.3104408690278566E-2</v>
       </c>
-      <c r="F13" s="35">
+      <c r="I13" s="35">
         <f>'confusion matrices'!T59</f>
         <v>0.31603999999999999</v>
       </c>
-      <c r="G13" s="36">
+      <c r="J13" s="36">
         <f>'confusion matrices'!N64</f>
         <v>0.82962119980490978</v>
       </c>
-      <c r="H13" s="36">
+      <c r="K13" s="36">
         <f>'confusion matrices'!N65</f>
         <v>0.93667400881057272</v>
       </c>
-      <c r="I13" s="36">
+      <c r="L13" s="36">
         <f>'confusion matrices'!O64</f>
         <v>0.87990343995171993</v>
       </c>
-      <c r="J13" s="34">
+      <c r="M13" s="34">
         <v>8</v>
       </c>
-      <c r="K13" s="34">
+      <c r="N13" s="34">
         <v>62149028</v>
       </c>
-      <c r="L13" s="34">
+      <c r="O13" s="34">
         <v>600000</v>
       </c>
-      <c r="M13" s="34">
-        <f>0.04*L13</f>
+      <c r="P13" s="34">
+        <f>0.04*O13</f>
         <v>24000</v>
       </c>
-      <c r="N13" s="34">
+      <c r="Q13" s="34">
         <v>50000</v>
       </c>
-      <c r="O13" s="34">
+      <c r="R13" s="34">
         <v>1955</v>
       </c>
-      <c r="P13" s="64" t="s">
+      <c r="S13" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="Q13" s="76">
-        <f t="shared" si="2"/>
+      <c r="T13" s="76">
+        <f t="shared" si="6"/>
         <v>31789.784143222507</v>
       </c>
     </row>
@@ -9181,8 +9226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B3942E-9FC7-4237-A72A-436C0A2724D2}">
   <dimension ref="A1:U105"/>
   <sheetViews>
-    <sheetView topLeftCell="F73" workbookViewId="0">
-      <selection activeCell="J83" sqref="J83:M86"/>
+    <sheetView topLeftCell="F94" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12262,7 +12307,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E531359-AF06-4E17-9A1D-24EDE25633C4}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:O11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12275,52 +12322,52 @@
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="85" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" s="90" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="92" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="E1" s="93" t="s">
         <v>133</v>
-      </c>
-      <c r="D1" s="92" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="93" t="s">
-        <v>135</v>
       </c>
       <c r="F1" s="94"/>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="85" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="90" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="91" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="93" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="F2" s="94"/>
+      <c r="G2" s="109" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="91" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="92" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="93" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="94"/>
-      <c r="G2" s="104" t="s">
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="109" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="104" t="s">
-        <v>144</v>
-      </c>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="85">
@@ -12342,39 +12389,39 @@
         <f>SUM(B3:E3)</f>
         <v>24998</v>
       </c>
-      <c r="G3" s="86">
+      <c r="G3" s="105">
         <f>B3/$F3</f>
         <v>0.87018961516921356</v>
       </c>
-      <c r="H3" s="89">
+      <c r="H3" s="106">
         <f t="shared" ref="H3:J6" si="0">C3/$F3</f>
         <v>0.11408912713017041</v>
       </c>
-      <c r="I3" s="86">
+      <c r="I3" s="105">
         <f t="shared" si="0"/>
         <v>1.0320825666053284E-2</v>
       </c>
-      <c r="J3" s="86">
+      <c r="J3" s="105">
         <f t="shared" si="0"/>
         <v>5.4004320345627651E-3</v>
       </c>
-      <c r="K3" s="106"/>
-      <c r="L3" s="86">
+      <c r="K3" s="111"/>
+      <c r="L3" s="105">
         <v>0.92954060474292388</v>
       </c>
-      <c r="M3" s="89">
+      <c r="M3" s="106">
         <v>6.6513669122679878E-2</v>
       </c>
-      <c r="N3" s="86">
+      <c r="N3" s="105">
         <v>2.2144381366509644E-3</v>
       </c>
-      <c r="O3" s="86">
+      <c r="O3" s="105">
         <v>1.7312879977452993E-3</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="85" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B4" s="83">
         <v>7729</v>
@@ -12392,33 +12439,33 @@
         <f t="shared" ref="F4:F6" si="1">SUM(B4:E4)</f>
         <v>25017</v>
       </c>
-      <c r="G4" s="88">
+      <c r="G4" s="107">
         <f t="shared" ref="G4:G6" si="2">B4/$F4</f>
         <v>0.30894991405844024</v>
       </c>
-      <c r="H4" s="87">
+      <c r="H4" s="108">
         <f t="shared" si="0"/>
         <v>0.4278690490466483</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="108">
         <f t="shared" si="0"/>
         <v>0.18575368749250509</v>
       </c>
-      <c r="J4" s="89">
+      <c r="J4" s="106">
         <f t="shared" si="0"/>
         <v>7.7427349402406365E-2</v>
       </c>
-      <c r="K4" s="106"/>
-      <c r="L4" s="89">
+      <c r="K4" s="111"/>
+      <c r="L4" s="106">
         <v>0.10252684265762493</v>
       </c>
-      <c r="M4" s="89">
+      <c r="M4" s="106">
         <v>0.77020263179139425</v>
       </c>
-      <c r="N4" s="87">
+      <c r="N4" s="108">
         <v>0.12226527811415193</v>
       </c>
-      <c r="O4" s="86">
+      <c r="O4" s="105">
         <v>5.0052474368289333E-3</v>
       </c>
     </row>
@@ -12439,33 +12486,33 @@
         <f t="shared" si="1"/>
         <v>24947</v>
       </c>
-      <c r="G5" s="89">
+      <c r="G5" s="106">
         <f t="shared" si="2"/>
         <v>8.698440694271857E-2</v>
       </c>
-      <c r="H5" s="88">
+      <c r="H5" s="107">
         <f t="shared" si="0"/>
         <v>0.308133242474045</v>
       </c>
-      <c r="I5" s="88">
+      <c r="I5" s="107">
         <f t="shared" si="0"/>
         <v>0.31418607447789315</v>
       </c>
-      <c r="J5" s="87">
+      <c r="J5" s="108">
         <f t="shared" si="0"/>
         <v>0.29069627610534332</v>
       </c>
-      <c r="K5" s="106"/>
-      <c r="L5" s="86">
+      <c r="K5" s="111"/>
+      <c r="L5" s="105">
         <v>6.608543333731438E-3</v>
       </c>
-      <c r="M5" s="87">
+      <c r="M5" s="108">
         <v>0.29734463951590429</v>
       </c>
-      <c r="N5" s="87">
+      <c r="N5" s="108">
         <v>0.51896970420797006</v>
       </c>
-      <c r="O5" s="87">
+      <c r="O5" s="108">
         <v>0.1770771129423942</v>
       </c>
     </row>
@@ -12486,50 +12533,50 @@
         <f t="shared" si="1"/>
         <v>25038</v>
       </c>
-      <c r="G6" s="86">
+      <c r="G6" s="105">
         <f t="shared" si="2"/>
         <v>2.2765396597172298E-2</v>
       </c>
-      <c r="H6" s="87">
+      <c r="H6" s="108">
         <f t="shared" si="0"/>
         <v>0.15827941528876108</v>
       </c>
-      <c r="I6" s="87">
+      <c r="I6" s="108">
         <f t="shared" si="0"/>
         <v>0.28951992970684559</v>
       </c>
-      <c r="J6" s="87">
+      <c r="J6" s="108">
         <f t="shared" si="0"/>
         <v>0.52943525840722105</v>
       </c>
-      <c r="K6" s="106"/>
-      <c r="L6" s="86">
+      <c r="K6" s="111"/>
+      <c r="L6" s="105">
         <v>6.7273446774831819E-4</v>
       </c>
-      <c r="M6" s="86">
+      <c r="M6" s="105">
         <v>4.9861495844875349E-2</v>
       </c>
-      <c r="N6" s="88">
+      <c r="N6" s="107">
         <v>0.34772457459438066</v>
       </c>
-      <c r="O6" s="89">
+      <c r="O6" s="106">
         <v>0.60174119509299562</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G7" s="105" t="s">
+      <c r="G7" s="110" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="110" t="s">
         <v>143</v>
       </c>
-      <c r="H7" s="105"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="105" t="s">
-        <v>145</v>
-      </c>
-      <c r="M7" s="105"/>
-      <c r="N7" s="105"/>
-      <c r="O7" s="105"/>
+      <c r="M7" s="110"/>
+      <c r="N7" s="110"/>
+      <c r="O7" s="110"/>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="85">
@@ -12551,39 +12598,39 @@
         <f>SUM(B8:E8)</f>
         <v>24834</v>
       </c>
-      <c r="G8" s="86">
+      <c r="G8" s="105">
         <f>B8/$F8</f>
         <v>0.93323669163243939</v>
       </c>
-      <c r="H8" s="89">
+      <c r="H8" s="106">
         <f t="shared" ref="H8:H11" si="3">C8/$F8</f>
         <v>6.2615768704195857E-2</v>
       </c>
-      <c r="I8" s="86">
+      <c r="I8" s="105">
         <f t="shared" ref="I8:I11" si="4">D8/$F8</f>
         <v>2.2549730208585007E-3</v>
       </c>
-      <c r="J8" s="86">
+      <c r="J8" s="105">
         <f t="shared" ref="J8:J11" si="5">E8/$F8</f>
         <v>1.8925666425062414E-3</v>
       </c>
-      <c r="K8" s="106"/>
-      <c r="L8" s="86">
+      <c r="K8" s="111"/>
+      <c r="L8" s="105">
         <v>0.86464790971228744</v>
       </c>
-      <c r="M8" s="89">
+      <c r="M8" s="106">
         <v>0.13241138133841995</v>
       </c>
-      <c r="N8" s="86">
+      <c r="N8" s="105">
         <v>2.1061834366555396E-3</v>
       </c>
-      <c r="O8" s="86">
+      <c r="O8" s="105">
         <v>8.3452551263710065E-4</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="85" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B9" s="83">
         <v>4907</v>
@@ -12601,33 +12648,33 @@
         <f t="shared" ref="F9:F11" si="6">SUM(B9:E9)</f>
         <v>25191</v>
       </c>
-      <c r="G9" s="87">
+      <c r="G9" s="108">
         <f t="shared" ref="G9:G11" si="7">B9/$F9</f>
         <v>0.19479179071890754</v>
       </c>
-      <c r="H9" s="89">
+      <c r="H9" s="106">
         <f t="shared" si="3"/>
         <v>0.63498868643563178</v>
       </c>
-      <c r="I9" s="89">
+      <c r="I9" s="106">
         <f t="shared" si="4"/>
         <v>0.14862450875312611</v>
       </c>
-      <c r="J9" s="86">
+      <c r="J9" s="105">
         <f t="shared" si="5"/>
         <v>2.1595014092334563E-2</v>
       </c>
-      <c r="K9" s="106"/>
-      <c r="L9" s="86">
+      <c r="K9" s="111"/>
+      <c r="L9" s="105">
         <v>2.606578317100431E-2</v>
       </c>
-      <c r="M9" s="89">
+      <c r="M9" s="106">
         <v>0.78245249880249079</v>
       </c>
-      <c r="N9" s="87">
+      <c r="N9" s="108">
         <v>0.18641226249401247</v>
       </c>
-      <c r="O9" s="86">
+      <c r="O9" s="105">
         <v>5.0694555324924161E-3</v>
       </c>
     </row>
@@ -12648,33 +12695,33 @@
         <f t="shared" si="6"/>
         <v>24952</v>
       </c>
-      <c r="G10" s="86">
+      <c r="G10" s="105">
         <f t="shared" si="7"/>
         <v>2.3845783905097787E-2</v>
       </c>
-      <c r="H10" s="88">
+      <c r="H10" s="107">
         <f t="shared" si="3"/>
         <v>0.33388105161910869</v>
       </c>
-      <c r="I10" s="88">
+      <c r="I10" s="107">
         <f t="shared" si="4"/>
         <v>0.3940766271240782</v>
       </c>
-      <c r="J10" s="87">
+      <c r="J10" s="108">
         <f t="shared" si="5"/>
         <v>0.24819653735171529</v>
       </c>
-      <c r="K10" s="106"/>
-      <c r="L10" s="86">
+      <c r="K10" s="111"/>
+      <c r="L10" s="105">
         <v>2.390152571405808E-4</v>
       </c>
-      <c r="M10" s="89">
+      <c r="M10" s="106">
         <v>0.11341273951320559</v>
       </c>
-      <c r="N10" s="89">
+      <c r="N10" s="106">
         <v>0.59929092140381623</v>
       </c>
-      <c r="O10" s="87">
+      <c r="O10" s="108">
         <v>0.28705732382583754</v>
       </c>
     </row>
@@ -12695,33 +12742,33 @@
         <f t="shared" si="6"/>
         <v>25023</v>
       </c>
-      <c r="G11" s="86">
+      <c r="G11" s="105">
         <f t="shared" si="7"/>
         <v>2.4377572633177478E-3</v>
       </c>
-      <c r="H11" s="89">
+      <c r="H11" s="106">
         <f t="shared" si="3"/>
         <v>8.9917276105982491E-2</v>
       </c>
-      <c r="I11" s="88">
+      <c r="I11" s="107">
         <f t="shared" si="4"/>
         <v>0.31530991487831195</v>
       </c>
-      <c r="J11" s="87">
+      <c r="J11" s="108">
         <f t="shared" si="5"/>
         <v>0.59233505175238776</v>
       </c>
-      <c r="K11" s="106"/>
-      <c r="L11" s="86">
+      <c r="K11" s="111"/>
+      <c r="L11" s="105">
         <v>4.0516996880191239E-5</v>
       </c>
-      <c r="M11" s="86">
+      <c r="M11" s="105">
         <v>3.9301486973785504E-3</v>
       </c>
-      <c r="N11" s="89">
+      <c r="N11" s="106">
         <v>0.14784652161581782</v>
       </c>
-      <c r="O11" s="86">
+      <c r="O11" s="105">
         <v>0.84818281268992346</v>
       </c>
     </row>
@@ -12765,7 +12812,7 @@
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="85" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B14" s="83">
         <v>2540</v>
@@ -12908,7 +12955,7 @@
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="85" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" s="83">
         <v>653</v>
@@ -13020,6 +13067,7 @@
     <mergeCell ref="K2:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13226,7 +13274,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0"/>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14063,23 +14113,23 @@
       <c r="K25" s="49"/>
       <c r="L25" s="49"/>
     </row>
-    <row r="26" spans="1:12" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A26" s="99" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C26" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="59" t="s">
+      <c r="D26" s="102" t="s">
         <v>151</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="102" t="s">
         <v>152</v>
       </c>
-      <c r="F26" s="59" t="s">
+      <c r="F26" s="102" t="s">
         <v>153</v>
       </c>
       <c r="G26" s="59" t="s">
@@ -14088,169 +14138,169 @@
       <c r="H26" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="I26" s="59" t="s">
-        <v>147</v>
+      <c r="I26" s="102" t="s">
+        <v>154</v>
       </c>
       <c r="J26" s="62" t="s">
-        <v>148</v>
-      </c>
-      <c r="K26" s="62" t="s">
-        <v>149</v>
+        <v>155</v>
+      </c>
+      <c r="K26" s="104" t="s">
+        <v>156</v>
       </c>
       <c r="L26" s="59" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="97"/>
       <c r="B28" s="30" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="97" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B29" s="100">
-        <f>G18</f>
-        <v>0.7621</v>
+        <f>1-G18</f>
+        <v>0.2379</v>
       </c>
       <c r="C29" s="100">
-        <f>G19</f>
-        <v>0.67979999999999996</v>
+        <f>1-G19</f>
+        <v>0.32020000000000004</v>
       </c>
       <c r="D29" s="30"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="97" t="str">
         <f>B26</f>
-        <v>2D Features (Spectrogram)</v>
+        <v>Spectrogram</v>
       </c>
       <c r="B30" s="100">
-        <f>B18</f>
-        <v>0.753</v>
+        <f>1-B18</f>
+        <v>0.247</v>
       </c>
       <c r="C30" s="100">
-        <f>B19</f>
-        <v>0.67549999999999999</v>
+        <f>1-B19</f>
+        <v>0.32450000000000001</v>
       </c>
       <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="97" t="str">
         <f>C26</f>
-        <v>2D Features + Aggressive Regularization</v>
+        <v>+Aggressive Regularization</v>
       </c>
       <c r="B31" s="100">
-        <f>C18</f>
-        <v>0.72430000000000005</v>
+        <f>1-C18</f>
+        <v>0.27569999999999995</v>
       </c>
       <c r="C31" s="100">
-        <f>C19</f>
-        <v>0.70209999999999995</v>
+        <f>1-C19</f>
+        <v>0.29790000000000005</v>
       </c>
       <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="97" t="str">
         <f>D26</f>
-        <v>2D Features + 50% More Training Examples</v>
+        <v>+50% More Training Examples</v>
       </c>
       <c r="B32" s="100">
-        <f>D18</f>
-        <v>0.7218</v>
+        <f>1-D18</f>
+        <v>0.2782</v>
       </c>
       <c r="C32" s="100">
-        <f>D19</f>
-        <v>0.72289999999999999</v>
+        <f>1-D19</f>
+        <v>0.27710000000000001</v>
       </c>
       <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="101" t="str">
         <f>E26</f>
-        <v>2D Features + Higher Order Filters</v>
+        <v>+Higher Order Filters</v>
       </c>
       <c r="B33" s="100">
-        <f>E18</f>
-        <v>0.69969999999999999</v>
+        <f>1-E18</f>
+        <v>0.30030000000000001</v>
       </c>
       <c r="C33" s="100">
-        <f>E19</f>
-        <v>0.71699999999999997</v>
+        <f>1-E19</f>
+        <v>0.28300000000000003</v>
       </c>
       <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="97" t="str">
         <f>F26</f>
-        <v>2D Features + Extra Convolutional Layer</v>
+        <v>+Extra Convolutional Layer</v>
       </c>
       <c r="B34" s="100">
-        <f>F18</f>
-        <v>0.72070000000000001</v>
+        <f>1-F18</f>
+        <v>0.27929999999999999</v>
       </c>
       <c r="C34" s="100">
-        <f>F19</f>
-        <v>0.71289999999999998</v>
+        <f>1-F19</f>
+        <v>0.28710000000000002</v>
       </c>
       <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="97" t="str">
         <f>I26</f>
-        <v>1D + 2D Features (Spectrogram, Envelope, Hist.)</v>
+        <v>+Envelope and Histogram</v>
       </c>
       <c r="B35" s="100">
-        <f>I18</f>
-        <v>0.77070000000000005</v>
+        <f>1-I18</f>
+        <v>0.22929999999999995</v>
       </c>
       <c r="C35" s="100">
-        <f>I19</f>
-        <v>0.71050000000000002</v>
+        <f>1-I19</f>
+        <v>0.28949999999999998</v>
       </c>
       <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="97" t="str">
         <f>J26</f>
-        <v>1D + 2D Features, Lower Learning Rate</v>
+        <v>Lower Learning Rate</v>
       </c>
       <c r="B36" s="100">
-        <f>J18</f>
-        <v>0.75470000000000004</v>
+        <f>1-J18</f>
+        <v>0.24529999999999996</v>
       </c>
       <c r="C36" s="100">
-        <f>J19</f>
-        <v>0.73480000000000001</v>
+        <f>1-J19</f>
+        <v>0.26519999999999999</v>
       </c>
       <c r="D36" s="100">
-        <f>J21</f>
-        <v>0.70509999999999995</v>
+        <f>1-J21</f>
+        <v>0.29490000000000005</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="97" t="str">
         <f>K26</f>
-        <v>MFCC Replaced Spectrogram</v>
+        <v>+MFCC -Spectrogram</v>
       </c>
       <c r="B37" s="100">
-        <f>K18</f>
-        <v>0.79020000000000001</v>
+        <f>1-K18</f>
+        <v>0.20979999999999999</v>
       </c>
       <c r="C37" s="100">
-        <f>K19</f>
-        <v>0.74980000000000002</v>
+        <f>1-K19</f>
+        <v>0.25019999999999998</v>
       </c>
       <c r="D37" s="103">
-        <f>K21</f>
-        <v>0.69498631436402913</v>
+        <f>1-K21</f>
+        <v>0.30501368563597087</v>
       </c>
     </row>
   </sheetData>
@@ -15013,7 +15063,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE1B5DB-A7CE-4976-BA44-166DD16E4014}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15565,81 +15617,81 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="30" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="44" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B25" s="100">
-        <f>B13</f>
-        <v>0.54859999999999998</v>
+        <f>1-B13</f>
+        <v>0.45140000000000002</v>
       </c>
       <c r="C25" s="100">
-        <f>B14</f>
-        <v>0.53910000000000002</v>
+        <f>1-B14</f>
+        <v>0.46089999999999998</v>
       </c>
       <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="44" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B26" s="100">
-        <f>D13</f>
-        <v>0.54349999999999998</v>
+        <f>1-D13</f>
+        <v>0.45650000000000002</v>
       </c>
       <c r="C26" s="100">
-        <f>D14</f>
-        <v>0.55620000000000003</v>
+        <f>1-D14</f>
+        <v>0.44379999999999997</v>
       </c>
       <c r="D26" s="51">
-        <f>D16</f>
-        <v>0.53539999999999999</v>
+        <f>1-D16</f>
+        <v>0.46460000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="44" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B27" s="100">
-        <f>H13</f>
-        <v>0.61040000000000005</v>
+        <f>1-H13</f>
+        <v>0.38959999999999995</v>
       </c>
       <c r="C27" s="100">
-        <f>H14</f>
-        <v>0.5575</v>
+        <f>1-H14</f>
+        <v>0.4425</v>
       </c>
       <c r="D27" s="51">
-        <f>H16</f>
-        <v>0.53129999999999999</v>
+        <f>1-H16</f>
+        <v>0.46870000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="44" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B28" s="100">
-        <f>I13</f>
-        <v>0.55889999999999995</v>
+        <f>1-I13</f>
+        <v>0.44110000000000005</v>
       </c>
       <c r="C28" s="100">
-        <f>I14</f>
-        <v>0.55820000000000003</v>
+        <f>1-I14</f>
+        <v>0.44179999999999997</v>
       </c>
       <c r="D28" s="51">
-        <f>I16</f>
-        <v>0.53539999999999999</v>
+        <f>1-I16</f>
+        <v>0.46460000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -15653,7 +15705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A5FAF3-C0D2-4D79-B23C-18AD251D1D2D}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15920,7 +15972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCA155E-1F93-4F27-934F-D628A4DA6CCF}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>